<commit_message>
final revisi BRD: Sub menu Barang dan inventory
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="178">
   <si>
     <t xml:space="preserve">Revisi2</t>
   </si>
@@ -279,10 +279,7 @@
     <t xml:space="preserve">FK tabel p_subkategori_produk</t>
   </si>
   <si>
-    <t xml:space="preserve">id_satuan_brg_asal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK p_satuan_brg</t>
+    <t xml:space="preserve">id_barang_tujuan</t>
   </si>
   <si>
     <t xml:space="preserve">id_subsubkategori_produk</t>
@@ -291,7 +288,13 @@
     <t xml:space="preserve">FK tabel p_subsubkategori_produk</t>
   </si>
   <si>
-    <t xml:space="preserve">id_barang_tujuan</t>
+    <t xml:space="preserve">jumlah_konversi_satuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jumlah konversi barang</t>
   </si>
   <si>
     <t xml:space="preserve">kd_barang</t>
@@ -300,7 +303,10 @@
     <t xml:space="preserve">int(8)</t>
   </si>
   <si>
-    <t xml:space="preserve">id_satuan_brg_tujuan</t>
+    <t xml:space="preserve">id_perusahaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK tabel usaha</t>
   </si>
   <si>
     <t xml:space="preserve">barcode</t>
@@ -309,6 +315,72 @@
     <t xml:space="preserve">varchar(200)</t>
   </si>
   <si>
+    <t xml:space="preserve">id_karyawan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK tabel karyawan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nm_barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buku, kamera, laptop, kaos, dll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_satuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK tabel satuan_barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spec_barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spec barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_histori_konversi_brg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desc_barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rincian barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_rak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no rak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK tabel histori konversi barang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stok_minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stok minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_konversi_brg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK p_konversi_brg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stok_akhir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">tgl_konversi</t>
   </si>
   <si>
@@ -318,79 +390,19 @@
     <t xml:space="preserve">today</t>
   </si>
   <si>
-    <t xml:space="preserve">nm_barang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buku, kamera, laptop, kaos, dll</t>
+    <t xml:space="preserve">hpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desimal(12,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harga pokok penjualan</t>
   </si>
   <si>
     <t xml:space="preserve">jum_brg_dikonversi</t>
   </si>
   <si>
-    <t xml:space="preserve">int(15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jumlah barang yg akan di konversi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_satuan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK tabel satuan_barang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_perusahaan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK tabel usaha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spec_barang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spec barang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_karyawan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK tabel karyawan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desc_barang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rincian barang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_rak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no rak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stok_minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stok minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stok_akhir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desimal(12,2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">harga pokok penjualan</t>
+    <t xml:space="preserve">jumlah brg asal yg akan di konversi</t>
   </si>
   <si>
     <t xml:space="preserve">metode_jual</t>
@@ -420,54 +432,51 @@
     <t xml:space="preserve">PK tabel satuan barang</t>
   </si>
   <si>
+    <t xml:space="preserve">satuan_brg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nama satuan brg</t>
+  </si>
+  <si>
     <t xml:space="preserve">PK tabel harga_jual</t>
   </si>
   <si>
-    <t xml:space="preserve">satuan_brg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nama satuan brg</t>
-  </si>
-  <si>
     <t xml:space="preserve">id_barang</t>
   </si>
   <si>
     <t xml:space="preserve">FK tabel p_barang</t>
   </si>
   <si>
+    <t xml:space="preserve">p_stok_awal</t>
+  </si>
+  <si>
     <t xml:space="preserve">harga_jual</t>
   </si>
   <si>
     <t xml:space="preserve">harga jual barang</t>
   </si>
   <si>
-    <t xml:space="preserve">p_stok_awal</t>
-  </si>
-  <si>
     <t xml:space="preserve">PK tabel stok_awal</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">jumlah_brg</t>
   </si>
   <si>
     <t xml:space="preserve">jumlah barang</t>
   </si>
   <si>
+    <t xml:space="preserve">expired_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tgl kedaluarsa</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_harga_jual_baseon_jumlah</t>
   </si>
   <si>
-    <t xml:space="preserve">expired_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tgl kedaluarsa</t>
-  </si>
-  <si>
     <t xml:space="preserve">jumlah_maks_brg</t>
   </si>
   <si>
@@ -483,13 +492,16 @@
     <t xml:space="preserve">PK tabel item_masuk_keluar</t>
   </si>
   <si>
+    <t xml:space="preserve">jenis_item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: item masuk, 1 : item keluar</t>
+  </si>
+  <si>
     <t xml:space="preserve">PK tabel stok opname</t>
   </si>
   <si>
-    <t xml:space="preserve">jenis_item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0: item masuk, 1 : item keluar</t>
+    <t xml:space="preserve">tgl</t>
   </si>
   <si>
     <t xml:space="preserve">tgl_so</t>
@@ -498,25 +510,22 @@
     <t xml:space="preserve">tgl stok opname</t>
   </si>
   <si>
-    <t xml:space="preserve">tgl</t>
+    <t xml:space="preserve">ket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keterangan item masuk dr mana</t>
   </si>
   <si>
     <t xml:space="preserve">stok akhir ambil dr tabel p_stok_akhir</t>
   </si>
   <si>
-    <t xml:space="preserve">ket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keterangan item masuk dr mana?</t>
+    <t xml:space="preserve">jumlah brg item masuk/ item keluar</t>
   </si>
   <si>
     <t xml:space="preserve">bukti_fisik</t>
   </si>
   <si>
     <t xml:space="preserve">jumlah bukti barang secara fisik yg di hitung. Setelah di input, jumlah butki_fisik ini mereplace stok_akhir di tabel p_stok_akhir yg id_brgnya sama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jumlah brg masuk</t>
   </si>
   <si>
     <t xml:space="preserve">selisih</t>
@@ -557,7 +566,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -588,12 +597,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -615,7 +618,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -635,13 +638,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -691,7 +687,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,35 +740,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,15 +760,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1320,16 +1300,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.7"/>
@@ -1443,7 +1423,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
         <v>3</v>
       </c>
@@ -1466,57 +1446,57 @@
         <v>76</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="F7" s="10" t="n">
         <v>4</v>
       </c>
       <c r="G7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="I7" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" s="11"/>
       <c r="F8" s="10" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,23 +1504,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D9" s="11"/>
       <c r="F9" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>96</v>
+      <c r="G9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,266 +1528,278 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="G10" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>106</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>111</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="F13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+        <v>111</v>
+      </c>
+      <c r="F14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="20" t="s">
+      <c r="F16" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+        <v>124</v>
+      </c>
+      <c r="F17" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>123</v>
+      <c r="B18" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+        <v>128</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="B19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="n">
+      <c r="A20" s="14" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="18"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="F23" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>71</v>
       </c>
@@ -1820,20 +1812,16 @@
       <c r="D24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="n">
         <v>1</v>
       </c>
@@ -1844,84 +1832,84 @@
         <v>76</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>135</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="10" t="n">
-        <v>3</v>
-      </c>
       <c r="G27" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="F28" s="10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
         <v>71</v>
       </c>
@@ -1935,19 +1923,19 @@
         <v>74</v>
       </c>
       <c r="F29" s="10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="n">
         <v>1</v>
       </c>
@@ -1958,225 +1946,231 @@
         <v>76</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>145</v>
+      </c>
+      <c r="F30" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>76</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="F32" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>147</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F34" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="n">
         <v>6</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="F35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="10" t="n">
+      <c r="G36" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="G36" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="10" t="n">
+      <c r="G37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="G37" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="10" t="n">
+      <c r="G38" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="G38" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="10" t="n">
+      <c r="G39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="G39" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="10" t="n">
+      <c r="G40" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F41" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="18"/>
-      <c r="B42" s="13"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14"/>
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
         <v>9</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
-      <c r="F43" s="9" t="n">
-        <v>12</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F43" s="14"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>71</v>
       </c>
@@ -2189,20 +2183,16 @@
       <c r="D44" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F44" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="n">
         <v>1</v>
       </c>
@@ -2213,255 +2203,267 @@
         <v>76</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="F45" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>124</v>
+      <c r="B46" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F46" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="n">
         <v>3</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="D47" s="12"/>
       <c r="F47" s="10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F48" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>118</v>
+        <v>3</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F49" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>162</v>
+        <v>4</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="H49" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I49" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I49" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="38.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="n">
         <v>6</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>164</v>
+        <v>146</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>165</v>
       </c>
       <c r="F50" s="10" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I50" s="21" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I50" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="n">
         <v>7</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>76</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F51" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="G51" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="H51" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="I51" s="20" t="s">
+      <c r="H51" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I51" s="17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="n">
         <v>8</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>76</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="F52" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D53" s="16"/>
+      <c r="F53" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="G52" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
-      <c r="B53" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="D53" s="13"/>
-      <c r="F53" s="24" t="n">
-        <v>10</v>
-      </c>
       <c r="G53" s="11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
+      </c>
+      <c r="F54" s="20" t="n">
+        <v>10</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="18"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="F55" s="18"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="25"/>
+        <v>177</v>
+      </c>
+      <c r="F55" s="14"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="21"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D57" s="0" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="0" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2469,10 +2471,10 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G12:I12"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G33:I33"/>
     <mergeCell ref="B43:D43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
revisi saldo awal (tabel + sub menu inventory)
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
   <si>
     <t xml:space="preserve">Revisi2</t>
   </si>
@@ -465,16 +465,25 @@
     <t xml:space="preserve">jumlah_brg</t>
   </si>
   <si>
-    <t xml:space="preserve">jumlah barang</t>
+    <t xml:space="preserve">jumlah barang sisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diambil dari p_barang.hpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_harga_jual_baseon_jumlah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total = jumlah_brg * hpp</t>
   </si>
   <si>
     <t xml:space="preserve">expired_date</t>
   </si>
   <si>
     <t xml:space="preserve">tgl kedaluarsa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p_harga_jual_baseon_jumlah</t>
   </si>
   <si>
     <t xml:space="preserve">jumlah_maks_brg</t>
@@ -618,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -644,6 +653,13 @@
       <left style="thin"/>
       <right style="thin"/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -687,7 +703,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -760,11 +776,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1302,8 +1330,8 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1981,13 +2009,13 @@
       <c r="A32" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="0" t="s">
+      <c r="C32" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>147</v>
       </c>
       <c r="G32" s="0" t="s">
@@ -1998,20 +2026,20 @@
       <c r="A33" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="F33" s="5" t="n">
         <v>7</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -2020,14 +2048,14 @@
       <c r="A34" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>71</v>
@@ -2047,13 +2075,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>98</v>
+        <v>152</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="F35" s="10" t="n">
         <v>1</v>
@@ -2069,6 +2097,18 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>94</v>
+      </c>
       <c r="F36" s="10" t="n">
         <v>2</v>
       </c>
@@ -2083,17 +2123,29 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="F37" s="10" t="n">
         <v>3</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H37" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,7 +2213,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -2187,7 +2239,7 @@
         <v>12</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
@@ -2203,7 +2255,7 @@
         <v>76</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>71</v>
@@ -2223,13 +2275,13 @@
         <v>2</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>128</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F46" s="10" t="n">
         <v>1</v>
@@ -2241,7 +2293,7 @@
         <v>76</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>120</v>
@@ -2259,13 +2311,13 @@
         <v>2</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>120</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2299,13 +2351,13 @@
         <v>5</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>104</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F49" s="10" t="n">
         <v>4</v>
@@ -2317,7 +2369,7 @@
         <v>76</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="38.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,20 +2382,20 @@
       <c r="C50" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>165</v>
+      <c r="D50" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="F50" s="10" t="n">
         <v>5</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,7 +2405,7 @@
       <c r="B51" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="22" t="s">
         <v>76</v>
       </c>
       <c r="D51" s="11" t="s">
@@ -2363,13 +2415,13 @@
         <v>7</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>76</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,7 +2431,7 @@
       <c r="B52" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="22" t="s">
         <v>76</v>
       </c>
       <c r="D52" s="11" t="s">
@@ -2389,22 +2441,22 @@
         <v>8</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="16" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D53" s="16"/>
       <c r="F53" s="10" t="n">
@@ -2423,12 +2475,12 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F54" s="20" t="n">
+        <v>179</v>
+      </c>
+      <c r="F54" s="23" t="n">
         <v>10</v>
       </c>
       <c r="G54" s="11" t="s">
@@ -2444,12 +2496,12 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="14"/>
       <c r="B55" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
-      <c r="I55" s="21"/>
+      <c r="I55" s="24"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D57" s="0" t="s">

</xml_diff>

<commit_message>
update revisi menu pembelian-PO-order-pembayaran
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -12,7 +12,7 @@
     <sheet name="revisi sub menu brg &amp; inventory" sheetId="3" r:id="rId3"/>
     <sheet name="revisi sub menu pembelian" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="287">
   <si>
     <t>Revisi2</t>
   </si>
@@ -616,6 +616,331 @@
   </si>
   <si>
     <t>no_po</t>
+  </si>
+  <si>
+    <t>diskon_item</t>
+  </si>
+  <si>
+    <t>jumlah_harga</t>
+  </si>
+  <si>
+    <t>jumlah harga per item</t>
+  </si>
+  <si>
+    <t>pajak</t>
+  </si>
+  <si>
+    <t>p_detail_tb</t>
+  </si>
+  <si>
+    <t>PK tabel detail tawar beli</t>
+  </si>
+  <si>
+    <t>PK tabel pesanan pembelian</t>
+  </si>
+  <si>
+    <t>p_detail_po</t>
+  </si>
+  <si>
+    <t>id_po</t>
+  </si>
+  <si>
+    <t>FK tabel p_po</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK tabel p_tawar_beli, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pajak pembelian brg, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>diskon total brg po,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>diskon per item brg,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>dp_po</t>
+  </si>
+  <si>
+    <t>uang muka PO</t>
+  </si>
+  <si>
+    <t>nomor po</t>
+  </si>
+  <si>
+    <t>tgl po</t>
+  </si>
+  <si>
+    <t>diskon_tambahan</t>
+  </si>
+  <si>
+    <t>kurang bayar PO</t>
+  </si>
+  <si>
+    <t>kurang_bayar</t>
+  </si>
+  <si>
+    <t>tgl_dikirim</t>
+  </si>
+  <si>
+    <t>tgl brg di kirim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK tabel beli brg/order </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK tabel p_po, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>tgl beli</t>
+  </si>
+  <si>
+    <t>no_order</t>
+  </si>
+  <si>
+    <t>p_order  --&gt; tabel yg lama p_beli_barang</t>
+  </si>
+  <si>
+    <t>tgl_order</t>
+  </si>
+  <si>
+    <t>nomor order</t>
+  </si>
+  <si>
+    <t>tgl_tiba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tgl brg tiba </t>
+  </si>
+  <si>
+    <t>bayar</t>
+  </si>
+  <si>
+    <t>pembayaran brg yg dibeli</t>
+  </si>
+  <si>
+    <t>ongkir</t>
+  </si>
+  <si>
+    <t>ongkos kirim brg</t>
+  </si>
+  <si>
+    <t>p_detail_order</t>
+  </si>
+  <si>
+    <t>id_order</t>
+  </si>
+  <si>
+    <t>FK tabel p_order</t>
+  </si>
+  <si>
+    <t>jumlah harga beli per item brg</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_barang.id_barang atau p_detail_po.id_barang</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_barang.hpp atau p_detail_po.hpp</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_detail_po.jumlah_beli ato di isi manual</t>
+  </si>
+  <si>
+    <t>tgl_jatuh_tempo</t>
+  </si>
+  <si>
+    <t>tgl jatuh tempo hutang pembelian kredit</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>keterangan PO</t>
+  </si>
+  <si>
+    <t>status_po</t>
+  </si>
+  <si>
+    <t>int(1)</t>
+  </si>
+  <si>
+    <t>0 = open, 1 = close</t>
+  </si>
+  <si>
+    <t>kurang bayar pembelian/hutang</t>
+  </si>
+  <si>
+    <t>metode_bayar</t>
+  </si>
+  <si>
+    <t>status_bayar</t>
+  </si>
+  <si>
+    <t>0 = lunas, 1 = belum lunas</t>
+  </si>
+  <si>
+    <t>p_cek_barang</t>
+  </si>
+  <si>
+    <t>PK tabel cek brg</t>
+  </si>
+  <si>
+    <t>di ambil dari p_detail_po.id_barang</t>
+  </si>
+  <si>
+    <t>cek_jumlah</t>
+  </si>
+  <si>
+    <t>0 = sesuai, 1 = non sesuai</t>
+  </si>
+  <si>
+    <t>cek_kualitas</t>
+  </si>
+  <si>
+    <t>keterangan untuk menjelaskan hasil cek_jumlah dan cek_kualitas</t>
+  </si>
+  <si>
+    <t>p_bayar</t>
+  </si>
+  <si>
+    <t>PK tabel pembayaran</t>
+  </si>
+  <si>
+    <t>jenis_bayar</t>
+  </si>
+  <si>
+    <t>0= bayar PO, 1 = bayar order</t>
+  </si>
+  <si>
+    <t>FK p_po, nullable</t>
+  </si>
+  <si>
+    <t>FK p_order, nullable</t>
+  </si>
+  <si>
+    <t>jumlah_bayar</t>
+  </si>
+  <si>
+    <t>jika bayar po, ambil data p_po.dp_po. Jika bayar order : ambil data p_order.bayar</t>
+  </si>
+  <si>
+    <t>0 = transfer bank, 1 = cek, 3 = langsung</t>
+  </si>
+  <si>
+    <t>bukti_bayar</t>
+  </si>
+  <si>
+    <t>varchar (200)</t>
+  </si>
+  <si>
+    <t>scan/foto bukti bayar</t>
+  </si>
+  <si>
+    <t>kirim_bukti</t>
+  </si>
+  <si>
+    <t>0= blm konfirm pembayaran, 1 = sdh konfirm pembayaran</t>
+  </si>
+  <si>
+    <t>tgl_bayar</t>
+  </si>
+  <si>
+    <t>jika bayar po,  p_po.tgl_po (editable),    jika bayar order,  p_o.tgl_order.tgl_order (editable)</t>
+  </si>
+  <si>
+    <t>0 = tunai, 1 = kredit/hutang/cicil</t>
+  </si>
+  <si>
+    <t>bank_tujuan</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>no_rek_tujuan</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>p_rek_supplier</t>
+  </si>
+  <si>
+    <t>tambahkan tabel:</t>
+  </si>
+  <si>
+    <t>rekening_supplier</t>
+  </si>
+  <si>
+    <t>rekening_ukm</t>
+  </si>
+  <si>
+    <t>bank_asal</t>
+  </si>
+  <si>
+    <t>rek_asal</t>
+  </si>
+  <si>
+    <t>p_rek_ukm</t>
   </si>
 </sst>
 </file>
@@ -626,7 +951,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -649,8 +974,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,6 +1005,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -757,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -807,9 +1151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -820,8 +1161,32 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1620,7 +1985,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:D37"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1637,30 +2002,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -1886,11 +2251,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -2109,11 +2474,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -2131,11 +2496,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -2326,11 +2691,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -2500,11 +2865,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -2824,18 +3189,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
@@ -2855,8 +3220,8 @@
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>194</v>
+      <c r="G1" s="30" t="s">
+        <v>202</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -2897,7 +3262,7 @@
       <c r="C3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>182</v>
       </c>
       <c r="F3" s="10">
@@ -2909,8 +3274,8 @@
       <c r="H3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>139</v>
+      <c r="I3" s="25" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2929,7 +3294,7 @@
       <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>195</v>
       </c>
       <c r="H4" s="20" t="s">
@@ -2943,235 +3308,1302 @@
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>184</v>
       </c>
       <c r="F5" s="10">
         <v>3</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>196</v>
+      <c r="G5" s="26" t="s">
+        <v>140</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="20" t="s">
-        <v>155</v>
+      <c r="I5" s="26" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>185</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>186</v>
       </c>
       <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>197</v>
+      <c r="G6" s="26" t="s">
+        <v>187</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>144</v>
+      <c r="I6" s="26" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>140</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>141</v>
+      <c r="D7" s="26" t="s">
+        <v>191</v>
       </c>
       <c r="F7" s="10">
         <v>5</v>
       </c>
-      <c r="G7" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>186</v>
+      <c r="G7" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>187</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>188</v>
+      <c r="D8" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="F8" s="10">
         <v>6</v>
       </c>
-      <c r="G8" s="27" t="s">
-        <v>140</v>
+      <c r="G8" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="H8" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>141</v>
+      <c r="I8" s="26" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>190</v>
-      </c>
+      <c r="A9" s="14"/>
+      <c r="B9" s="27"/>
       <c r="F9" s="10">
         <v>7</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5">
+        <v>3</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="F11" s="5">
+        <v>4</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="10">
+        <v>1</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" s="10">
+        <v>2</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="10">
+        <v>3</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="10">
+        <v>4</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" s="10">
+        <v>4</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="H9" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="27" t="s">
+      <c r="H16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="26" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="10">
+    <row r="17" spans="1:9">
+      <c r="A17" s="10">
+        <v>5</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="10">
+        <v>5</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="10">
+        <v>6</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="F18" s="10">
+        <v>6</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="10">
+        <v>7</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="F19" s="10">
+        <v>7</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B20" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="F20" s="10">
+        <v>8</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="H20" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="10">
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="10">
+        <v>9</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" s="10">
+        <v>9</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="10">
+        <v>10</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="10">
+        <v>11</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="G23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10">
+        <v>12</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="10">
+        <v>13</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="10">
+        <v>14</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="5">
+        <v>6</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="F27" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="5">
+        <v>5</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="10">
+        <v>2</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30">
+      <c r="A30" s="10">
+        <v>1</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="10">
+        <v>3</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30">
+      <c r="A31" s="10">
+        <v>2</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="10">
+        <v>4</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30">
+      <c r="A32" s="10">
+        <v>3</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="10">
+        <v>5</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="10">
+        <v>4</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="F33" s="10">
+        <v>6</v>
+      </c>
+      <c r="G33" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="H33" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="10">
+        <v>5</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F34" s="10">
+        <v>7</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="10">
+        <v>6</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" s="10">
         <v>8</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G35" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="10">
+        <v>7</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="F36" s="10">
+        <v>9</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="10">
+        <v>8</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="10">
+        <v>9</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="5">
+        <v>7</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="10">
+        <v>10</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="10">
+        <v>11</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="F40" s="10">
+        <v>1</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="10">
+        <v>12</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="F41" s="10">
+        <v>2</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="10">
+        <v>13</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="F42" s="10">
+        <v>3</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="37" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30">
+      <c r="A43" s="10">
+        <v>14</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="F43" s="10">
+        <v>4</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I43" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30">
+      <c r="A44" s="10">
+        <v>15</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F44" s="10">
+        <v>5</v>
+      </c>
+      <c r="G44" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="10">
+      <c r="H44" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I44" s="37" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="10">
+        <v>16</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="F45" s="10">
+        <v>6</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="H45" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="10">
+        <v>17</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" s="10">
+        <v>7</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I46" s="32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="10">
+        <v>18</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="10">
+        <v>8</v>
+      </c>
+      <c r="G47" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="H47" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="I47" s="41" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="F48" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="G48" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="H48" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="I48" s="41" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30">
+      <c r="F49" s="10">
+        <v>10</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="H49" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I49" s="41" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="F50" s="10">
+        <v>11</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="5">
+        <v>8</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="F51" s="10">
+        <v>12</v>
+      </c>
+      <c r="G51" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="20" t="s">
+      <c r="H51" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I51" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="10">
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" s="29"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="10">
+        <v>1</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="H53" s="29"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="10">
+        <v>2</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="G54" t="s">
+        <v>281</v>
+      </c>
+      <c r="H54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="10">
+        <v>3</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="G55" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="10">
+        <v>4</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="G56" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="45">
+      <c r="A57" s="10">
+        <v>5</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="G57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="10">
+        <v>6</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>246</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="10">
+        <v>7</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="C59" s="26"/>
+      <c r="D59" s="43" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="10">
+        <v>8</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" s="26"/>
+      <c r="D60" s="43" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="10">
         <v>9</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="B61" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="D61" s="43" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="10">
+        <v>10</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="45">
+      <c r="A63" s="26"/>
+      <c r="B63" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="26"/>
+      <c r="B64" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30">
+      <c r="A65" s="26"/>
+      <c r="B65" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D65" s="43" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="26"/>
+      <c r="B66" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="27" t="s">
+      <c r="C66" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="26" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="F12" s="10">
-        <v>10</v>
-      </c>
-      <c r="G12" s="20" t="s">
+    <row r="67" spans="1:4">
+      <c r="A67" s="26"/>
+      <c r="B67" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="20" t="s">
+      <c r="C67" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="14"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="30"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="C16" s="30"/>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="30"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="C18" s="30"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="C19" s="30"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="C20" s="30"/>
-      <c r="D20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="C21" s="30"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="C22" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update revisi sub menu pembelian: return pembelian
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="301">
   <si>
     <t>Revisi2</t>
   </si>
@@ -850,9 +850,6 @@
     <t>cek_jumlah</t>
   </si>
   <si>
-    <t>0 = sesuai, 1 = non sesuai</t>
-  </si>
-  <si>
     <t>cek_kualitas</t>
   </si>
   <si>
@@ -941,6 +938,51 @@
   </si>
   <si>
     <t>p_rek_ukm</t>
+  </si>
+  <si>
+    <t>0 = sesuai, 1 = tdk sesuai</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_detail_po.jumlah_beli ato di isi manual jika beli tanpa PO</t>
+  </si>
+  <si>
+    <t>p_return_brg</t>
+  </si>
+  <si>
+    <t>PK tabel return</t>
+  </si>
+  <si>
+    <t>id_cek_barang</t>
+  </si>
+  <si>
+    <t>FK tabel p_cek_barang</t>
+  </si>
+  <si>
+    <t>tgl_return</t>
+  </si>
+  <si>
+    <t>jenis_return</t>
+  </si>
+  <si>
+    <t>0 = return barang, 1 = return uang, 3 = potong hutang</t>
+  </si>
+  <si>
+    <t>konfirm</t>
+  </si>
+  <si>
+    <t>0 = belum, 1 =sudah</t>
+  </si>
+  <si>
+    <t>status_return</t>
+  </si>
+  <si>
+    <t>0=open, 1=close</t>
+  </si>
+  <si>
+    <t>ongkir_return</t>
+  </si>
+  <si>
+    <t>ongkos kirim brg yg di return</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1178,9 +1220,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1188,6 +1227,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2002,30 +2048,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -2251,11 +2297,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -2474,11 +2520,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -2496,11 +2542,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -2691,11 +2737,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G33" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -2865,11 +2911,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -3191,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="C51" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3737,8 +3783,8 @@
       <c r="D23" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="G23" t="s">
-        <v>109</v>
+      <c r="G23" s="45" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3754,6 +3800,9 @@
       <c r="D24" s="31" t="s">
         <v>247</v>
       </c>
+      <c r="G24" s="45" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -3767,6 +3816,9 @@
       </c>
       <c r="D25" s="26" t="s">
         <v>191</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4137,7 +4189,7 @@
         <v>246</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F41" s="10">
         <v>2</v>
@@ -4227,7 +4279,7 @@
         <v>76</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>240</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4304,36 +4356,36 @@
       <c r="H47" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="I47" s="41" t="s">
-        <v>256</v>
+      <c r="I47" s="40" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="F48" s="10">
         <v>9</v>
       </c>
-      <c r="G48" s="31" t="s">
-        <v>257</v>
-      </c>
-      <c r="H48" s="35" t="s">
+      <c r="G48" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="H48" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="I48" s="41" t="s">
-        <v>256</v>
+      <c r="I48" s="40" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
       <c r="F49" s="10">
         <v>10</v>
       </c>
-      <c r="G49" s="31" t="s">
+      <c r="G49" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="H49" s="35" t="s">
+      <c r="H49" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="I49" s="41" t="s">
-        <v>258</v>
+      <c r="I49" s="40" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -4355,7 +4407,7 @@
         <v>8</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C51" s="38"/>
       <c r="D51" s="38"/>
@@ -4398,7 +4450,10 @@
         <v>76</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="G53" t="s">
+        <v>109</v>
       </c>
       <c r="H53" s="29"/>
     </row>
@@ -4407,20 +4462,22 @@
         <v>2</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>246</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="G54" t="s">
-        <v>281</v>
-      </c>
-      <c r="H54" t="s">
-        <v>109</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="F54" s="5">
+        <v>7</v>
+      </c>
+      <c r="G54" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="10">
@@ -4433,10 +4490,19 @@
         <v>76</v>
       </c>
       <c r="D55" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="G55" t="s">
-        <v>282</v>
+        <v>262</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -4450,10 +4516,19 @@
         <v>76</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>264</v>
-      </c>
-      <c r="G56" t="s">
-        <v>283</v>
+        <v>263</v>
+      </c>
+      <c r="F56" s="10">
+        <v>1</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H56" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I56" s="25" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45">
@@ -4461,16 +4536,25 @@
         <v>5</v>
       </c>
       <c r="B57" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="C57" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="G57" t="s">
-        <v>109</v>
+      <c r="F57" s="10">
+        <v>2</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -4480,26 +4564,45 @@
       <c r="B58" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="C58" s="42" t="s">
+      <c r="C58" s="41" t="s">
         <v>246</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="G58" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>266</v>
+      </c>
+      <c r="F58" s="10">
+        <v>3</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H58" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="I58" s="37"/>
+    </row>
+    <row r="59" spans="1:9" ht="30">
       <c r="A59" s="10">
         <v>7</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C59" s="26"/>
-      <c r="D59" s="43" t="s">
-        <v>286</v>
+      <c r="D59" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="F59" s="10">
+        <v>4</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="H59" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="I59" s="37" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4507,11 +4610,23 @@
         <v>8</v>
       </c>
       <c r="B60" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="C60" s="26"/>
+      <c r="D60" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="43" t="s">
-        <v>286</v>
+      <c r="F60" s="10">
+        <v>5</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I60" s="41" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4519,13 +4634,25 @@
         <v>9</v>
       </c>
       <c r="B61" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C61" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="C61" s="42" t="s">
-        <v>277</v>
-      </c>
-      <c r="D61" s="43" t="s">
-        <v>280</v>
+      <c r="D61" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="F61" s="10">
+        <v>6</v>
+      </c>
+      <c r="G61" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="I61" s="40" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4533,52 +4660,98 @@
         <v>10</v>
       </c>
       <c r="B62" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C62" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="C62" s="42" t="s">
+      <c r="D62" s="42" t="s">
         <v>279</v>
       </c>
-      <c r="D62" s="43" t="s">
-        <v>280</v>
+      <c r="F62" s="10">
+        <v>7</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="H62" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="I62" s="40" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="45">
       <c r="A63" s="26"/>
       <c r="B63" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C63" s="20" t="s">
         <v>123</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="F63" s="10">
+        <v>8</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="H63" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="I63" s="32" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="26"/>
       <c r="B64" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C64" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="D64" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="D64" s="32" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="30">
+      <c r="F64" s="10">
+        <v>9</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I64" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="26"/>
       <c r="B65" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C65" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="D65" s="43" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="D65" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="F65" s="10"/>
+      <c r="G65" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I65" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="26"/>
       <c r="B66" s="20" t="s">
         <v>93</v>
@@ -4589,8 +4762,11 @@
       <c r="D66" s="26" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="F66" s="14"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="26"/>
       <c r="B67" s="20" t="s">
         <v>97</v>
@@ -4601,6 +4777,9 @@
       <c r="D67" s="20" t="s">
         <v>98</v>
       </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
update revisi sub menu pembelian : seting jurnal otomatis sub menu pembelian
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="316">
   <si>
     <t>Revisi2</t>
   </si>
@@ -880,9 +880,6 @@
     <t>jika bayar po, ambil data p_po.dp_po. Jika bayar order : ambil data p_order.bayar</t>
   </si>
   <si>
-    <t>0 = transfer bank, 1 = cek, 3 = langsung</t>
-  </si>
-  <si>
     <t>bukti_bayar</t>
   </si>
   <si>
@@ -983,6 +980,54 @@
   </si>
   <si>
     <t>ongkos kirim brg yg di return</t>
+  </si>
+  <si>
+    <t>p_akun_pembelian</t>
+  </si>
+  <si>
+    <t>PK tabel seting akun sub menu pembelian</t>
+  </si>
+  <si>
+    <t>jenis_transaksi</t>
+  </si>
+  <si>
+    <t>FK tabel k_transaksi</t>
+  </si>
+  <si>
+    <t>id_ket_transaksi</t>
+  </si>
+  <si>
+    <t>enum('0','1')</t>
+  </si>
+  <si>
+    <t>note:</t>
+  </si>
+  <si>
+    <t>enum('0','1',2')</t>
+  </si>
+  <si>
+    <t>0 = transfer bank, 1 = cek, 2 = langsung</t>
+  </si>
+  <si>
+    <t>id_akun_aktif</t>
+  </si>
+  <si>
+    <t>posisi_akun</t>
+  </si>
+  <si>
+    <t>int(10)</t>
+  </si>
+  <si>
+    <t>FK k_akun_aktif_ukm</t>
+  </si>
+  <si>
+    <t>0 = Penerimaan, 1: Pengeluaran</t>
+  </si>
+  <si>
+    <t>0 = Debet, 1: Kredit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = PO, 1 = pembelian tunai, 2=pembelian kredit, 3 = pembelian tunai, 4 = return pembelian </t>
   </si>
 </sst>
 </file>
@@ -993,7 +1038,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1028,6 +1073,13 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1143,7 +1195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1230,10 +1282,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2030,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2048,30 +2104,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -2297,11 +2353,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -2520,11 +2576,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -2542,11 +2598,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="43" t="s">
+      <c r="G24" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -2737,11 +2793,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="43" t="s">
+      <c r="G33" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -2911,11 +2967,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -3235,10 +3291,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C51" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3734,13 +3790,13 @@
       <c r="A21" s="10">
         <v>9</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="36" t="s">
         <v>213</v>
       </c>
       <c r="F21" s="10">
@@ -3760,13 +3816,13 @@
       <c r="A22" s="10">
         <v>10</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="32" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3774,34 +3830,37 @@
       <c r="A23" s="10">
         <v>11</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="G23" s="45" t="s">
-        <v>280</v>
+      <c r="F23" s="47" t="s">
+        <v>306</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10">
         <v>12</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="D24" s="31" t="s">
+      <c r="C24" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G24" s="45" t="s">
-        <v>281</v>
+      <c r="G24" s="44" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3817,8 +3876,8 @@
       <c r="D25" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="G25" s="45" t="s">
-        <v>282</v>
+      <c r="G25" s="44" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4185,11 +4244,11 @@
       <c r="B41" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="C41" s="32" t="s">
-        <v>246</v>
+      <c r="C41" s="26" t="s">
+        <v>305</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F41" s="10">
         <v>2</v>
@@ -4279,7 +4338,7 @@
         <v>76</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4290,7 +4349,7 @@
         <v>250</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>246</v>
+        <v>305</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>251</v>
@@ -4353,11 +4412,11 @@
       <c r="G47" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="H47" s="35" t="s">
-        <v>246</v>
+      <c r="H47" s="32" t="s">
+        <v>305</v>
       </c>
       <c r="I47" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4367,11 +4426,11 @@
       <c r="G48" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="H48" s="41" t="s">
-        <v>246</v>
+      <c r="H48" s="32" t="s">
+        <v>305</v>
       </c>
       <c r="I48" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
@@ -4471,10 +4530,10 @@
         <v>261</v>
       </c>
       <c r="F54" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G54" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H54" s="39"/>
       <c r="I54" s="39"/>
@@ -4528,7 +4587,7 @@
         <v>76</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45">
@@ -4536,25 +4595,25 @@
         <v>5</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C57" s="41" t="s">
         <v>120</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F57" s="10">
         <v>2</v>
       </c>
       <c r="G57" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I57" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="H57" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I57" s="26" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -4564,17 +4623,17 @@
       <c r="B58" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="C58" s="41" t="s">
-        <v>246</v>
+      <c r="C58" s="26" t="s">
+        <v>307</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="F58" s="10">
         <v>3</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H58" s="26" t="s">
         <v>120</v>
@@ -4586,23 +4645,23 @@
         <v>7</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C59" s="26"/>
       <c r="D59" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F59" s="10">
         <v>4</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H59" s="26" t="s">
         <v>246</v>
       </c>
       <c r="I59" s="37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4610,23 +4669,23 @@
         <v>8</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C60" s="26"/>
       <c r="D60" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F60" s="10">
         <v>5</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H60" s="20" t="s">
         <v>123</v>
       </c>
       <c r="I60" s="41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4634,25 +4693,25 @@
         <v>9</v>
       </c>
       <c r="B61" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="C61" s="41" t="s">
-        <v>276</v>
-      </c>
       <c r="D61" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F61" s="10">
         <v>6</v>
       </c>
       <c r="G61" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="H61" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="I61" s="40" t="s">
         <v>295</v>
-      </c>
-      <c r="H61" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="I61" s="40" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4660,13 +4719,13 @@
         <v>10</v>
       </c>
       <c r="B62" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C62" s="41" t="s">
         <v>277</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="D62" s="42" t="s">
         <v>278</v>
-      </c>
-      <c r="D62" s="42" t="s">
-        <v>279</v>
       </c>
       <c r="F62" s="10">
         <v>7</v>
@@ -4674,11 +4733,11 @@
       <c r="G62" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="H62" s="41" t="s">
-        <v>246</v>
+      <c r="H62" s="32" t="s">
+        <v>305</v>
       </c>
       <c r="I62" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="45">
@@ -4696,25 +4755,25 @@
         <v>8</v>
       </c>
       <c r="G63" s="32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H63" s="26" t="s">
         <v>246</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="26"/>
       <c r="B64" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C64" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="D64" s="32" t="s">
         <v>268</v>
-      </c>
-      <c r="D64" s="32" t="s">
-        <v>269</v>
       </c>
       <c r="F64" s="10">
         <v>9</v>
@@ -4732,13 +4791,13 @@
     <row r="65" spans="1:9" ht="30">
       <c r="A65" s="26"/>
       <c r="B65" s="32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C65" s="32" t="s">
         <v>246</v>
       </c>
       <c r="D65" s="42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="20" t="s">
@@ -4780,6 +4839,151 @@
       <c r="F67" s="14"/>
       <c r="G67" s="27"/>
       <c r="H67" s="27"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="5">
+        <v>10</v>
+      </c>
+      <c r="B70" s="43" t="s">
+        <v>300</v>
+      </c>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="10">
+        <v>1</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>301</v>
+      </c>
+      <c r="G72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="45">
+      <c r="A73" s="10">
+        <v>2</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D73" s="37" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="10">
+        <v>3</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" s="37" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="10">
+        <v>4</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" s="37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="10">
+        <v>5</v>
+      </c>
+      <c r="B76" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="10">
+        <v>6</v>
+      </c>
+      <c r="B77" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="D77" s="40" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="10">
+        <v>7</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="10">
+        <v>8</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="14"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
update revisi sub menu pembelian : jurnal umum otomatis di tab PO
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -1027,7 +1027,11 @@
     <t>0 = Debet, 1: Kredit</t>
   </si>
   <si>
-    <t xml:space="preserve">0 = PO, 1 = pembelian tunai, 2=pembelian kredit, 3 = pembelian tunai, 4 = return pembelian </t>
+    <t xml:space="preserve">0 = PO, 1 = pembelian tunai, 2=pembelian tunai, 3 = pembelian kredit, 4 = potongan pembelian, 5= Beban angkut pembelian,
+6=Return pembelian ganti barang,
+7= Return pembelian ganti uang,
+8=Return pembelian potong hutang
+</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1283,13 +1287,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2104,30 +2117,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -2353,11 +2366,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -2576,11 +2589,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -2598,11 +2611,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -2793,11 +2806,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -2967,11 +2980,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="45" t="s">
+      <c r="B43" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -3293,8 +3306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3839,7 +3852,7 @@
       <c r="D23" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="F23" s="47" t="s">
+      <c r="F23" s="45" t="s">
         <v>306</v>
       </c>
       <c r="G23" s="44" t="s">
@@ -4881,17 +4894,17 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="45">
-      <c r="A73" s="10">
+    <row r="73" spans="1:9" ht="120">
+      <c r="A73" s="48">
         <v>2</v>
       </c>
-      <c r="B73" s="26" t="s">
+      <c r="B73" s="49" t="s">
         <v>302</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="49" t="s">
         <v>246</v>
       </c>
-      <c r="D73" s="37" t="s">
+      <c r="D73" s="50" t="s">
         <v>315</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update revisi sub menu pembelian-jurnal umum otomatis pembelian tunai
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="317">
   <si>
     <t>Revisi2</t>
   </si>
@@ -1032,6 +1032,9 @@
 7= Return pembelian ganti uang,
 8=Return pembelian potong hutang
 </t>
+  </si>
+  <si>
+    <t>jenis_jurnal</t>
   </si>
 </sst>
 </file>
@@ -1288,12 +1291,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1302,6 +1299,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2117,30 +2120,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -2366,11 +2369,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -2589,11 +2592,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -2611,11 +2614,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -2806,11 +2809,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -2980,11 +2983,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -3307,7 +3310,7 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -4895,16 +4898,16 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="120">
-      <c r="A73" s="48">
+      <c r="A73" s="46">
         <v>2</v>
       </c>
-      <c r="B73" s="49" t="s">
-        <v>302</v>
-      </c>
-      <c r="C73" s="49" t="s">
+      <c r="B73" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="C73" s="47" t="s">
         <v>246</v>
       </c>
-      <c r="D73" s="50" t="s">
+      <c r="D73" s="48" t="s">
         <v>315</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update revisi sub menu pembelian: jurnal otomatis sub menu pembelian
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="319">
   <si>
     <t>Revisi2</t>
   </si>
@@ -865,9 +865,6 @@
     <t>jenis_bayar</t>
   </si>
   <si>
-    <t>0= bayar PO, 1 = bayar order</t>
-  </si>
-  <si>
     <t>FK p_po, nullable</t>
   </si>
   <si>
@@ -877,30 +874,18 @@
     <t>jumlah_bayar</t>
   </si>
   <si>
-    <t>jika bayar po, ambil data p_po.dp_po. Jika bayar order : ambil data p_order.bayar</t>
-  </si>
-  <si>
     <t>bukti_bayar</t>
   </si>
   <si>
     <t>varchar (200)</t>
   </si>
   <si>
-    <t>scan/foto bukti bayar</t>
-  </si>
-  <si>
     <t>kirim_bukti</t>
   </si>
   <si>
-    <t>0= blm konfirm pembayaran, 1 = sdh konfirm pembayaran</t>
-  </si>
-  <si>
     <t>tgl_bayar</t>
   </si>
   <si>
-    <t>jika bayar po,  p_po.tgl_po (editable),    jika bayar order,  p_o.tgl_order.tgl_order (editable)</t>
-  </si>
-  <si>
     <t>0 = tunai, 1 = kredit/hutang/cicil</t>
   </si>
   <si>
@@ -916,9 +901,6 @@
     <t>varchar(20)</t>
   </si>
   <si>
-    <t>p_rek_supplier</t>
-  </si>
-  <si>
     <t>tambahkan tabel:</t>
   </si>
   <si>
@@ -934,9 +916,6 @@
     <t>rek_asal</t>
   </si>
   <si>
-    <t>p_rek_ukm</t>
-  </si>
-  <si>
     <t>0 = sesuai, 1 = tdk sesuai</t>
   </si>
   <si>
@@ -1006,9 +985,6 @@
     <t>enum('0','1',2')</t>
   </si>
   <si>
-    <t>0 = transfer bank, 1 = cek, 2 = langsung</t>
-  </si>
-  <si>
     <t>id_akun_aktif</t>
   </si>
   <si>
@@ -1027,14 +1003,148 @@
     <t>0 = Debet, 1: Kredit</t>
   </si>
   <si>
-    <t xml:space="preserve">0 = PO, 1 = pembelian tunai, 2=pembelian tunai, 3 = pembelian kredit, 4 = potongan pembelian, 5= Beban angkut pembelian,
-6=Return pembelian ganti barang,
-7= Return pembelian ganti uang,
-8=Return pembelian potong hutang
+    <t>jenis_jurnal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = PO, 1 = pembelian tunai tanpa pajak, 2=pembelian tunai dg pajak, 3 = pembelian kredit tanpa pajak, 4= pembelian kredit dg pajak, 5=  Beban angkut pembelian,
+5=Return pembelian tunai
+6= Return pembelian kredit
 </t>
   </si>
   <si>
-    <t>jenis_jurnal</t>
+    <t>0 = transfer bank, 1 = cek, 2 = langsung, 3 = return barang</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">p_rek_ukm, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullabe</t>
+    </r>
+  </si>
+  <si>
+    <t>jika bayar po, ambil data p_po.dp_po. Jika bayar order : ambil data p_order.bayar, jika return pembelian: ambil data total hrg brg yg di return</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">p_rek_supplier,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullabe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">scan/foto bukti bayar, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0= blm konfirm pembayaran, 1 = sdh konfirm pembayaran, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>jika bayar po</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,  p_po.tgl_po (editable),    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>jika bayar order,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  p_o.tgl_order.tgl_order (editable),                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jika return pembelian : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>p_returb_brg.tgl_return</t>
+    </r>
+  </si>
+  <si>
+    <t>0= bayar PO, 1 = bayar order. 3 = return brg</t>
+  </si>
+  <si>
+    <t>id_return_barang</t>
+  </si>
+  <si>
+    <t>FK p_return_barang, nullable</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1155,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1087,6 +1197,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1202,7 +1325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1305,6 +1428,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3309,8 +3435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3856,10 +3982,10 @@
         <v>244</v>
       </c>
       <c r="F23" s="45" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="G23" s="44" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3870,13 +3996,13 @@
         <v>245</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>247</v>
       </c>
       <c r="G24" s="44" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3893,7 +4019,7 @@
         <v>191</v>
       </c>
       <c r="G25" s="44" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4261,10 +4387,10 @@
         <v>249</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F41" s="10">
         <v>2</v>
@@ -4354,7 +4480,7 @@
         <v>76</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4365,7 +4491,7 @@
         <v>250</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>251</v>
@@ -4429,10 +4555,10 @@
         <v>255</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="I47" s="40" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4443,10 +4569,10 @@
         <v>256</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="I48" s="40" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
@@ -4543,13 +4669,13 @@
         <v>246</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>261</v>
+        <v>316</v>
       </c>
       <c r="F54" s="5">
         <v>9</v>
       </c>
       <c r="G54" s="39" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H54" s="39"/>
       <c r="I54" s="39"/>
@@ -4565,7 +4691,7 @@
         <v>76</v>
       </c>
       <c r="D55" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>71</v>
@@ -4591,7 +4717,7 @@
         <v>76</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F56" s="10">
         <v>1</v>
@@ -4603,53 +4729,53 @@
         <v>76</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="45">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="10">
         <v>5</v>
       </c>
-      <c r="B57" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="C57" s="41" t="s">
-        <v>120</v>
+      <c r="B57" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>272</v>
+        <v>318</v>
       </c>
       <c r="F57" s="10">
         <v>2</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H57" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I57" s="26" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="75">
       <c r="A58" s="10">
         <v>6</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>307</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>308</v>
+        <v>267</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" s="51" t="s">
+        <v>315</v>
       </c>
       <c r="F58" s="10">
         <v>3</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H58" s="26" t="s">
         <v>120</v>
@@ -4661,23 +4787,25 @@
         <v>7</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="C59" s="26"/>
-      <c r="D59" s="42" t="s">
-        <v>284</v>
+        <v>249</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>309</v>
       </c>
       <c r="F59" s="10">
         <v>4</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="H59" s="26" t="s">
         <v>246</v>
       </c>
       <c r="I59" s="37" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4685,23 +4813,23 @@
         <v>8</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C60" s="26"/>
       <c r="D60" s="42" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="F60" s="10">
         <v>5</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="H60" s="20" t="s">
         <v>123</v>
       </c>
       <c r="I60" s="41" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4709,25 +4837,23 @@
         <v>9</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="C61" s="41" t="s">
-        <v>275</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="C61" s="26"/>
       <c r="D61" s="42" t="s">
-        <v>278</v>
+        <v>310</v>
       </c>
       <c r="F61" s="10">
         <v>6</v>
       </c>
       <c r="G61" s="31" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H61" s="32" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="I61" s="40" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4735,13 +4861,13 @@
         <v>10</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C62" s="41" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="F62" s="10">
         <v>7</v>
@@ -4750,46 +4876,46 @@
         <v>256</v>
       </c>
       <c r="H62" s="32" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="I62" s="40" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="45">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="26"/>
-      <c r="B63" s="26" t="s">
-        <v>264</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="37" t="s">
-        <v>265</v>
+      <c r="B63" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C63" s="41" t="s">
+        <v>272</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>312</v>
       </c>
       <c r="F63" s="10">
         <v>8</v>
       </c>
       <c r="G63" s="32" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="H63" s="26" t="s">
         <v>246</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="60">
       <c r="A64" s="26"/>
-      <c r="B64" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="C64" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="D64" s="32" t="s">
-        <v>268</v>
+      <c r="B64" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="37" t="s">
+        <v>311</v>
       </c>
       <c r="F64" s="10">
         <v>9</v>
@@ -4804,16 +4930,16 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9">
       <c r="A65" s="26"/>
       <c r="B65" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="D65" s="42" t="s">
-        <v>270</v>
+        <v>264</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>313</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="20" t="s">
@@ -4826,16 +4952,16 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="26"/>
-      <c r="B66" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C66" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>191</v>
+      <c r="B66" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D66" s="42" t="s">
+        <v>314</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="27"/>
@@ -4844,24 +4970,37 @@
     <row r="67" spans="1:9">
       <c r="A67" s="26"/>
       <c r="B67" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F67" s="14"/>
+      <c r="G67" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="27"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="B68" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C67" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" s="20" t="s">
+      <c r="C68" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="F67" s="14"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="5">
         <v>10</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C70" s="43"/>
       <c r="D70" s="43"/>
@@ -4891,24 +5030,24 @@
         <v>76</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="G72" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="120">
+    <row r="73" spans="1:9" ht="135">
       <c r="A73" s="46">
         <v>2</v>
       </c>
       <c r="B73" s="47" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C73" s="47" t="s">
         <v>246</v>
       </c>
       <c r="D73" s="48" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4916,13 +5055,13 @@
         <v>3</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -4930,13 +5069,13 @@
         <v>4</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C75" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D75" s="37" t="s">
         <v>305</v>
-      </c>
-      <c r="D75" s="37" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -4944,13 +5083,13 @@
         <v>5</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -4958,13 +5097,13 @@
         <v>6</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="78" spans="1:9">

</xml_diff>

<commit_message>
update revisi sub menu pembelian-tambah revisi sub menu penjualan
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Item Revisi" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="revisi sub menu brg &amp; inventory" sheetId="3" r:id="rId3"/>
-    <sheet name="revisi sub menu pembelian" sheetId="5" r:id="rId4"/>
+    <sheet name="rev brg &amp; inventory" sheetId="3" r:id="rId3"/>
+    <sheet name="rev pembelian" sheetId="5" r:id="rId4"/>
+    <sheet name="rev penjualan" sheetId="7" r:id="rId5"/>
+    <sheet name="rev marketing" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="416">
   <si>
     <t>Revisi2</t>
   </si>
@@ -901,15 +903,6 @@
     <t>varchar(20)</t>
   </si>
   <si>
-    <t>tambahkan tabel:</t>
-  </si>
-  <si>
-    <t>rekening_supplier</t>
-  </si>
-  <si>
-    <t>rekening_ukm</t>
-  </si>
-  <si>
     <t>bank_asal</t>
   </si>
   <si>
@@ -977,9 +970,6 @@
   </si>
   <si>
     <t>enum('0','1')</t>
-  </si>
-  <si>
-    <t>note:</t>
   </si>
   <si>
     <t>enum('0','1',2')</t>
@@ -1146,6 +1136,423 @@
   <si>
     <t>FK p_return_barang, nullable</t>
   </si>
+  <si>
+    <t>int(3)</t>
+  </si>
+  <si>
+    <t>p_rek_suplier</t>
+  </si>
+  <si>
+    <t>PK tabel rekening supplier</t>
+  </si>
+  <si>
+    <t>FK p_supplier</t>
+  </si>
+  <si>
+    <t>nama_bank</t>
+  </si>
+  <si>
+    <t>nama bank</t>
+  </si>
+  <si>
+    <t>no_rek</t>
+  </si>
+  <si>
+    <t>nomor rekening</t>
+  </si>
+  <si>
+    <t>atas_nama</t>
+  </si>
+  <si>
+    <t>nama pemilik rekening</t>
+  </si>
+  <si>
+    <t>p_rek_ukm</t>
+  </si>
+  <si>
+    <t>PK tabel rekening  ukm</t>
+  </si>
+  <si>
+    <t>id_usaha</t>
+  </si>
+  <si>
+    <t>FK u_perusahaan</t>
+  </si>
+  <si>
+    <t>p_tawar_jual</t>
+  </si>
+  <si>
+    <t>PK tabel penawaran penjualan</t>
+  </si>
+  <si>
+    <t>nomor penawaran penjualan</t>
+  </si>
+  <si>
+    <t>id_klien</t>
+  </si>
+  <si>
+    <t>FK tabel a_klien</t>
+  </si>
+  <si>
+    <t>tgl_berlaku</t>
+  </si>
+  <si>
+    <t>batas akhir penawaran berlaku</t>
+  </si>
+  <si>
+    <t>p_detail_tj</t>
+  </si>
+  <si>
+    <t>PK tabel detail tawar jual</t>
+  </si>
+  <si>
+    <t>id_tawar_jual</t>
+  </si>
+  <si>
+    <t>FK tabel p_tawar_jual</t>
+  </si>
+  <si>
+    <t>FK tabel p_tawar_beli</t>
+  </si>
+  <si>
+    <t>hpp harga jual</t>
+  </si>
+  <si>
+    <t>jumlah_barang</t>
+  </si>
+  <si>
+    <t>jumlah brg yg akan di tawarkan</t>
+  </si>
+  <si>
+    <t>tgl_kirim</t>
+  </si>
+  <si>
+    <t>tgl penawaran di kirim</t>
+  </si>
+  <si>
+    <t>nama_promo</t>
+  </si>
+  <si>
+    <t>text(200)</t>
+  </si>
+  <si>
+    <t>nama promo</t>
+  </si>
+  <si>
+    <t>syarat</t>
+  </si>
+  <si>
+    <t>fasilitas_promo</t>
+  </si>
+  <si>
+    <t>promo klien dapat apa saja</t>
+  </si>
+  <si>
+    <t>syarat promo apa saja</t>
+  </si>
+  <si>
+    <t>jenis_promo</t>
+  </si>
+  <si>
+    <t>0 = promo barang, 1 =promo jasa</t>
+  </si>
+  <si>
+    <t>PK tabel promo barang / jasa</t>
+  </si>
+  <si>
+    <t>tgl_dibuat</t>
+  </si>
+  <si>
+    <t>date now</t>
+  </si>
+  <si>
+    <t>batas akhir promo</t>
+  </si>
+  <si>
+    <t>PK tabel detail promo</t>
+  </si>
+  <si>
+    <t>id_jasa</t>
+  </si>
+  <si>
+    <t>harga jual barang / jasa</t>
+  </si>
+  <si>
+    <t>diskon</t>
+  </si>
+  <si>
+    <t>diskon barang /jasa</t>
+  </si>
+  <si>
+    <t>id_promo</t>
+  </si>
+  <si>
+    <t>FK p_promo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK tabel p_barang, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK tabel p_jasa, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullabel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK p_barang, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable. Jika promo jasa, ini null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK tabel p_jasa, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable. Jika promo brg,ini null</t>
+    </r>
+  </si>
+  <si>
+    <t>minimum_beli</t>
+  </si>
+  <si>
+    <t>diskon per item</t>
+  </si>
+  <si>
+    <t>m_promo</t>
+  </si>
+  <si>
+    <t>m_detail_promo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">jumlah minimum beli brg, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>p_so</t>
+  </si>
+  <si>
+    <t>tgl so</t>
+  </si>
+  <si>
+    <t>no_so</t>
+  </si>
+  <si>
+    <t>nomor so</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nomor po, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>tgl brg di kirim ke klien</t>
+  </si>
+  <si>
+    <t>dp_so</t>
+  </si>
+  <si>
+    <t>uang muka SO</t>
+  </si>
+  <si>
+    <r>
+      <t>diskon total brg so,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pajak penjualan  brg, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>kurang bayar SO</t>
+  </si>
+  <si>
+    <t>keterangan SO</t>
+  </si>
+  <si>
+    <t>status_so</t>
+  </si>
+  <si>
+    <t>p_detail_so</t>
+  </si>
+  <si>
+    <t>id_so</t>
+  </si>
+  <si>
+    <t>PK tabel detail po</t>
+  </si>
+  <si>
+    <t>PK tabel detail so</t>
+  </si>
+  <si>
+    <t>PK tabel pesanan penjualan/sales order</t>
+  </si>
+  <si>
+    <t>p_sales</t>
+  </si>
+  <si>
+    <t>PK tabel penjualan</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK tabel s_po, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>tgl_sales</t>
+  </si>
+  <si>
+    <t>tgl jual</t>
+  </si>
+  <si>
+    <t>no_sales</t>
+  </si>
+  <si>
+    <t>vachar(200)</t>
+  </si>
+  <si>
+    <t>nomor transaksi penjualan</t>
+  </si>
+  <si>
+    <t>tgl barang di kirim</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pajak penjualan brg, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>tgl jatuh tempo hutang penjualan kredit</t>
+  </si>
+  <si>
+    <t>pembayaran brg yg dijual</t>
+  </si>
+  <si>
+    <t>kurang bayar penjualan/hutang</t>
+  </si>
+  <si>
+    <t>p_detail_sales</t>
+  </si>
+  <si>
+    <t>PK tabel detail penjualan</t>
+  </si>
+  <si>
+    <t>id_sales</t>
+  </si>
+  <si>
+    <t>FK tabel p_sales</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_barang.id_barang atau p_detail_so.id_barang</t>
+  </si>
+  <si>
+    <t>jumlah_jual</t>
+  </si>
+  <si>
+    <t>jumlah brg yg akan di jual</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_detail_po.jumlah_jual ato di isi manual</t>
+  </si>
+  <si>
+    <t>jumlah harga jual per item brg</t>
+  </si>
 </sst>
 </file>
 
@@ -1155,7 +1562,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1211,8 +1618,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1237,8 +1652,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1320,12 +1741,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1412,7 +1842,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1426,11 +1855,40 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2011,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2226,10 +2684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2246,30 +2704,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -2495,11 +2953,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -2718,11 +3176,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -2740,11 +3198,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -2935,11 +3393,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="49" t="s">
+      <c r="G33" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -3109,11 +3567,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -3400,18 +3858,13 @@
       <c r="H55" s="16"/>
       <c r="I55" s="24"/>
     </row>
-    <row r="57" spans="1:9">
-      <c r="D57" t="s">
+    <row r="71" spans="4:7">
+      <c r="D71" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
-      <c r="B58" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="D61" t="s">
+    <row r="72" spans="4:7">
+      <c r="G72" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3427,16 +3880,16 @@
     <mergeCell ref="B23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3526,14 +3979,14 @@
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s">
-        <v>193</v>
+      <c r="B4" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>184</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
@@ -3544,8 +3997,8 @@
       <c r="H4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>141</v>
+      <c r="I4" s="26" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3553,13 +4006,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="F5" s="10">
         <v>3</v>
@@ -3578,14 +4031,14 @@
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>186</v>
+      <c r="B6" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>335</v>
       </c>
       <c r="F6" s="10">
         <v>4</v>
@@ -3602,16 +4055,16 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="10">
-        <v>8</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>76</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>191</v>
+        <v>345</v>
       </c>
       <c r="F7" s="10">
         <v>5</v>
@@ -3628,16 +4081,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
-        <v>9</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>97</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>185</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>98</v>
+      <c r="D8" s="26" t="s">
+        <v>186</v>
       </c>
       <c r="F8" s="10">
         <v>6</v>
@@ -3653,8 +4106,18 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="14"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>191</v>
+      </c>
       <c r="F9" s="10">
         <v>7</v>
       </c>
@@ -3669,8 +4132,18 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="F10" s="14"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
@@ -3743,7 +4216,7 @@
         <v>76</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>203</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3805,8 +4278,8 @@
       <c r="B16" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>123</v>
+      <c r="C16" s="26" t="s">
+        <v>379</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>214</v>
@@ -3981,12 +4454,6 @@
       <c r="D23" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="F23" s="45" t="s">
-        <v>299</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>273</v>
-      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10">
@@ -3996,13 +4463,10 @@
         <v>245</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>247</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4017,9 +4481,6 @@
       </c>
       <c r="D25" s="26" t="s">
         <v>191</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4387,7 +4848,7 @@
         <v>249</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D41" s="36" t="s">
         <v>268</v>
@@ -4480,7 +4941,7 @@
         <v>76</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4491,7 +4952,7 @@
         <v>250</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>251</v>
@@ -4555,10 +5016,10 @@
         <v>255</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I47" s="40" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4569,13 +5030,19 @@
         <v>256</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I48" s="40" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
+      <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" t="s">
+        <v>109</v>
+      </c>
       <c r="F49" s="10">
         <v>10</v>
       </c>
@@ -4669,13 +5136,13 @@
         <v>246</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F54" s="5">
         <v>9</v>
       </c>
       <c r="G54" s="39" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H54" s="39"/>
       <c r="I54" s="39"/>
@@ -4729,7 +5196,7 @@
         <v>76</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -4737,25 +5204,25 @@
         <v>5</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F57" s="10">
         <v>2</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H57" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I57" s="26" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="75">
@@ -4768,14 +5235,14 @@
       <c r="C58" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="51" t="s">
-        <v>315</v>
+      <c r="D58" s="49" t="s">
+        <v>311</v>
       </c>
       <c r="F58" s="10">
         <v>3</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H58" s="26" t="s">
         <v>120</v>
@@ -4790,22 +5257,22 @@
         <v>249</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F59" s="10">
         <v>4</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H59" s="26" t="s">
         <v>246</v>
       </c>
       <c r="I59" s="37" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4813,23 +5280,23 @@
         <v>8</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C60" s="26"/>
       <c r="D60" s="42" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F60" s="10">
         <v>5</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H60" s="20" t="s">
         <v>123</v>
       </c>
       <c r="I60" s="41" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4837,23 +5304,23 @@
         <v>9</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C61" s="26"/>
       <c r="D61" s="42" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F61" s="10">
         <v>6</v>
       </c>
       <c r="G61" s="31" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H61" s="32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I61" s="40" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4867,7 +5334,7 @@
         <v>270</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F62" s="10">
         <v>7</v>
@@ -4876,10 +5343,10 @@
         <v>256</v>
       </c>
       <c r="H62" s="32" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I62" s="40" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -4891,19 +5358,19 @@
         <v>272</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F63" s="10">
         <v>8</v>
       </c>
       <c r="G63" s="32" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H63" s="26" t="s">
         <v>246</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="60">
@@ -4915,7 +5382,7 @@
         <v>123</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F64" s="10">
         <v>9</v>
@@ -4930,7 +5397,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:11">
       <c r="A65" s="26"/>
       <c r="B65" s="32" t="s">
         <v>264</v>
@@ -4939,7 +5406,7 @@
         <v>265</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="20" t="s">
@@ -4952,7 +5419,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:11" ht="30">
       <c r="A66" s="26"/>
       <c r="B66" s="32" t="s">
         <v>266</v>
@@ -4961,13 +5428,13 @@
         <v>246</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="27"/>
       <c r="H66" s="27"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:11">
       <c r="A67" s="26"/>
       <c r="B67" s="20" t="s">
         <v>93</v>
@@ -4978,13 +5445,11 @@
       <c r="D67" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="F67" s="14"/>
-      <c r="G67" s="27" t="s">
-        <v>109</v>
-      </c>
+      <c r="F67" s="44"/>
+      <c r="G67" s="54"/>
       <c r="H67" s="27"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:11">
       <c r="B68" s="20" t="s">
         <v>97</v>
       </c>
@@ -4994,18 +5459,22 @@
       <c r="D68" s="20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="G68" s="54"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="G69" s="54"/>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="5">
         <v>10</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C70" s="43"/>
       <c r="D70" s="43"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:11">
       <c r="A71" s="9" t="s">
         <v>71</v>
       </c>
@@ -5019,7 +5488,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:11">
       <c r="A72" s="10">
         <v>1</v>
       </c>
@@ -5030,83 +5499,130 @@
         <v>76</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G72" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="135">
-      <c r="A73" s="46">
+    <row r="73" spans="1:11" ht="135">
+      <c r="A73" s="45">
         <v>2</v>
       </c>
-      <c r="B73" s="47" t="s">
-        <v>307</v>
-      </c>
-      <c r="C73" s="47" t="s">
+      <c r="B73" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="C73" s="46" t="s">
         <v>246</v>
       </c>
-      <c r="D73" s="48" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="D73" s="47" t="s">
+        <v>304</v>
+      </c>
+      <c r="K73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="10">
         <v>3</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>293</v>
+      </c>
+      <c r="F74" s="50">
+        <v>11</v>
+      </c>
+      <c r="G74" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="H74" s="52"/>
+      <c r="I74" s="52"/>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="10">
         <v>4</v>
       </c>
       <c r="B75" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C75" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="C75" s="26" t="s">
-        <v>298</v>
-      </c>
       <c r="D75" s="37" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>301</v>
+      </c>
+      <c r="F75" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="G75" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="H75" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="I75" s="53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="10">
         <v>5</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>300</v>
+      </c>
+      <c r="F76" s="10">
+        <v>1</v>
+      </c>
+      <c r="G76" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H76" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="10">
         <v>6</v>
       </c>
       <c r="B77" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D77" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="C77" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="D77" s="40" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="F77" s="10">
+        <v>2</v>
+      </c>
+      <c r="G77" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H77" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I77" s="26" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="10">
         <v>7</v>
       </c>
@@ -5119,8 +5635,20 @@
       <c r="D78" s="26" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="F78" s="10">
+        <v>3</v>
+      </c>
+      <c r="G78" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="H78" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="I78" s="32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="10">
         <v>8</v>
       </c>
@@ -5133,15 +5661,1571 @@
       <c r="D79" s="20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="F79" s="10">
+        <v>4</v>
+      </c>
+      <c r="G79" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="H79" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="I79" s="32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="14"/>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="14"/>
+      <c r="F80" s="10">
+        <v>5</v>
+      </c>
+      <c r="G80" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="H80" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="I80" s="32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="50">
+        <v>11</v>
+      </c>
+      <c r="B81" s="55" t="s">
+        <v>325</v>
+      </c>
+      <c r="C81" s="52"/>
+      <c r="D81" s="52"/>
+      <c r="F81" s="10">
+        <v>6</v>
+      </c>
+      <c r="G81" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="H81" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="I81" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D82" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F82" s="10">
+        <v>7</v>
+      </c>
+      <c r="G82" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="H82" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="I82" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="10">
+        <v>1</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="F83" s="14"/>
+      <c r="G83" s="27"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="10">
+        <v>2</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="C84" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="10">
+        <v>3</v>
+      </c>
+      <c r="B85" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="C85" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="D85" s="32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="10">
+        <v>4</v>
+      </c>
+      <c r="B86" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="C86" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="D86" s="32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="10">
+        <v>5</v>
+      </c>
+      <c r="B87" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="C87" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="D87" s="32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="10">
+        <v>6</v>
+      </c>
+      <c r="B88" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D88" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="10">
+        <v>7</v>
+      </c>
+      <c r="B89" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="D89" s="32" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5">
+        <v>1</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="F1" s="5">
+        <v>2</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>360</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="H8" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="61" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="F9" s="10">
+        <v>7</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="10">
+        <v>9</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>375</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="F14" s="5">
+        <v>4</v>
+      </c>
+      <c r="G14" s="57" t="s">
+        <v>389</v>
+      </c>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="10">
+        <v>1</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="10">
+        <v>2</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="10">
+        <v>3</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="F18" s="10">
+        <v>3</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="10">
+        <v>4</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="F19" s="10">
+        <v>4</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="10">
+        <v>5</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="F20" s="10">
+        <v>5</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="10">
+        <v>6</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="F21" s="10">
+        <v>6</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="10">
+        <v>7</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="F22" s="10">
+        <v>7</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="10">
+        <v>8</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="F23" s="10">
+        <v>8</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10">
+        <v>9</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="F24" s="10">
+        <v>9</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="10">
+        <v>10</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="10">
+        <v>11</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="10">
+        <v>12</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="10">
+        <v>13</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="10">
+        <v>14</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="10">
+        <v>15</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="5">
+        <v>5</v>
+      </c>
+      <c r="B32" s="57" t="s">
+        <v>394</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="F32" s="5">
+        <v>6</v>
+      </c>
+      <c r="G32" s="57" t="s">
+        <v>407</v>
+      </c>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="10">
+        <v>1</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="10">
+        <v>2</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="F35" s="10">
+        <v>2</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30">
+      <c r="A36" s="10">
+        <v>3</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="F36" s="10">
+        <v>3</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="37" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30">
+      <c r="A37" s="10">
+        <v>4</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="F37" s="10">
+        <v>4</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30">
+      <c r="A38" s="10">
+        <v>5</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="F38" s="10">
+        <v>5</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="37" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="10">
+        <v>6</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>344</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="F39" s="10">
+        <v>6</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="10">
+        <v>7</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="F40" s="10">
+        <v>7</v>
+      </c>
+      <c r="G40" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="10">
+        <v>8</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="F41" s="10">
+        <v>8</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="10">
+        <v>9</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>383</v>
+      </c>
+      <c r="F42" s="10">
+        <v>9</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="10">
+        <v>10</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="10">
+        <v>11</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="10">
+        <v>12</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="10">
+        <v>13</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="10">
+        <v>14</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="10">
+        <v>15</v>
+      </c>
+      <c r="B48" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="10">
+        <v>16</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="10">
+        <v>17</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="10">
+        <v>18</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="9">
+        <v>13</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="F1" s="9">
+        <v>14</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="F9" s="10">
+        <v>7</v>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="10">
+        <v>9</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update revisi pembelian-update tabel revisi- revisi penjualan: final jurnal sub menu penjualan otomatis
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="464">
   <si>
     <t>Revisi2</t>
   </si>
@@ -861,18 +861,9 @@
     <t>p_bayar</t>
   </si>
   <si>
-    <t>PK tabel pembayaran</t>
-  </si>
-  <si>
     <t>jenis_bayar</t>
   </si>
   <si>
-    <t>FK p_po, nullable</t>
-  </si>
-  <si>
-    <t>FK p_order, nullable</t>
-  </si>
-  <si>
     <t>jumlah_bayar</t>
   </si>
   <si>
@@ -915,9 +906,6 @@
     <t>bisa di ambil dari p_detail_po.jumlah_beli ato di isi manual jika beli tanpa PO</t>
   </si>
   <si>
-    <t>p_return_brg</t>
-  </si>
-  <si>
     <t>PK tabel return</t>
   </si>
   <si>
@@ -994,12 +982,6 @@
   </si>
   <si>
     <t>jenis_jurnal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 = PO, 1 = pembelian tunai tanpa pajak, 2=pembelian tunai dg pajak, 3 = pembelian kredit tanpa pajak, 4= pembelian kredit dg pajak, 5=  Beban angkut pembelian,
-5=Return pembelian tunai
-6= Return pembelian kredit
-</t>
   </si>
   <si>
     <t>0 = transfer bank, 1 = cek, 2 = langsung, 3 = return barang</t>
@@ -1018,9 +1000,6 @@
       </rPr>
       <t>nullabe</t>
     </r>
-  </si>
-  <si>
-    <t>jika bayar po, ambil data p_po.dp_po. Jika bayar order : ambil data p_order.bayar, jika return pembelian: ambil data total hrg brg yg di return</t>
   </si>
   <si>
     <r>
@@ -1128,9 +1107,6 @@
     </r>
   </si>
   <si>
-    <t>0= bayar PO, 1 = bayar order. 3 = return brg</t>
-  </si>
-  <si>
     <t>id_return_barang</t>
   </si>
   <si>
@@ -1518,15 +1494,9 @@
     </r>
   </si>
   <si>
-    <t>tgl jatuh tempo hutang penjualan kredit</t>
-  </si>
-  <si>
     <t>pembayaran brg yg dijual</t>
   </si>
   <si>
-    <t>kurang bayar penjualan/hutang</t>
-  </si>
-  <si>
     <t>p_detail_sales</t>
   </si>
   <si>
@@ -1552,17 +1522,450 @@
   </si>
   <si>
     <t>jumlah harga jual per item brg</t>
+  </si>
+  <si>
+    <t>p_komisi_sales</t>
+  </si>
+  <si>
+    <t>PK tabel komisi salesman</t>
+  </si>
+  <si>
+    <t>id_ky</t>
+  </si>
+  <si>
+    <t>PK p_karyawan</t>
+  </si>
+  <si>
+    <t>jenis_komisi</t>
+  </si>
+  <si>
+    <t>persen_komisi</t>
+  </si>
+  <si>
+    <t>besarnya persentase komisi, mis: 5 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = komisi per harga barang, 1= komisi per faktur </t>
+  </si>
+  <si>
+    <t>id_komisi_sales</t>
+  </si>
+  <si>
+    <t>FK tabel p_komisi_sales</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>jika bayar po</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, ambil data p_po.dp_po. Jika </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bayar order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : ambil data p_order.bayar, jika </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>return pembelian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: ambil data total hrg brg yg di return</t>
+    </r>
+  </si>
+  <si>
+    <t>kurang bayar penjualan/piutang</t>
+  </si>
+  <si>
+    <t>tgl jatuh tempo piutang penjualan kredit</t>
+  </si>
+  <si>
+    <t>PK tabel pembayaran pembelian</t>
+  </si>
+  <si>
+    <t>p_terima_bayar</t>
+  </si>
+  <si>
+    <t>PK tabel pembayaran penjualan</t>
+  </si>
+  <si>
+    <t>0= bayar SO, 1 = bayar sales. 3 = return brg jual</t>
+  </si>
+  <si>
+    <t>0= bayar PO, 1 = bayar order. 3 = return brg beli</t>
+  </si>
+  <si>
+    <t>FK p_so, nullable</t>
+  </si>
+  <si>
+    <t>FK p_sales, nullable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK p_return_barang, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK p_order, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK p_po, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>0 = transfer bank, 1 = cek, 2 = langsung, 3 = return barang jual</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">p_rek_ukm,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullabe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">p_rek_klien, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullabe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">p_klien, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullabe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>jika bayar so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, ambil data p_so.dp_so. Jika </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bayar sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : ambil data p_sales.bayar, jika </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>return penjualan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: ambil data total hrg brg yg di return</t>
+    </r>
+  </si>
+  <si>
+    <t>terima_bukti</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0= uang blm masuk, 1 =uang sdh masuk, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>jika bayar so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,  p_so.tgl_so (editable),    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>jika bayar order,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  p_sales.tgl_sales (editable),                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jika return penjualam : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>p_return_brg.tgl_return</t>
+    </r>
+  </si>
+  <si>
+    <t>p_rek_klien</t>
+  </si>
+  <si>
+    <t>PK tabel rekening  klien</t>
+  </si>
+  <si>
+    <t>FK a_klien</t>
+  </si>
+  <si>
+    <t>0 = di terima, 1 = ditolak</t>
+  </si>
+  <si>
+    <t>p_complain_barang</t>
+  </si>
+  <si>
+    <t>bisa di ambil dari p_barang.hpp atau p_detail_so.hpp</t>
+  </si>
+  <si>
+    <t>complain_jumlah</t>
+  </si>
+  <si>
+    <t>complain_kualitas</t>
+  </si>
+  <si>
+    <t>jumlah brg yg kurang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kualitas brg </t>
+  </si>
+  <si>
+    <t>keterangan tambahan</t>
+  </si>
+  <si>
+    <t>status_complain</t>
+  </si>
+  <si>
+    <t>alasan_ditolak</t>
+  </si>
+  <si>
+    <t>alasan diterima atau di tolak complain brg dr klien</t>
+  </si>
+  <si>
+    <t>konfirm_klien</t>
+  </si>
+  <si>
+    <t>0 = sdh konfirm ke klien, 1 = blm konfirm ke klien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alasan return di tolak </t>
+  </si>
+  <si>
+    <t>p_return_penjualan</t>
+  </si>
+  <si>
+    <t>p_return_pembelian</t>
+  </si>
+  <si>
+    <t>PK tabel return penjualan</t>
+  </si>
+  <si>
+    <t>id_complain_barang</t>
+  </si>
+  <si>
+    <t>FK tabel p_complain_barang</t>
+  </si>
+  <si>
+    <t>p_akun_penjualan</t>
+  </si>
+  <si>
+    <t>PK tabel seting akun sub menu penjualan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = Pesanan Pembelian tunai, 1 = Pesanan Pembelian transfer,  2 = pembelian tunai tanpa pajak, 3=pembelian tunai dg pajak, 4 = pembelian kredit tanpa pajak, 5= pembelian kredit dg pajak, 6=  Beban angkut pembelian,
+7=Return pembelian tunai
+8= Return pembelian kredit
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = Pesanan Penjualan tunai, 1 = Pesanan Penjualan transfer, 2 = Pesanan Penjualan tunai dg pajak, 3 = Pesanan Penjualan transfer dg pajak, 4 = penjualan tunai tanpa pajak, 5 =penjualan tunai dg pajak, 6 = penjualan kredit tanpa pajak, 7= penjualan kredit dg pajak, 8= potongan penjualan tunai; 9=  Beban angkut penjualan,
+10=Return penjualan mengambalikan kas
+11= Return penjualan kurangi piutang
+12 = return penjualan mengembalikan barang
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1572,13 +1975,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1751,11 +2147,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1811,7 +2206,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1842,7 +2236,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1855,23 +2249,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1887,12 +2281,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2686,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2704,30 +3121,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -2953,11 +3370,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="62" t="s">
+      <c r="G12" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -3176,11 +3593,11 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="73" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -3198,11 +3615,11 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="62" t="s">
+      <c r="G24" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10">
@@ -3393,11 +3810,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="62" t="s">
+      <c r="G33" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10">
@@ -3567,11 +3984,11 @@
       <c r="A43" s="5">
         <v>9</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
       <c r="F43" s="14"/>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -3888,8 +4305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:I36"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3897,7 +4314,7 @@
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
@@ -3917,7 +4334,7 @@
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>202</v>
       </c>
       <c r="H1" s="8"/>
@@ -3998,7 +4415,7 @@
         <v>76</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4032,13 +4449,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F6" s="10">
         <v>4</v>
@@ -4058,13 +4475,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F7" s="10">
         <v>5</v>
@@ -4153,19 +4570,19 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
       <c r="F11" s="5">
         <v>4</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="9" t="s">
@@ -4216,7 +4633,7 @@
         <v>76</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4279,7 +4696,7 @@
         <v>197</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>214</v>
@@ -4327,25 +4744,25 @@
       <c r="A18" s="10">
         <v>6</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>220</v>
       </c>
       <c r="F18" s="10">
         <v>6</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="H18" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" s="32" t="s">
+      <c r="H18" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="31" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4353,25 +4770,25 @@
       <c r="A19" s="10">
         <v>7</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="32" t="s">
+      <c r="C19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="31" t="s">
         <v>210</v>
       </c>
       <c r="F19" s="10">
         <v>7</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="31" t="s">
         <v>199</v>
       </c>
       <c r="H19" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="31" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4379,7 +4796,7 @@
       <c r="A20" s="10">
         <v>8</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="31" t="s">
         <v>201</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -4405,13 +4822,13 @@
       <c r="A21" s="10">
         <v>9</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="35" t="s">
         <v>213</v>
       </c>
       <c r="F21" s="10">
@@ -4431,13 +4848,13 @@
       <c r="A22" s="10">
         <v>10</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="31" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4445,13 +4862,13 @@
       <c r="A23" s="10">
         <v>11</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="31" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4459,13 +4876,13 @@
       <c r="A24" s="10">
         <v>12</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="C24" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="D24" s="32" t="s">
+      <c r="C24" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="D24" s="31" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4499,11 +4916,11 @@
       <c r="F26" s="5">
         <v>6</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G26" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:9">
       <c r="F27" s="9" t="s">
@@ -4523,11 +4940,11 @@
       <c r="A28" s="5">
         <v>5</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
       <c r="F28" s="10">
         <v>1</v>
       </c>
@@ -4589,7 +5006,7 @@
       <c r="H30" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I30" s="37" t="s">
+      <c r="I30" s="36" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4618,7 +5035,7 @@
       <c r="H31" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I31" s="37" t="s">
+      <c r="I31" s="36" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4644,7 +5061,7 @@
       <c r="H32" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="37" t="s">
+      <c r="I32" s="36" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4664,13 +5081,13 @@
       <c r="F33" s="10">
         <v>6</v>
       </c>
-      <c r="G33" s="32" t="s">
+      <c r="G33" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="H33" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="32" t="s">
+      <c r="H33" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="31" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4690,13 +5107,13 @@
       <c r="F34" s="10">
         <v>7</v>
       </c>
-      <c r="G34" s="32" t="s">
+      <c r="G34" s="31" t="s">
         <v>199</v>
       </c>
       <c r="H34" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I34" s="32" t="s">
+      <c r="I34" s="31" t="s">
         <v>237</v>
       </c>
     </row>
@@ -4704,13 +5121,13 @@
       <c r="A35" s="10">
         <v>6</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="30" t="s">
         <v>229</v>
       </c>
       <c r="F35" s="10">
@@ -4730,13 +5147,13 @@
       <c r="A36" s="10">
         <v>7</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C36" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="32" t="s">
+      <c r="C36" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="31" t="s">
         <v>210</v>
       </c>
       <c r="F36" s="10">
@@ -4756,7 +5173,7 @@
       <c r="A37" s="10">
         <v>8</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="31" t="s">
         <v>201</v>
       </c>
       <c r="C37" s="26" t="s">
@@ -4770,35 +5187,35 @@
       <c r="A38" s="10">
         <v>9</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="35" t="s">
         <v>213</v>
       </c>
       <c r="F38" s="5">
         <v>7</v>
       </c>
-      <c r="G38" s="38" t="s">
+      <c r="G38" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="10">
         <v>10</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>231</v>
       </c>
       <c r="F39" s="9" t="s">
@@ -4818,13 +5235,13 @@
       <c r="A40" s="10">
         <v>11</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="35" t="s">
         <v>248</v>
       </c>
       <c r="F40" s="10">
@@ -4844,14 +5261,14 @@
       <c r="A41" s="10">
         <v>12</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>249</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="D41" s="36" t="s">
-        <v>268</v>
+        <v>291</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>265</v>
       </c>
       <c r="F41" s="10">
         <v>2</v>
@@ -4870,13 +5287,13 @@
       <c r="A42" s="10">
         <v>13</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="32" t="s">
+      <c r="D42" s="31" t="s">
         <v>242</v>
       </c>
       <c r="F42" s="10">
@@ -4888,7 +5305,7 @@
       <c r="H42" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I42" s="37" t="s">
+      <c r="I42" s="36" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4896,13 +5313,13 @@
       <c r="A43" s="10">
         <v>14</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="33" t="s">
         <v>233</v>
       </c>
       <c r="F43" s="10">
@@ -4914,7 +5331,7 @@
       <c r="H43" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I43" s="37" t="s">
+      <c r="I43" s="36" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4922,13 +5339,13 @@
       <c r="A44" s="10">
         <v>15</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="35" t="s">
         <v>243</v>
       </c>
       <c r="F44" s="10">
@@ -4940,8 +5357,8 @@
       <c r="H44" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I44" s="37" t="s">
-        <v>276</v>
+      <c r="I44" s="36" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4952,7 +5369,7 @@
         <v>250</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D45" s="26" t="s">
         <v>251</v>
@@ -4960,13 +5377,13 @@
       <c r="F45" s="10">
         <v>6</v>
       </c>
-      <c r="G45" s="32" t="s">
+      <c r="G45" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="H45" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="I45" s="32" t="s">
+      <c r="H45" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45" s="31" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4986,13 +5403,13 @@
       <c r="F46" s="10">
         <v>7</v>
       </c>
-      <c r="G46" s="32" t="s">
+      <c r="G46" s="31" t="s">
         <v>199</v>
       </c>
       <c r="H46" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I46" s="32" t="s">
+      <c r="I46" s="31" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5012,28 +5429,28 @@
       <c r="F47" s="10">
         <v>8</v>
       </c>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="H47" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="I47" s="40" t="s">
-        <v>275</v>
+      <c r="H47" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="I47" s="39" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="F48" s="10">
         <v>9</v>
       </c>
-      <c r="G48" s="32" t="s">
+      <c r="G48" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="H48" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="I48" s="40" t="s">
-        <v>275</v>
+      <c r="H48" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="I48" s="39" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
@@ -5046,13 +5463,13 @@
       <c r="F49" s="10">
         <v>10</v>
       </c>
-      <c r="G49" s="32" t="s">
+      <c r="G49" s="66" t="s">
         <v>165</v>
       </c>
-      <c r="H49" s="41" t="s">
+      <c r="H49" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="I49" s="40" t="s">
+      <c r="I49" s="39" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5060,36 +5477,36 @@
       <c r="F50" s="10">
         <v>11</v>
       </c>
-      <c r="G50" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H50" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I50" s="26" t="s">
-        <v>191</v>
+      <c r="G50" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="H50" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="I50" s="41" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="5">
         <v>8</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="61" t="s">
         <v>258</v>
       </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
       <c r="F51" s="10">
         <v>12</v>
       </c>
-      <c r="G51" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I51" s="20" t="s">
-        <v>98</v>
+      <c r="G51" s="31" t="s">
+        <v>450</v>
+      </c>
+      <c r="H51" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="I51" s="41" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -5105,7 +5522,18 @@
       <c r="D52" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H52" s="29"/>
+      <c r="F52" s="10">
+        <v>13</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H52" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I52" s="26" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="10">
@@ -5118,34 +5546,34 @@
         <v>76</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="G53" t="s">
-        <v>109</v>
-      </c>
-      <c r="H53" s="29"/>
+        <v>420</v>
+      </c>
+      <c r="F53" s="10">
+        <v>14</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H53" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I53" s="20" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="10">
         <v>2</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>246</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="F54" s="5">
-        <v>9</v>
-      </c>
-      <c r="G54" s="39" t="s">
-        <v>277</v>
-      </c>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
+        <v>424</v>
+      </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="10">
@@ -5157,21 +5585,17 @@
       <c r="C55" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D55" s="37" t="s">
-        <v>261</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I55" s="9" t="s">
-        <v>74</v>
-      </c>
+      <c r="D55" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="F55" s="5">
+        <v>9</v>
+      </c>
+      <c r="G55" s="64" t="s">
+        <v>456</v>
+      </c>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="10">
@@ -5183,141 +5607,141 @@
       <c r="C56" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="37" t="s">
-        <v>262</v>
-      </c>
-      <c r="F56" s="10">
-        <v>1</v>
-      </c>
-      <c r="G56" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H56" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I56" s="25" t="s">
-        <v>278</v>
+      <c r="D56" s="36" t="s">
+        <v>428</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="10">
         <v>5</v>
       </c>
-      <c r="B57" s="31" t="s">
-        <v>313</v>
+      <c r="B57" s="30" t="s">
+        <v>306</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D57" s="37" t="s">
-        <v>314</v>
+      <c r="D57" s="36" t="s">
+        <v>427</v>
       </c>
       <c r="F57" s="10">
-        <v>2</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>279</v>
+        <v>1</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>75</v>
       </c>
       <c r="H57" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I57" s="26" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="75">
+      <c r="I57" s="25" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="60">
       <c r="A58" s="10">
         <v>6</v>
       </c>
-      <c r="B58" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="C58" s="41" t="s">
+      <c r="B58" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C58" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="49" t="s">
-        <v>311</v>
+      <c r="D58" s="48" t="s">
+        <v>305</v>
       </c>
       <c r="F58" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="I58" s="37"/>
+        <v>275</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I58" s="26" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="59" spans="1:9" ht="30">
       <c r="A59" s="10">
         <v>7</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="31" t="s">
         <v>249</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>305</v>
+        <v>292</v>
+      </c>
+      <c r="D59" s="36" t="s">
+        <v>300</v>
       </c>
       <c r="F59" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="I59" s="37" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>120</v>
+      </c>
+      <c r="I59" s="36"/>
+    </row>
+    <row r="60" spans="1:9" ht="30">
       <c r="A60" s="10">
         <v>8</v>
       </c>
-      <c r="B60" s="32" t="s">
-        <v>273</v>
+      <c r="B60" s="31" t="s">
+        <v>270</v>
       </c>
       <c r="C60" s="26"/>
-      <c r="D60" s="42" t="s">
-        <v>306</v>
+      <c r="D60" s="41" t="s">
+        <v>301</v>
       </c>
       <c r="F60" s="10">
-        <v>5</v>
-      </c>
-      <c r="G60" s="32" t="s">
-        <v>288</v>
-      </c>
-      <c r="H60" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I60" s="41" t="s">
-        <v>289</v>
+        <v>4</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="H60" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="I60" s="36" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="10">
         <v>9</v>
       </c>
-      <c r="B61" s="32" t="s">
-        <v>274</v>
+      <c r="B61" s="31" t="s">
+        <v>271</v>
       </c>
       <c r="C61" s="26"/>
-      <c r="D61" s="42" t="s">
-        <v>306</v>
+      <c r="D61" s="41" t="s">
+        <v>301</v>
       </c>
       <c r="F61" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G61" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="H61" s="32" t="s">
-        <v>295</v>
+      <c r="H61" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="I61" s="40" t="s">
         <v>285</v>
@@ -5327,65 +5751,69 @@
       <c r="A62" s="10">
         <v>10</v>
       </c>
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="C62" s="40" t="s">
+        <v>267</v>
+      </c>
+      <c r="D62" s="41" t="s">
+        <v>302</v>
+      </c>
+      <c r="F62" s="10">
+        <v>6</v>
+      </c>
+      <c r="G62" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="I62" s="39" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="10">
+        <v>11</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="C63" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="C62" s="41" t="s">
-        <v>270</v>
-      </c>
-      <c r="D62" s="42" t="s">
-        <v>308</v>
-      </c>
-      <c r="F62" s="10">
+      <c r="D63" s="41" t="s">
+        <v>302</v>
+      </c>
+      <c r="F63" s="10">
         <v>7</v>
       </c>
-      <c r="G62" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="H62" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="I62" s="40" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="26"/>
-      <c r="B63" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="C63" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="D63" s="42" t="s">
-        <v>308</v>
-      </c>
-      <c r="F63" s="10">
-        <v>8</v>
-      </c>
-      <c r="G63" s="32" t="s">
-        <v>286</v>
+      <c r="G63" s="31" t="s">
+        <v>282</v>
       </c>
       <c r="H63" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="I63" s="32" t="s">
-        <v>287</v>
+      <c r="I63" s="31" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="60">
-      <c r="A64" s="26"/>
+      <c r="A64" s="10">
+        <v>12</v>
+      </c>
       <c r="B64" s="26" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D64" s="37" t="s">
-        <v>307</v>
+      <c r="D64" s="48" t="s">
+        <v>417</v>
       </c>
       <c r="F64" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>93</v>
@@ -5398,17 +5826,21 @@
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="26"/>
-      <c r="B65" s="32" t="s">
-        <v>264</v>
+      <c r="A65" s="10">
+        <v>13</v>
+      </c>
+      <c r="B65" s="31" t="s">
+        <v>261</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="D65" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="F65" s="10"/>
+        <v>262</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>303</v>
+      </c>
+      <c r="F65" s="10">
+        <v>9</v>
+      </c>
       <c r="G65" s="20" t="s">
         <v>97</v>
       </c>
@@ -5420,22 +5852,25 @@
       </c>
     </row>
     <row r="66" spans="1:11" ht="30">
-      <c r="A66" s="26"/>
-      <c r="B66" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="C66" s="32" t="s">
+      <c r="A66" s="10">
+        <v>14</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C66" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="D66" s="42" t="s">
-        <v>310</v>
+      <c r="D66" s="41" t="s">
+        <v>304</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="26"/>
+      <c r="A67" s="10">
+        <v>15</v>
+      </c>
       <c r="B67" s="20" t="s">
         <v>93</v>
       </c>
@@ -5445,11 +5880,14 @@
       <c r="D67" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="F67" s="44"/>
-      <c r="G67" s="54"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="53"/>
       <c r="H67" s="27"/>
     </row>
     <row r="68" spans="1:11">
+      <c r="A68" s="10">
+        <v>16</v>
+      </c>
       <c r="B68" s="20" t="s">
         <v>97</v>
       </c>
@@ -5459,20 +5897,20 @@
       <c r="D68" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G68" s="54"/>
+      <c r="G68" s="53"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="G69" s="54"/>
+      <c r="G69" s="53"/>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="5">
         <v>10</v>
       </c>
-      <c r="B70" s="43" t="s">
-        <v>290</v>
-      </c>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
+      <c r="B70" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="9" t="s">
@@ -5499,24 +5937,24 @@
         <v>76</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G72" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="135">
-      <c r="A73" s="45">
+      <c r="A73" s="44">
         <v>2</v>
       </c>
-      <c r="B73" s="46" t="s">
-        <v>303</v>
-      </c>
-      <c r="C73" s="46" t="s">
+      <c r="B73" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C73" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="D73" s="47" t="s">
-        <v>304</v>
+      <c r="D73" s="46" t="s">
+        <v>462</v>
       </c>
       <c r="K73" t="s">
         <v>109</v>
@@ -5527,46 +5965,46 @@
         <v>3</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D74" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="F74" s="50">
+      <c r="D74" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="F74" s="49">
         <v>11</v>
       </c>
-      <c r="G74" s="51" t="s">
-        <v>316</v>
-      </c>
-      <c r="H74" s="52"/>
-      <c r="I74" s="52"/>
+      <c r="G74" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="H74" s="51"/>
+      <c r="I74" s="51"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="10">
         <v>4</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="D75" s="37" t="s">
-        <v>301</v>
-      </c>
-      <c r="F75" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="D75" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="F75" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G75" s="53" t="s">
+      <c r="G75" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="H75" s="53" t="s">
+      <c r="H75" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="I75" s="53" t="s">
+      <c r="I75" s="52" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5574,14 +6012,14 @@
       <c r="A76" s="10">
         <v>5</v>
       </c>
-      <c r="B76" s="32" t="s">
-        <v>297</v>
+      <c r="B76" s="31" t="s">
+        <v>293</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="D76" s="32" t="s">
-        <v>300</v>
+        <v>295</v>
+      </c>
+      <c r="D76" s="31" t="s">
+        <v>296</v>
       </c>
       <c r="F76" s="10">
         <v>1</v>
@@ -5593,21 +6031,21 @@
         <v>76</v>
       </c>
       <c r="I76" s="25" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="10">
         <v>6</v>
       </c>
-      <c r="B77" s="31" t="s">
+      <c r="B77" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D77" s="39" t="s">
         <v>298</v>
-      </c>
-      <c r="C77" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="D77" s="40" t="s">
-        <v>302</v>
       </c>
       <c r="F77" s="10">
         <v>2</v>
@@ -5619,7 +6057,7 @@
         <v>76</v>
       </c>
       <c r="I77" s="26" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -5638,14 +6076,14 @@
       <c r="F78" s="10">
         <v>3</v>
       </c>
-      <c r="G78" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="H78" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="I78" s="32" t="s">
-        <v>320</v>
+      <c r="G78" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="H78" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="I78" s="31" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -5664,14 +6102,14 @@
       <c r="F79" s="10">
         <v>4</v>
       </c>
-      <c r="G79" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="H79" s="32" t="s">
+      <c r="G79" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="H79" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="I79" s="32" t="s">
-        <v>322</v>
+      <c r="I79" s="31" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -5679,61 +6117,61 @@
       <c r="F80" s="10">
         <v>5</v>
       </c>
-      <c r="G80" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="H80" s="32" t="s">
+      <c r="G80" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="H80" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="I80" s="32" t="s">
-        <v>324</v>
+      <c r="I80" s="31" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="50">
+      <c r="A81" s="49">
         <v>11</v>
       </c>
-      <c r="B81" s="55" t="s">
-        <v>325</v>
-      </c>
-      <c r="C81" s="52"/>
-      <c r="D81" s="52"/>
+      <c r="B81" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="C81" s="51"/>
+      <c r="D81" s="51"/>
       <c r="F81" s="10">
         <v>6</v>
       </c>
-      <c r="G81" s="32" t="s">
+      <c r="G81" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="H81" s="32" t="s">
+      <c r="H81" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="I81" s="32" t="s">
+      <c r="I81" s="31" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="53" t="s">
+      <c r="A82" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B82" s="53" t="s">
+      <c r="B82" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C82" s="53" t="s">
+      <c r="C82" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="D82" s="53" t="s">
+      <c r="D82" s="52" t="s">
         <v>74</v>
       </c>
       <c r="F82" s="10">
         <v>7</v>
       </c>
-      <c r="G82" s="32" t="s">
+      <c r="G82" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="H82" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="I82" s="32" t="s">
+      <c r="H82" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="I82" s="31" t="s">
         <v>98</v>
       </c>
     </row>
@@ -5748,7 +6186,7 @@
         <v>76</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F83" s="14"/>
       <c r="G83" s="27"/>
@@ -5758,68 +6196,68 @@
         <v>2</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="10">
         <v>3</v>
       </c>
-      <c r="B85" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="C85" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="D85" s="32" t="s">
-        <v>320</v>
+      <c r="B85" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="C85" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="D85" s="31" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="10">
         <v>4</v>
       </c>
-      <c r="B86" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="C86" s="32" t="s">
+      <c r="B86" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="C86" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D86" s="32" t="s">
-        <v>322</v>
+      <c r="D86" s="31" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="10">
         <v>5</v>
       </c>
-      <c r="B87" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="C87" s="32" t="s">
+      <c r="B87" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="C87" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D87" s="32" t="s">
-        <v>324</v>
+      <c r="D87" s="31" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="10">
         <v>6</v>
       </c>
-      <c r="B88" s="32" t="s">
+      <c r="B88" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="C88" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="D88" s="32" t="s">
+      <c r="D88" s="31" t="s">
         <v>94</v>
       </c>
     </row>
@@ -5827,13 +6265,13 @@
       <c r="A89" s="10">
         <v>7</v>
       </c>
-      <c r="B89" s="32" t="s">
+      <c r="B89" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="C89" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="D89" s="32" t="s">
+      <c r="C89" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="D89" s="31" t="s">
         <v>98</v>
       </c>
     </row>
@@ -5845,42 +6283,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>329</v>
-      </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="48" t="s">
-        <v>336</v>
-      </c>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="G1" s="47" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -5919,7 +6357,7 @@
         <v>76</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -5931,7 +6369,7 @@
         <v>76</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5939,25 +6377,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C4" t="s">
         <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -5971,7 +6409,7 @@
         <v>174</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="F5" s="10">
         <v>3</v>
@@ -5983,7 +6421,7 @@
         <v>76</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -6002,14 +6440,14 @@
       <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="58" t="s">
+        <v>353</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="58" t="s">
         <v>360</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="59" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -6017,13 +6455,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F7" s="10">
         <v>5</v>
@@ -6035,7 +6473,7 @@
         <v>123</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6043,25 +6481,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F8" s="10">
         <v>6</v>
       </c>
-      <c r="G8" s="60" t="s">
-        <v>362</v>
-      </c>
-      <c r="H8" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="61" t="s">
-        <v>371</v>
+      <c r="G8" s="59" t="s">
+        <v>355</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="60" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -6069,38 +6507,38 @@
         <v>7</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F9" s="10">
         <v>7</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>76</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>243</v>
       </c>
       <c r="F10" s="10">
@@ -6160,19 +6598,19 @@
       <c r="A14" s="5">
         <v>3</v>
       </c>
-      <c r="B14" s="57" t="s">
-        <v>375</v>
-      </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="B14" s="56" t="s">
+        <v>368</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
       <c r="F14" s="5">
         <v>4</v>
       </c>
-      <c r="G14" s="57" t="s">
-        <v>389</v>
-      </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
+      <c r="G14" s="56" t="s">
+        <v>382</v>
+      </c>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
@@ -6210,8 +6648,8 @@
       <c r="C16" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>393</v>
+      <c r="D16" s="72" t="s">
+        <v>386</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
@@ -6223,7 +6661,7 @@
         <v>76</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -6243,7 +6681,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="H17" s="20" t="s">
         <v>76</v>
@@ -6263,7 +6701,7 @@
         <v>76</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F18" s="10">
         <v>3</v>
@@ -6283,13 +6721,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="F19" s="10">
         <v>4</v>
@@ -6312,22 +6750,22 @@
         <v>197</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F20" s="10">
         <v>5</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="H20" s="26" t="s">
         <v>76</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -6335,24 +6773,24 @@
         <v>6</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F21" s="10">
         <v>6</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="H21" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="32" t="s">
+      <c r="H21" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="31" t="s">
         <v>211</v>
       </c>
     </row>
@@ -6360,25 +6798,25 @@
       <c r="A22" s="10">
         <v>7</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="31" t="s">
-        <v>381</v>
+      <c r="D22" s="30" t="s">
+        <v>374</v>
       </c>
       <c r="F22" s="10">
         <v>7</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="31" t="s">
         <v>199</v>
       </c>
       <c r="H22" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="31" t="s">
         <v>200</v>
       </c>
     </row>
@@ -6386,14 +6824,14 @@
       <c r="A23" s="10">
         <v>8</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C23" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>384</v>
+      <c r="C23" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>377</v>
       </c>
       <c r="F23" s="10">
         <v>8</v>
@@ -6412,14 +6850,14 @@
       <c r="A24" s="10">
         <v>9</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="31" t="s">
         <v>201</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="F24" s="10">
         <v>9</v>
@@ -6438,55 +6876,55 @@
       <c r="A25" s="10">
         <v>10</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>382</v>
-      </c>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="36" t="s">
-        <v>383</v>
+      <c r="D25" s="35" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="10">
         <v>11</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="32" t="s">
-        <v>386</v>
+      <c r="D26" s="31" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="10">
         <v>12</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>387</v>
+      <c r="D27" s="31" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="10">
         <v>13</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>388</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="D28" s="32" t="s">
+      <c r="B28" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="D28" s="31" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6522,19 +6960,19 @@
       <c r="A32" s="5">
         <v>5</v>
       </c>
-      <c r="B32" s="57" t="s">
-        <v>394</v>
-      </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
+      <c r="B32" s="56" t="s">
+        <v>387</v>
+      </c>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
       <c r="F32" s="5">
         <v>6</v>
       </c>
-      <c r="G32" s="57" t="s">
-        <v>407</v>
-      </c>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
+      <c r="G32" s="56" t="s">
+        <v>398</v>
+      </c>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="9" t="s">
@@ -6573,7 +7011,7 @@
         <v>76</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F34" s="10">
         <v>1</v>
@@ -6585,7 +7023,7 @@
         <v>76</v>
       </c>
       <c r="I34" s="25" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -6593,25 +7031,25 @@
         <v>2</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="F35" s="10">
         <v>2</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I35" s="26" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30">
@@ -6619,13 +7057,13 @@
         <v>3</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="F36" s="10">
         <v>3</v>
@@ -6636,8 +7074,8 @@
       <c r="H36" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I36" s="37" t="s">
-        <v>411</v>
+      <c r="I36" s="36" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30">
@@ -6645,13 +7083,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F37" s="10">
         <v>4</v>
@@ -6662,7 +7100,7 @@
       <c r="H37" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I37" s="37" t="s">
+      <c r="I37" s="36" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6671,50 +7109,50 @@
         <v>5</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F38" s="10">
         <v>5</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="H38" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I38" s="37" t="s">
-        <v>414</v>
+      <c r="I38" s="36" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="10">
         <v>6</v>
       </c>
-      <c r="B39" s="31" t="s">
-        <v>344</v>
-      </c>
-      <c r="C39" s="35" t="s">
+      <c r="B39" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="C39" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="31" t="s">
-        <v>402</v>
+      <c r="D39" s="30" t="s">
+        <v>395</v>
       </c>
       <c r="F39" s="10">
         <v>6</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="H39" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="I39" s="32" t="s">
+      <c r="H39" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="31" t="s">
         <v>211</v>
       </c>
     </row>
@@ -6722,40 +7160,40 @@
       <c r="A40" s="10">
         <v>7</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C40" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>384</v>
+      <c r="C40" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>377</v>
       </c>
       <c r="F40" s="10">
         <v>7</v>
       </c>
-      <c r="G40" s="32" t="s">
+      <c r="G40" s="31" t="s">
         <v>199</v>
       </c>
       <c r="H40" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I40" s="32" t="s">
-        <v>415</v>
+      <c r="I40" s="31" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="10">
         <v>8</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>201</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="F41" s="10">
         <v>8</v>
@@ -6774,14 +7212,14 @@
       <c r="A42" s="10">
         <v>9</v>
       </c>
-      <c r="B42" s="32" t="s">
-        <v>382</v>
-      </c>
-      <c r="C42" s="32" t="s">
+      <c r="B42" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="C42" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="36" t="s">
-        <v>383</v>
+      <c r="D42" s="35" t="s">
+        <v>376</v>
       </c>
       <c r="F42" s="10">
         <v>9</v>
@@ -6800,87 +7238,131 @@
       <c r="A43" s="10">
         <v>10</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="36" t="s">
-        <v>405</v>
+      <c r="D43" s="35" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="10">
         <v>11</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="36" t="s">
-        <v>406</v>
+      <c r="D44" s="35" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="10">
         <v>12</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="31" t="s">
         <v>249</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="D45" s="36" t="s">
-        <v>268</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="F45" s="5">
+        <v>6</v>
+      </c>
+      <c r="G45" s="61" t="s">
+        <v>407</v>
+      </c>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="10">
         <v>13</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D46" s="32" t="s">
-        <v>404</v>
+      <c r="D46" s="31" t="s">
+        <v>419</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="10">
         <v>14</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="33" t="s">
         <v>233</v>
+      </c>
+      <c r="F47" s="10">
+        <v>1</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="25" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="10">
         <v>15</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="35" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="F48" s="10">
+        <v>2</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="10">
         <v>16</v>
       </c>
@@ -6888,37 +7370,927 @@
         <v>250</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D49" s="26" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="F49" s="10">
+        <v>3</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>411</v>
+      </c>
+      <c r="H49" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="I49" s="36" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="10">
         <v>17</v>
       </c>
-      <c r="B50" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="B50" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="F50" s="10">
+        <v>4</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I50" s="36" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="10">
         <v>18</v>
       </c>
       <c r="B51" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="62"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="10">
+        <v>19</v>
+      </c>
+      <c r="B52" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="20" t="s">
+      <c r="C52" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="F53" s="14"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="58"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="5">
+        <v>8</v>
+      </c>
+      <c r="B54" s="61" t="s">
+        <v>421</v>
+      </c>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="F54" s="49">
+        <v>11</v>
+      </c>
+      <c r="G54" s="54" t="s">
+        <v>438</v>
+      </c>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="H55" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" s="52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="10">
+        <v>1</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="F56" s="10">
+        <v>1</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I56" s="25" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="10">
+        <v>2</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="F57" s="10">
+        <v>2</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="10">
+        <v>3</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>425</v>
+      </c>
+      <c r="F58" s="10">
+        <v>3</v>
+      </c>
+      <c r="G58" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="H58" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="I58" s="31" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="10">
+        <v>4</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="F59" s="10">
+        <v>4</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="H59" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="I59" s="31" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="10">
+        <v>5</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="F60" s="10">
+        <v>5</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="H60" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="I60" s="31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="60">
+      <c r="A61" s="10">
+        <v>6</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C61" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="48" t="s">
+        <v>437</v>
+      </c>
+      <c r="F61" s="10">
+        <v>6</v>
+      </c>
+      <c r="G61" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="H61" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="I61" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="30">
+      <c r="A62" s="10">
+        <v>7</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="D62" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="F62" s="10">
+        <v>7</v>
+      </c>
+      <c r="G62" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="I62" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="10">
+        <v>8</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="41" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="10">
+        <v>9</v>
+      </c>
+      <c r="B64" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="41" t="s">
+        <v>432</v>
+      </c>
+      <c r="F64" s="5">
+        <v>7</v>
+      </c>
+      <c r="G64" s="63" t="s">
+        <v>442</v>
+      </c>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="10">
+        <v>10</v>
+      </c>
+      <c r="B65" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="C65" s="40" t="s">
+        <v>267</v>
+      </c>
+      <c r="D65" s="41" t="s">
+        <v>431</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="10">
+        <v>11</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="C66" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="D66" s="41" t="s">
+        <v>431</v>
+      </c>
+      <c r="F66" s="10">
+        <v>1</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I66" s="25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="60">
+      <c r="A67" s="10">
+        <v>12</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="F67" s="10">
+        <v>2</v>
+      </c>
+      <c r="G67" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H67" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I67" s="26" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="10">
+        <v>13</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>303</v>
+      </c>
+      <c r="F68" s="10">
+        <v>3</v>
+      </c>
+      <c r="G68" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I68" s="36" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="30">
+      <c r="A69" s="10">
+        <v>14</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>435</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="D69" s="41" t="s">
+        <v>436</v>
+      </c>
+      <c r="F69" s="10">
+        <v>4</v>
+      </c>
+      <c r="G69" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I69" s="36" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="30">
+      <c r="A70" s="10">
+        <v>15</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F70" s="10">
+        <v>5</v>
+      </c>
+      <c r="G70" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="H70" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I70" s="36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="10">
+        <v>16</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F71" s="10">
+        <v>6</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="H71" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I71" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="F72" s="10">
+        <v>7</v>
+      </c>
+      <c r="G72" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I72" s="31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="5">
+        <v>9</v>
+      </c>
+      <c r="B73" s="64" t="s">
+        <v>455</v>
+      </c>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="F73" s="10">
+        <v>8</v>
+      </c>
+      <c r="G73" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="H73" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I73" s="39" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F74" s="10">
+        <v>9</v>
+      </c>
+      <c r="G74" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="H74" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="I74" s="39" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="10">
+        <v>1</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>457</v>
+      </c>
+      <c r="F75" s="65">
+        <v>10</v>
+      </c>
+      <c r="G75" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="H75" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="I75" s="39" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="10">
+        <v>2</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>458</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="F76" s="10">
+        <v>11</v>
+      </c>
+      <c r="G76" s="35" t="s">
+        <v>449</v>
+      </c>
+      <c r="H76" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="I76" s="41" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="10">
+        <v>3</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D77" s="36"/>
+      <c r="F77" s="10">
+        <v>12</v>
+      </c>
+      <c r="G77" s="68" t="s">
+        <v>450</v>
+      </c>
+      <c r="H77" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="I77" s="68" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="30">
+      <c r="A78" s="10">
+        <v>4</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C78" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D78" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="F78" s="10">
+        <v>13</v>
+      </c>
+      <c r="G78" s="70" t="s">
+        <v>452</v>
+      </c>
+      <c r="H78" s="71" t="s">
+        <v>291</v>
+      </c>
+      <c r="I78" s="70" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="10">
+        <v>5</v>
+      </c>
+      <c r="B79" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D79" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="F79" s="10">
+        <v>14</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H79" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I79" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="10">
+        <v>6</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="D80" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="F80" s="10">
+        <v>15</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I80" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="10">
+        <v>7</v>
+      </c>
+      <c r="B81" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="C81" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D81" s="31" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="10">
+        <v>8</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="10">
+        <v>9</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="5">
+        <v>10</v>
+      </c>
+      <c r="B85" s="64" t="s">
+        <v>460</v>
+      </c>
+      <c r="C85" s="64"/>
+      <c r="D85" s="64"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="10">
+        <v>1</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D87" s="72" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="180">
+      <c r="A88" s="44">
+        <v>2</v>
+      </c>
+      <c r="B88" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C88" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D88" s="46" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="10">
+        <v>3</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C89" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D89" s="36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="10">
+        <v>4</v>
+      </c>
+      <c r="B90" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D90" s="36" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="10">
+        <v>5</v>
+      </c>
+      <c r="B91" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="C91" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D91" s="31" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="10">
+        <v>6</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D92" s="39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="10">
+        <v>7</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="10">
+        <v>8</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D94" s="20" t="s">
         <v>98</v>
       </c>
     </row>
@@ -6950,19 +8322,19 @@
       <c r="A1" s="9">
         <v>13</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>372</v>
-      </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="56" t="s">
+        <v>365</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
       <c r="F1" s="9">
         <v>14</v>
       </c>
-      <c r="G1" s="57" t="s">
-        <v>373</v>
-      </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="G1" s="56" t="s">
+        <v>366</v>
+      </c>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -7001,7 +8373,7 @@
         <v>76</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -7013,33 +8385,33 @@
         <v>76</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="75">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>354</v>
+        <v>291</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>347</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="41" t="s">
-        <v>364</v>
-      </c>
-      <c r="H4" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="41" t="s">
-        <v>365</v>
+      <c r="G4" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7047,13 +8419,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="F5" s="10">
         <v>3</v>
@@ -7065,7 +8437,7 @@
         <v>76</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7073,25 +8445,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="F6" s="10">
         <v>4</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>76</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7099,13 +8471,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>104</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="F7" s="10">
         <v>5</v>
@@ -7117,7 +8489,7 @@
         <v>123</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7125,25 +8497,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="F8" s="10">
         <v>6</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>76</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7151,25 +8523,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="37" t="s">
-        <v>358</v>
+      <c r="D9" s="36" t="s">
+        <v>351</v>
       </c>
       <c r="F9" s="10">
         <v>7</v>
       </c>
-      <c r="G9" s="60" t="s">
-        <v>370</v>
-      </c>
-      <c r="H9" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>374</v>
+      <c r="G9" s="59" t="s">
+        <v>363</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:9">

</xml_diff>

<commit_message>
update revisi sub menu jasa : proses bisnis-pengambilan layanan
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="679">
   <si>
     <t>Revisi2</t>
   </si>
@@ -1672,9 +1672,6 @@
     </r>
   </si>
   <si>
-    <t>0 = transfer bank, 1 = cek, 2 = langsung, 3 = return barang jual</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">p_rek_ukm,  </t>
     </r>
@@ -2506,9 +2503,6 @@
     <t>apa hasilnya</t>
   </si>
   <si>
-    <t>pengecekkan</t>
-  </si>
-  <si>
     <t>tgl_mulai</t>
   </si>
   <si>
@@ -2521,60 +2515,12 @@
     <t>jam_selesai</t>
   </si>
   <si>
-    <t>alur</t>
-  </si>
-  <si>
-    <t>tgl mulai</t>
-  </si>
-  <si>
-    <t>jam mulai</t>
-  </si>
-  <si>
-    <t>what do</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>tgl_end</t>
-  </si>
-  <si>
-    <t>jam end</t>
-  </si>
-  <si>
-    <t>buka pake hirens</t>
-  </si>
-  <si>
-    <t>bad sector</t>
-  </si>
-  <si>
-    <t>tgl_konfirm</t>
-  </si>
-  <si>
-    <t>jam_konfirm</t>
-  </si>
-  <si>
-    <t>respon</t>
-  </si>
-  <si>
-    <t>yes/no</t>
-  </si>
-  <si>
-    <t>yes --&gt; lanjut</t>
-  </si>
-  <si>
-    <t>no --&gt; end</t>
-  </si>
-  <si>
     <t>id_order_jasa</t>
   </si>
   <si>
     <t>FK p_order_jasa</t>
   </si>
   <si>
-    <t>pengerjaan</t>
-  </si>
-  <si>
     <t>now</t>
   </si>
   <si>
@@ -2584,9 +2530,6 @@
     <t>confirm_klien</t>
   </si>
   <si>
-    <t>0 =yes, 1 =no</t>
-  </si>
-  <si>
     <t>respon_klien</t>
   </si>
   <si>
@@ -2596,22 +2539,142 @@
     <t>status_service</t>
   </si>
   <si>
-    <t>status_pb</t>
-  </si>
-  <si>
-    <t>0 = proses bisnis  aktif, 1 = proses bisnis selesai</t>
-  </si>
-  <si>
-    <t>0 = baru masuk, 1 = cancel, 2 = selesai</t>
-  </si>
-  <si>
-    <t>p_cancel</t>
-  </si>
-  <si>
-    <t>0 = baru masuk, 1 = cancel service, 2 = selesai service</t>
-  </si>
-  <si>
-    <t>hapus sj</t>
+    <t>status_selesai</t>
+  </si>
+  <si>
+    <t>status_mulai</t>
+  </si>
+  <si>
+    <t>status_akhir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0 = lanjut service, 1=cancel service, 2= gagal service, 3= berhasil service</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0 = blm selesai, 1 = selesai etape ini, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>default 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0 =no, 1 =yes, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>default 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0 = blm mulai, 1 = mulai di kerjakan,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> default 0</t>
+    </r>
+  </si>
+  <si>
+    <t>status_ambil</t>
+  </si>
+  <si>
+    <t>0 = blm di ambil, 1 = sdh di ambil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 = baru masuk, 1 = sdg di kerjakan, 2 = lanjut service, 3 = cancel service, 4 = gagal service, 5 = berhasil service</t>
+  </si>
+  <si>
+    <t>tgl  bayar, today</t>
+  </si>
+  <si>
+    <t>jumlah bayar</t>
+  </si>
+  <si>
+    <t>jumlah_tagihan</t>
+  </si>
+  <si>
+    <t>jumlah tagihan</t>
+  </si>
+  <si>
+    <t>0 = transfer bank, 1 = cek, 2 = langsung/tunai, 3 = return barang jual</t>
+  </si>
+  <si>
+    <t>0 = transfer bank, 1 = cek, 2 = langsung/tunai,</t>
+  </si>
+  <si>
+    <t>0 = blm lunas, 1 = lunas</t>
+  </si>
+  <si>
+    <t>biaya_tambahan</t>
+  </si>
+  <si>
+    <t>0 = tidak ada biaya tambahan, 1 = ada biaya tambahan</t>
+  </si>
+  <si>
+    <t>ket_biaya</t>
+  </si>
+  <si>
+    <t>keterangan biaya tambahan apa saja</t>
+  </si>
+  <si>
+    <t>p_biaya tambahan</t>
+  </si>
+  <si>
+    <t>PK tabel  biaya tambahan</t>
+  </si>
+  <si>
+    <t>jumlah_biaya</t>
+  </si>
+  <si>
+    <t>nama layanan</t>
+  </si>
+  <si>
+    <t>ambil dari P_jasa.nama_layanan</t>
+  </si>
+  <si>
+    <t>ambil dari P_jasa.biaya</t>
+  </si>
+  <si>
+    <t>0= tunai, 1 = kredit</t>
+  </si>
+  <si>
+    <t>p_bayar_jasa</t>
+  </si>
+  <si>
+    <t>PK tabel  bayar</t>
+  </si>
+  <si>
+    <t>PK tabel  ambil service</t>
+  </si>
+  <si>
+    <t>tgl_ambil</t>
+  </si>
+  <si>
+    <t>id_tagihan</t>
+  </si>
+  <si>
+    <t>p_nota_tagihan</t>
+  </si>
+  <si>
+    <t>FK p_nota_Service</t>
   </si>
 </sst>
 </file>
@@ -2621,7 +2684,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2684,22 +2747,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2750,7 +2799,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2878,7 +2933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3069,9 +3124,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3090,11 +3142,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3910,30 +3970,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="95" t="s">
+      <c r="G2" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -4139,7 +4199,7 @@
         <v>76</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F11" s="14"/>
     </row>
@@ -4159,24 +4219,24 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="95" t="s">
+      <c r="G12" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
         <v>10</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>169</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>71</v>
@@ -4396,21 +4456,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="95" t="s">
+      <c r="G24" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="95" t="s">
-        <v>588</v>
-      </c>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
+      <c r="B25" s="94" t="s">
+        <v>587</v>
+      </c>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -4461,7 +4521,7 @@
         <v>76</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F27" s="10">
         <v>2</v>
@@ -4481,13 +4541,13 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
+        <v>588</v>
+      </c>
+      <c r="C28" t="s">
         <v>589</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>590</v>
-      </c>
-      <c r="D28" t="s">
-        <v>591</v>
       </c>
       <c r="F28" s="10">
         <v>3</v>
@@ -4513,7 +4573,7 @@
         <v>133</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F29" s="10">
         <v>4</v>
@@ -4558,11 +4618,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="95" t="s">
+      <c r="G33" s="94" t="s">
         <v>144</v>
       </c>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -4814,11 +4874,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="95" t="s">
+      <c r="B45" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="95"/>
-      <c r="D45" s="95"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -5123,8 +5183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -6302,7 +6362,7 @@
         <v>286</v>
       </c>
       <c r="I50" s="41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -6318,13 +6378,13 @@
         <v>12</v>
       </c>
       <c r="G51" s="31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H51" s="40" t="s">
         <v>103</v>
       </c>
       <c r="I51" s="41" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -6410,7 +6470,7 @@
         <v>9</v>
       </c>
       <c r="G55" s="64" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H55" s="38"/>
       <c r="I55" s="38"/>
@@ -6772,7 +6832,7 @@
         <v>241</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K73" t="s">
         <v>108</v>
@@ -7103,8 +7163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67:C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -8287,7 +8347,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="54" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H54" s="51"/>
       <c r="I54" s="51"/>
@@ -8341,7 +8401,7 @@
         <v>76</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -8367,7 +8427,7 @@
         <v>76</v>
       </c>
       <c r="I57" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -8459,7 +8519,7 @@
         <v>119</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F61" s="10">
         <v>6</v>
@@ -8485,7 +8545,7 @@
         <v>287</v>
       </c>
       <c r="D62" s="36" t="s">
-        <v>425</v>
+        <v>658</v>
       </c>
       <c r="F62" s="10">
         <v>7</v>
@@ -8511,7 +8571,7 @@
         <v>76</v>
       </c>
       <c r="D63" s="41" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -8525,13 +8585,13 @@
         <v>76</v>
       </c>
       <c r="D64" s="41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F64" s="5">
         <v>7</v>
       </c>
       <c r="G64" s="63" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H64" s="63"/>
       <c r="I64" s="63"/>
@@ -8547,7 +8607,7 @@
         <v>262</v>
       </c>
       <c r="D65" s="41" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>71</v>
@@ -8573,7 +8633,7 @@
         <v>264</v>
       </c>
       <c r="D66" s="41" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F66" s="10">
         <v>1</v>
@@ -8599,7 +8659,7 @@
         <v>122</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F67" s="10">
         <v>2</v>
@@ -8645,13 +8705,13 @@
         <v>14</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C69" s="31" t="s">
         <v>241</v>
       </c>
       <c r="D69" s="41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F69" s="10">
         <v>4</v>
@@ -8663,7 +8723,7 @@
         <v>76</v>
       </c>
       <c r="I69" s="36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="30">
@@ -8737,7 +8797,7 @@
         <v>9</v>
       </c>
       <c r="B73" s="64" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C73" s="64"/>
       <c r="D73" s="64"/>
@@ -8745,13 +8805,13 @@
         <v>8</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H73" s="31" t="s">
         <v>76</v>
       </c>
       <c r="I73" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -8771,13 +8831,13 @@
         <v>9</v>
       </c>
       <c r="G74" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H74" s="31" t="s">
         <v>96</v>
       </c>
       <c r="I74" s="39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -8791,7 +8851,7 @@
         <v>76</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F75" s="65">
         <v>10</v>
@@ -8803,7 +8863,7 @@
         <v>103</v>
       </c>
       <c r="I75" s="39" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -8811,25 +8871,25 @@
         <v>2</v>
       </c>
       <c r="B76" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="26" t="s">
         <v>453</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D76" s="26" t="s">
-        <v>454</v>
       </c>
       <c r="F76" s="10">
         <v>11</v>
       </c>
       <c r="G76" s="35" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H76" s="40" t="s">
         <v>286</v>
       </c>
       <c r="I76" s="41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -8847,13 +8907,13 @@
         <v>12</v>
       </c>
       <c r="G77" s="68" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H77" s="69" t="s">
         <v>103</v>
       </c>
       <c r="I77" s="68" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="30">
@@ -8873,13 +8933,13 @@
         <v>13</v>
       </c>
       <c r="G78" s="70" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H78" s="71" t="s">
         <v>286</v>
       </c>
       <c r="I78" s="70" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -8981,7 +9041,7 @@
         <v>10</v>
       </c>
       <c r="B85" s="64" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C85" s="64"/>
       <c r="D85" s="64"/>
@@ -9011,7 +9071,7 @@
         <v>76</v>
       </c>
       <c r="D87" s="72" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="180">
@@ -9025,7 +9085,7 @@
         <v>241</v>
       </c>
       <c r="D88" s="46" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -9440,21 +9500,21 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="98" t="s">
         <v>490</v>
       </c>
-      <c r="B1" s="99" t="s">
-        <v>491</v>
-      </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
       <c r="F1" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="G1" s="98" t="s">
         <v>508</v>
       </c>
-      <c r="G1" s="99" t="s">
-        <v>509</v>
-      </c>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -9493,7 +9553,7 @@
         <v>76</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -9505,7 +9565,7 @@
         <v>76</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -9513,25 +9573,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>241</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
       </c>
       <c r="G4" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="I4" s="20" t="s">
         <v>512</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -9539,25 +9599,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>241</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F5" s="10">
         <v>3</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>133</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -9565,13 +9625,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -9579,35 +9639,35 @@
         <v>5</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="G7" s="98" t="s">
         <v>516</v>
       </c>
-      <c r="G7" s="99" t="s">
-        <v>517</v>
-      </c>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C8" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>71</v>
@@ -9627,13 +9687,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>502</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>503</v>
       </c>
       <c r="F9" s="10">
         <v>1</v>
@@ -9645,7 +9705,7 @@
         <v>76</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -9653,25 +9713,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="77" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="I10" s="20" t="s">
         <v>512</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -9679,7 +9739,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>103</v>
@@ -9691,13 +9751,13 @@
         <v>3</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H11" s="20" t="s">
         <v>133</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -9705,7 +9765,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>103</v>
@@ -9726,13 +9786,13 @@
         <v>94</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>516</v>
-      </c>
-      <c r="G13" s="99" t="s">
-        <v>520</v>
-      </c>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
+        <v>515</v>
+      </c>
+      <c r="G13" s="98" t="s">
+        <v>519</v>
+      </c>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -9771,7 +9831,7 @@
         <v>76</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -9779,13 +9839,13 @@
         <v>2</v>
       </c>
       <c r="G16" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="I16" s="20" t="s">
         <v>512</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -9793,24 +9853,24 @@
         <v>3</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H17" s="20" t="s">
         <v>133</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="99" t="s">
-        <v>523</v>
-      </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
+      <c r="B18" s="98" t="s">
+        <v>522</v>
+      </c>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -9837,7 +9897,7 @@
         <v>76</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -9845,13 +9905,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="20" t="s">
+        <v>524</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>525</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -9859,13 +9919,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="78" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>96</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30">
@@ -9873,13 +9933,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -9914,19 +9974,19 @@
       <c r="A27" s="79">
         <v>17</v>
       </c>
-      <c r="B27" s="97" t="s">
-        <v>531</v>
-      </c>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
+      <c r="B27" s="96" t="s">
+        <v>530</v>
+      </c>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
       <c r="F27" s="81">
         <v>17</v>
       </c>
-      <c r="G27" s="98" t="s">
-        <v>558</v>
-      </c>
-      <c r="H27" s="98"/>
-      <c r="I27" s="98"/>
+      <c r="G27" s="97" t="s">
+        <v>557</v>
+      </c>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -9965,7 +10025,7 @@
         <v>76</v>
       </c>
       <c r="D29" s="85" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F29" s="10">
         <v>1</v>
@@ -9977,7 +10037,7 @@
         <v>76</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30">
@@ -9985,25 +10045,25 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>367</v>
       </c>
       <c r="D30" s="62" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F30" s="10">
         <v>2</v>
       </c>
       <c r="G30" s="20" t="s">
+        <v>559</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="17" t="s">
         <v>560</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30">
@@ -10011,25 +10071,25 @@
         <v>3</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>535</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>536</v>
       </c>
       <c r="F31" s="10">
         <v>3</v>
       </c>
       <c r="G31" s="82" t="s">
+        <v>561</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>562</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -10037,25 +10097,25 @@
         <v>4</v>
       </c>
       <c r="B32" s="20" t="s">
+        <v>536</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>537</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="D32" s="20" t="s">
         <v>538</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>539</v>
       </c>
       <c r="F32" s="10">
         <v>4</v>
       </c>
       <c r="G32" s="80" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H32" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -10063,19 +10123,19 @@
         <v>5</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C33" s="20" t="s">
+        <v>537</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>538</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>539</v>
       </c>
       <c r="F33" s="10">
         <v>5</v>
       </c>
       <c r="G33" s="83" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
@@ -10085,19 +10145,19 @@
         <v>6</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>540</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="D34" s="17" t="s">
         <v>542</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>543</v>
       </c>
       <c r="F34" s="10">
         <v>6</v>
       </c>
       <c r="G34" s="83" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H34" s="83" t="s">
         <v>76</v>
@@ -10109,7 +10169,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -10118,10 +10178,10 @@
         <v>7</v>
       </c>
       <c r="G35" s="83" t="s">
+        <v>544</v>
+      </c>
+      <c r="H35" s="83" t="s">
         <v>545</v>
-      </c>
-      <c r="H35" s="83" t="s">
-        <v>546</v>
       </c>
       <c r="I35" s="84"/>
     </row>
@@ -10130,10 +10190,10 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
+        <v>544</v>
+      </c>
+      <c r="C36" t="s">
         <v>545</v>
-      </c>
-      <c r="C36" t="s">
-        <v>546</v>
       </c>
       <c r="F36" s="10">
         <v>8</v>
@@ -10192,19 +10252,19 @@
       <c r="A41" s="79">
         <v>17</v>
       </c>
-      <c r="B41" s="97" t="s">
-        <v>547</v>
-      </c>
-      <c r="C41" s="97"/>
-      <c r="D41" s="97"/>
+      <c r="B41" s="96" t="s">
+        <v>546</v>
+      </c>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
       <c r="F41" s="81">
         <v>18</v>
       </c>
-      <c r="G41" s="98" t="s">
-        <v>565</v>
-      </c>
-      <c r="H41" s="98"/>
-      <c r="I41" s="98"/>
+      <c r="G41" s="97" t="s">
+        <v>564</v>
+      </c>
+      <c r="H41" s="97"/>
+      <c r="I41" s="97"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -10243,7 +10303,7 @@
         <v>76</v>
       </c>
       <c r="D43" s="85" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F43" s="10">
         <v>1</v>
@@ -10255,7 +10315,7 @@
         <v>76</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -10263,25 +10323,25 @@
         <v>2</v>
       </c>
       <c r="B44" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" t="s">
         <v>549</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" t="s">
-        <v>550</v>
       </c>
       <c r="F44" s="10">
         <v>2</v>
       </c>
       <c r="G44" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I44" s="17" t="s">
         <v>567</v>
-      </c>
-      <c r="H44" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="45">
@@ -10289,25 +10349,25 @@
         <v>3</v>
       </c>
       <c r="B45" s="80" t="s">
+        <v>550</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>537</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>551</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>538</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>552</v>
       </c>
       <c r="F45" s="10">
         <v>3</v>
       </c>
       <c r="G45" s="82" t="s">
+        <v>568</v>
+      </c>
+      <c r="H45" s="15" t="s">
         <v>569</v>
       </c>
-      <c r="H45" s="15" t="s">
+      <c r="I45" s="15" t="s">
         <v>570</v>
-      </c>
-      <c r="I45" s="15" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -10315,13 +10375,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="80" t="s">
+        <v>552</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="20" t="s">
         <v>553</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>554</v>
       </c>
       <c r="F46" s="10">
         <v>4</v>
@@ -10333,7 +10393,7 @@
         <v>76</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -10341,19 +10401,19 @@
         <v>5</v>
       </c>
       <c r="B47" s="80" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C47" s="86" t="s">
         <v>76</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F47" s="10">
         <v>5</v>
       </c>
       <c r="G47" s="83" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H47" s="83" t="s">
         <v>103</v>
@@ -10365,19 +10425,19 @@
         <v>6</v>
       </c>
       <c r="B48" s="20" t="s">
+        <v>555</v>
+      </c>
+      <c r="C48" s="87" t="s">
+        <v>541</v>
+      </c>
+      <c r="D48" s="20" t="s">
         <v>556</v>
-      </c>
-      <c r="C48" s="87" t="s">
-        <v>542</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>557</v>
       </c>
       <c r="F48" s="10">
         <v>6</v>
       </c>
       <c r="G48" s="83" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H48" s="83" t="s">
         <v>76</v>
@@ -10389,7 +10449,7 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C49" t="s">
         <v>76</v>
@@ -10399,10 +10459,10 @@
         <v>7</v>
       </c>
       <c r="G49" s="83" t="s">
+        <v>544</v>
+      </c>
+      <c r="H49" s="83" t="s">
         <v>545</v>
-      </c>
-      <c r="H49" s="83" t="s">
-        <v>546</v>
       </c>
       <c r="I49" s="84"/>
     </row>
@@ -10411,10 +10471,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
+        <v>544</v>
+      </c>
+      <c r="C50" t="s">
         <v>545</v>
-      </c>
-      <c r="C50" t="s">
-        <v>546</v>
       </c>
       <c r="D50" s="26"/>
       <c r="F50" s="10">
@@ -10453,7 +10513,7 @@
         <v>76</v>
       </c>
       <c r="I51" s="20" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -10474,11 +10534,11 @@
       <c r="A54" s="73">
         <v>2</v>
       </c>
-      <c r="B54" s="99" t="s">
-        <v>459</v>
-      </c>
-      <c r="C54" s="99"/>
-      <c r="D54" s="99"/>
+      <c r="B54" s="98" t="s">
+        <v>458</v>
+      </c>
+      <c r="C54" s="98"/>
+      <c r="D54" s="98"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -10505,7 +10565,7 @@
         <v>241</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -10513,13 +10573,13 @@
         <v>2</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>367</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -10527,7 +10587,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>103</v>
@@ -10539,13 +10599,13 @@
         <v>4</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>241</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30">
@@ -10553,13 +10613,13 @@
         <v>5</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>241</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G60" t="s">
         <v>108</v>
@@ -10573,13 +10633,13 @@
         <v>6</v>
       </c>
       <c r="B61" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>468</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="45">
@@ -10587,13 +10647,13 @@
         <v>7</v>
       </c>
       <c r="B62" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="C62" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="D62" s="17" t="s">
         <v>471</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -10601,13 +10661,13 @@
         <v>8</v>
       </c>
       <c r="B63" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="D63" s="20" t="s">
         <v>473</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -10615,13 +10675,13 @@
         <v>9</v>
       </c>
       <c r="B64" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="D64" s="20" t="s">
         <v>475</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -10629,13 +10689,13 @@
         <v>10</v>
       </c>
       <c r="B65" s="20" t="s">
+        <v>476</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="D65" s="20" t="s">
         <v>477</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -10643,13 +10703,13 @@
         <v>11</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C66" s="20" t="s">
         <v>169</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30">
@@ -10657,13 +10717,13 @@
         <v>12</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C67" s="20" t="s">
         <v>96</v>
       </c>
       <c r="D67" s="36" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30">
@@ -10671,13 +10731,13 @@
         <v>13</v>
       </c>
       <c r="B68" s="35" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C68" s="75" t="s">
         <v>96</v>
       </c>
       <c r="D68" s="76" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -10685,13 +10745,13 @@
         <v>14</v>
       </c>
       <c r="B69" s="75" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C69" s="75" t="s">
         <v>96</v>
       </c>
       <c r="D69" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -10699,13 +10759,13 @@
         <v>14</v>
       </c>
       <c r="B70" s="75" t="s">
+        <v>611</v>
+      </c>
+      <c r="C70" s="75" t="s">
         <v>612</v>
       </c>
-      <c r="C70" s="75" t="s">
-        <v>613</v>
-      </c>
       <c r="D70" s="35" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -10713,13 +10773,13 @@
         <v>15</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C71" s="20" t="s">
         <v>169</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -10727,24 +10787,24 @@
         <v>16</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C72" s="20" t="s">
         <v>96</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="B73" s="74" t="s">
+        <v>485</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="20" t="s">
         <v>486</v>
-      </c>
-      <c r="C73" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -10766,17 +10826,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
@@ -10790,19 +10850,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="95" t="s">
-        <v>575</v>
-      </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
+      <c r="B1" s="94" t="s">
+        <v>574</v>
+      </c>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="99" t="s">
-        <v>623</v>
-      </c>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
+      <c r="G1" s="98" t="s">
+        <v>622</v>
+      </c>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -10841,7 +10901,7 @@
         <v>76</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -10853,7 +10913,7 @@
         <v>76</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
@@ -10861,25 +10921,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>96</v>
       </c>
       <c r="D4" s="89" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>103</v>
       </c>
       <c r="I4" s="89" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -10887,13 +10947,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>595</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>596</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>597</v>
       </c>
       <c r="F5" s="10">
         <v>3</v>
@@ -10919,7 +10979,7 @@
         <v>76</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F6" s="10">
         <v>4</v>
@@ -10939,13 +10999,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -10953,13 +11013,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
+        <v>593</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>594</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -10967,35 +11027,35 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>127</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="95" t="s">
-        <v>604</v>
-      </c>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
+      <c r="G9" s="94" t="s">
+        <v>603</v>
+      </c>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>583</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>576</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>584</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>577</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>585</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>71</v>
@@ -11021,7 +11081,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F11" s="10">
         <v>1</v>
@@ -11033,7 +11093,7 @@
         <v>76</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -11059,7 +11119,7 @@
         <v>119</v>
       </c>
       <c r="I12" s="89" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -11085,7 +11145,7 @@
         <v>76</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -11099,18 +11159,18 @@
         <v>76</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="95" t="s">
-        <v>600</v>
-      </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
+      <c r="B15" s="94" t="s">
+        <v>599</v>
+      </c>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -11121,7 +11181,7 @@
         <v>76</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -11141,13 +11201,13 @@
         <v>6</v>
       </c>
       <c r="G16" s="26" t="s">
+        <v>609</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="90" t="s">
         <v>610</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="90" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -11161,19 +11221,19 @@
         <v>76</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F17" s="10">
         <v>7</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H17" s="30" t="s">
         <v>103</v>
       </c>
       <c r="I17" s="70" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -11181,13 +11241,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>96</v>
       </c>
       <c r="D18" s="89" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F18" s="10">
         <v>8</v>
@@ -11199,10 +11259,10 @@
         <v>103</v>
       </c>
       <c r="I18" s="91" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45">
       <c r="A19" s="10">
         <v>3</v>
       </c>
@@ -11215,17 +11275,17 @@
       <c r="D19" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="65">
         <v>9</v>
       </c>
-      <c r="G19" s="30" t="s">
-        <v>662</v>
-      </c>
-      <c r="H19" s="30" t="s">
+      <c r="G19" s="31" t="s">
+        <v>643</v>
+      </c>
+      <c r="H19" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="I19" s="70" t="s">
-        <v>667</v>
+      <c r="I19" s="41" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -11244,14 +11304,14 @@
       <c r="F20" s="10">
         <v>10</v>
       </c>
-      <c r="G20" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>94</v>
+      <c r="G20" s="30" t="s">
+        <v>651</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="I20" s="70" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -11271,38 +11331,40 @@
         <v>11</v>
       </c>
       <c r="G21" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="F22" s="65"/>
+      <c r="G22" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="20" t="s">
+      <c r="H22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="20" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="95" t="s">
-        <v>625</v>
-      </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
+      <c r="B23" s="94" t="s">
+        <v>624</v>
+      </c>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
       <c r="F23" s="92"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="100"/>
-      <c r="I23" s="100"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -11317,17 +11379,15 @@
       <c r="D24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="5">
-        <v>3</v>
-      </c>
-      <c r="G24" s="95" t="s">
-        <v>666</v>
-      </c>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="94" t="s">
+        <v>677</v>
+      </c>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="10">
+      <c r="A25" s="101">
         <v>1</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -11337,441 +11397,606 @@
         <v>76</v>
       </c>
       <c r="D25" s="25" t="s">
+        <v>625</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="101">
+        <v>2</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>636</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>637</v>
+      </c>
+      <c r="F26" s="10">
+        <v>2</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>636</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="101">
+        <v>3</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>626</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="10">
-        <v>2</v>
-      </c>
-      <c r="B26" s="57" t="s">
-        <v>653</v>
-      </c>
-      <c r="C26" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>654</v>
-      </c>
-      <c r="F26" s="10">
-        <v>1</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="10">
+      <c r="C27" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="89" t="s">
+        <v>627</v>
+      </c>
+      <c r="F27" s="10">
         <v>3</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>627</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="89" t="s">
+      <c r="G27" s="40" t="s">
+        <v>675</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" s="40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="101">
+        <v>4</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>632</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="F28" s="10">
+        <v>4</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>656</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" s="89" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="101">
+        <v>5</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>633</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="F29" s="10">
+        <v>5</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>589</v>
+      </c>
+      <c r="I29" s="39" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="101">
+        <v>6</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>645</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>650</v>
+      </c>
+      <c r="F30" s="65">
+        <v>6</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>589</v>
+      </c>
+      <c r="I30" s="41" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="102">
+        <v>7</v>
+      </c>
+      <c r="B31" s="31" t="s">
         <v>628</v>
-      </c>
-      <c r="F27" s="10">
-        <v>2</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="I27" s="89" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30">
-      <c r="A28" s="103" t="s">
-        <v>668</v>
-      </c>
-      <c r="B28" s="101" t="s">
-        <v>663</v>
-      </c>
-      <c r="C28" s="101" t="s">
-        <v>286</v>
-      </c>
-      <c r="D28" s="102" t="s">
-        <v>664</v>
-      </c>
-      <c r="F28" s="10">
-        <v>3</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="26" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="94">
-        <v>5</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>634</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>656</v>
-      </c>
-      <c r="F29" s="10">
-        <v>4</v>
-      </c>
-      <c r="G29" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" s="26" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="94">
-        <v>6</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>635</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>657</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>656</v>
-      </c>
-      <c r="F30" s="10">
-        <v>5</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I30" s="26" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="94">
-        <v>7</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>629</v>
       </c>
       <c r="C31" s="31" t="s">
         <v>103</v>
       </c>
       <c r="D31" s="26" t="s">
+        <v>629</v>
+      </c>
+      <c r="E31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="10">
+        <v>7</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="102">
+        <v>8</v>
+      </c>
+      <c r="B32" s="31" t="s">
         <v>630</v>
-      </c>
-      <c r="F31" s="10">
-        <v>6</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>610</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I31" s="90" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="94">
-        <v>8</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>631</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>103</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F32" s="10">
-        <v>7</v>
-      </c>
-      <c r="G32" s="30" t="s">
-        <v>616</v>
-      </c>
-      <c r="H32" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="70" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="94">
+        <v>8</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="102">
         <v>9</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>119</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>656</v>
-      </c>
-      <c r="F33" s="10">
+        <v>638</v>
+      </c>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="102">
+        <v>10</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="94" t="s">
+        <v>665</v>
+      </c>
+      <c r="H34" s="94"/>
+      <c r="I34" s="94"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="102">
+        <v>11</v>
+      </c>
+      <c r="B35" s="90" t="s">
+        <v>644</v>
+      </c>
+      <c r="C35" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="90" t="s">
+        <v>648</v>
+      </c>
+      <c r="F35" s="10">
+        <v>1</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="103">
+        <v>12</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>640</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>649</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="10">
+        <v>2</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>676</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="103">
+        <v>13</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>641</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>642</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="10">
+        <v>3</v>
+      </c>
+      <c r="G37" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="H37" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30">
+      <c r="A38" s="103">
+        <v>14</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>646</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>589</v>
+      </c>
+      <c r="D38" s="100" t="s">
+        <v>647</v>
+      </c>
+      <c r="F38" s="10">
+        <v>4</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>667</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="10">
+        <v>15</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>661</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>589</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>662</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="104">
+        <v>16</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>663</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>664</v>
+      </c>
+      <c r="G40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="104">
+        <v>17</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="104">
+        <v>18</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" s="92"/>
+      <c r="J42" s="92"/>
+      <c r="K42" s="92"/>
+      <c r="L42" s="92"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="14"/>
+      <c r="B43" s="27"/>
+      <c r="J43" s="93"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="5"/>
+      <c r="B44" s="94" t="s">
+        <v>672</v>
+      </c>
+      <c r="C44" s="94"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="27"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="10">
+        <v>1</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>673</v>
+      </c>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="10">
+        <v>2</v>
+      </c>
+      <c r="B46" s="58" t="s">
+        <v>676</v>
+      </c>
+      <c r="C46" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" t="s">
+        <v>678</v>
+      </c>
+      <c r="E46" t="s">
+        <v>108</v>
+      </c>
+      <c r="G46" t="s">
+        <v>108</v>
+      </c>
+      <c r="H46" t="s">
+        <v>108</v>
+      </c>
+      <c r="I46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="10">
+        <v>3</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="89" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="10">
+        <v>4</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="10">
+        <v>5</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="D49" s="36" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="10">
+        <v>6</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="10">
+        <v>7</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="41" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="10">
         <v>8</v>
       </c>
-      <c r="G33" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="H33" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="91" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="94">
+      <c r="B52" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="10">
+        <v>9</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="10">
         <v>10</v>
       </c>
-      <c r="B34" s="31" t="s">
-        <v>637</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>657</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>656</v>
-      </c>
-      <c r="F34" s="10">
-        <v>9</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>662</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="I34" s="70" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="94">
+      <c r="B54" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="10">
         <v>11</v>
       </c>
-      <c r="B35" s="31" t="s">
-        <v>658</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>659</v>
-      </c>
-      <c r="F35" s="10">
-        <v>10</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="94">
-        <v>12</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>660</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>661</v>
-      </c>
-      <c r="F36" s="10">
-        <v>11</v>
-      </c>
-      <c r="G36" s="20" t="s">
+      <c r="B55" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H36" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="20" t="s">
+      <c r="C55" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="94">
-        <v>13</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="94">
-        <v>14</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="14"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="14"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" t="s">
-        <v>230</v>
-      </c>
-      <c r="B42" s="92" t="s">
-        <v>638</v>
-      </c>
-      <c r="C42" s="92" t="s">
-        <v>639</v>
-      </c>
-      <c r="D42" s="92" t="s">
-        <v>640</v>
-      </c>
-      <c r="E42" s="92" t="s">
-        <v>641</v>
-      </c>
-      <c r="G42" s="92" t="s">
-        <v>642</v>
-      </c>
-      <c r="H42" s="92" t="s">
-        <v>643</v>
-      </c>
-      <c r="I42" s="92" t="s">
-        <v>644</v>
-      </c>
-      <c r="J42" s="92" t="s">
-        <v>647</v>
-      </c>
-      <c r="K42" s="92" t="s">
-        <v>648</v>
-      </c>
-      <c r="L42" s="92" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>633</v>
-      </c>
-      <c r="C43" s="93">
-        <v>43863</v>
-      </c>
-      <c r="D43">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E43" t="s">
-        <v>645</v>
-      </c>
-      <c r="G43" t="s">
-        <v>646</v>
-      </c>
-      <c r="H43" s="93">
-        <v>43863</v>
-      </c>
-      <c r="I43">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J43" s="93">
-        <v>43863</v>
-      </c>
-      <c r="K43">
-        <v>6.4</v>
-      </c>
-      <c r="L43" t="s">
-        <v>650</v>
-      </c>
-      <c r="M43" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>655</v>
-      </c>
-      <c r="C44" s="93">
-        <v>43863</v>
-      </c>
-      <c r="M44" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="D45" t="s">
+    <row r="57" spans="1:5">
+      <c r="E57" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="G24:I24"/>

</xml_diff>

<commit_message>
update sub menu jasa : pembayaran & jurnal umum otomatis pembayaran jasa
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="685">
   <si>
     <t>Revisi2</t>
   </si>
@@ -2665,9 +2665,6 @@
     <t>PK tabel  ambil service</t>
   </si>
   <si>
-    <t>tgl_ambil</t>
-  </si>
-  <si>
     <t>id_tagihan</t>
   </si>
   <si>
@@ -2675,6 +2672,27 @@
   </si>
   <si>
     <t>FK p_nota_Service</t>
+  </si>
+  <si>
+    <t>no_invoice</t>
+  </si>
+  <si>
+    <t>no tagihan</t>
+  </si>
+  <si>
+    <t>jenis_sk</t>
+  </si>
+  <si>
+    <t>0 = sk di nota order, 1 = sk di nota tagihan</t>
+  </si>
+  <si>
+    <t>p_akun_jasa</t>
+  </si>
+  <si>
+    <t>PK tabel seting akun sub menu jasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = pembayaran jasa tunai, 1 = pembayaran jasa kredit. </t>
   </si>
 </sst>
 </file>
@@ -2933,7 +2951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3127,6 +3145,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3142,19 +3178,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3970,30 +4000,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -4219,11 +4249,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="94" t="s">
+      <c r="G12" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="94"/>
-      <c r="I12" s="94"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -4456,21 +4486,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="94" t="s">
+      <c r="G24" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="100" t="s">
         <v>587</v>
       </c>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -4618,11 +4648,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="94" t="s">
+      <c r="G33" s="100" t="s">
         <v>144</v>
       </c>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -4874,11 +4904,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="94"/>
-      <c r="D45" s="94"/>
+      <c r="C45" s="100"/>
+      <c r="D45" s="100"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -7163,8 +7193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:C67"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -9064,10 +9094,10 @@
       <c r="A87" s="10">
         <v>1</v>
       </c>
-      <c r="B87" s="20" t="s">
+      <c r="B87" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="107" t="s">
         <v>76</v>
       </c>
       <c r="D87" s="72" t="s">
@@ -9078,10 +9108,10 @@
       <c r="A88" s="44">
         <v>2</v>
       </c>
-      <c r="B88" s="45" t="s">
+      <c r="B88" s="44" t="s">
         <v>294</v>
       </c>
-      <c r="C88" s="45" t="s">
+      <c r="C88" s="44" t="s">
         <v>241</v>
       </c>
       <c r="D88" s="46" t="s">
@@ -9092,10 +9122,10 @@
       <c r="A89" s="10">
         <v>3</v>
       </c>
-      <c r="B89" s="26" t="s">
+      <c r="B89" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="C89" s="26" t="s">
+      <c r="C89" s="10" t="s">
         <v>76</v>
       </c>
       <c r="D89" s="36" t="s">
@@ -9106,10 +9136,10 @@
       <c r="A90" s="10">
         <v>4</v>
       </c>
-      <c r="B90" s="26" t="s">
+      <c r="B90" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="C90" s="26" t="s">
+      <c r="C90" s="10" t="s">
         <v>286</v>
       </c>
       <c r="D90" s="36" t="s">
@@ -9120,10 +9150,10 @@
       <c r="A91" s="10">
         <v>5</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="99" t="s">
         <v>288</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="C91" s="10" t="s">
         <v>290</v>
       </c>
       <c r="D91" s="31" t="s">
@@ -9134,10 +9164,10 @@
       <c r="A92" s="10">
         <v>6</v>
       </c>
-      <c r="B92" s="30" t="s">
+      <c r="B92" s="108" t="s">
         <v>289</v>
       </c>
-      <c r="C92" s="26" t="s">
+      <c r="C92" s="10" t="s">
         <v>286</v>
       </c>
       <c r="D92" s="39" t="s">
@@ -9148,10 +9178,10 @@
       <c r="A93" s="10">
         <v>7</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B93" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="107" t="s">
         <v>76</v>
       </c>
       <c r="D93" s="26" t="s">
@@ -9162,10 +9192,10 @@
       <c r="A94" s="10">
         <v>8</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B94" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="107" t="s">
         <v>76</v>
       </c>
       <c r="D94" s="20" t="s">
@@ -9502,19 +9532,19 @@
       <c r="A1" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="104" t="s">
         <v>490</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
       <c r="F1" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="G1" s="98" t="s">
+      <c r="G1" s="104" t="s">
         <v>508</v>
       </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -9650,11 +9680,11 @@
       <c r="F7" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G7" s="98" t="s">
+      <c r="G7" s="104" t="s">
         <v>516</v>
       </c>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="104"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -9788,11 +9818,11 @@
       <c r="F13" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G13" s="98" t="s">
+      <c r="G13" s="104" t="s">
         <v>519</v>
       </c>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -9866,11 +9896,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="104" t="s">
         <v>522</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -9974,19 +10004,19 @@
       <c r="A27" s="79">
         <v>17</v>
       </c>
-      <c r="B27" s="96" t="s">
+      <c r="B27" s="102" t="s">
         <v>530</v>
       </c>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="102"/>
       <c r="F27" s="81">
         <v>17</v>
       </c>
-      <c r="G27" s="97" t="s">
+      <c r="G27" s="103" t="s">
         <v>557</v>
       </c>
-      <c r="H27" s="97"/>
-      <c r="I27" s="97"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -10252,19 +10282,19 @@
       <c r="A41" s="79">
         <v>17</v>
       </c>
-      <c r="B41" s="96" t="s">
+      <c r="B41" s="102" t="s">
         <v>546</v>
       </c>
-      <c r="C41" s="96"/>
-      <c r="D41" s="96"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="102"/>
       <c r="F41" s="81">
         <v>18</v>
       </c>
-      <c r="G41" s="97" t="s">
+      <c r="G41" s="103" t="s">
         <v>564</v>
       </c>
-      <c r="H41" s="97"/>
-      <c r="I41" s="97"/>
+      <c r="H41" s="103"/>
+      <c r="I41" s="103"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -10534,11 +10564,11 @@
       <c r="A54" s="73">
         <v>2</v>
       </c>
-      <c r="B54" s="98" t="s">
+      <c r="B54" s="104" t="s">
         <v>458</v>
       </c>
-      <c r="C54" s="98"/>
-      <c r="D54" s="98"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="104"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -10828,8 +10858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10850,19 +10880,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="100" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="98" t="s">
+      <c r="G1" s="104" t="s">
         <v>622</v>
       </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -10903,13 +10933,13 @@
       <c r="D3" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="44">
         <v>1</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="12" t="s">
         <v>76</v>
       </c>
       <c r="I3" s="25" t="s">
@@ -10929,17 +10959,17 @@
       <c r="D4" s="89" t="s">
         <v>582</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="106">
         <v>2</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>621</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4" s="89" t="s">
-        <v>623</v>
+      <c r="G4" s="25" t="s">
+        <v>680</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -10955,17 +10985,17 @@
       <c r="D5" s="26" t="s">
         <v>596</v>
       </c>
-      <c r="F5" s="10">
-        <v>3</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>94</v>
+      <c r="F5" s="44">
+        <v>2</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>621</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="89" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -10981,17 +11011,17 @@
       <c r="D6" s="26" t="s">
         <v>592</v>
       </c>
-      <c r="F6" s="10">
-        <v>4</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>98</v>
+      <c r="F6" s="44">
+        <v>3</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -11007,6 +11037,18 @@
       <c r="D7" s="26" t="s">
         <v>586</v>
       </c>
+      <c r="F7" s="44">
+        <v>4</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -11038,11 +11080,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="100" t="s">
         <v>603</v>
       </c>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="100"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -11166,11 +11208,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="100" t="s">
         <v>599</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -11341,7 +11383,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="F22" s="65"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="20" t="s">
         <v>97</v>
       </c>
@@ -11356,15 +11398,15 @@
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="100" t="s">
         <v>624</v>
       </c>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
       <c r="F23" s="92"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="99"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -11380,14 +11422,14 @@
         <v>74</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="94" t="s">
-        <v>677</v>
-      </c>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
+      <c r="G24" s="100" t="s">
+        <v>676</v>
+      </c>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="101">
+      <c r="A25" s="96">
         <v>1</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -11413,7 +11455,7 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="101">
+      <c r="A26" s="96">
         <v>2</v>
       </c>
       <c r="B26" s="57" t="s">
@@ -11439,7 +11481,7 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="101">
+      <c r="A27" s="96">
         <v>3</v>
       </c>
       <c r="B27" s="26" t="s">
@@ -11454,18 +11496,18 @@
       <c r="F27" s="10">
         <v>3</v>
       </c>
-      <c r="G27" s="40" t="s">
-        <v>675</v>
-      </c>
-      <c r="H27" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="I27" s="40" t="s">
-        <v>120</v>
+      <c r="G27" s="34" t="s">
+        <v>678</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="101">
+      <c r="A28" s="96">
         <v>4</v>
       </c>
       <c r="B28" s="31" t="s">
@@ -11491,7 +11533,7 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="101">
+      <c r="A29" s="96">
         <v>5</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -11517,7 +11559,7 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="101">
+      <c r="A30" s="96">
         <v>6</v>
       </c>
       <c r="B30" s="26" t="s">
@@ -11543,7 +11585,7 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="102">
+      <c r="A31" s="97">
         <v>7</v>
       </c>
       <c r="B31" s="31" t="s">
@@ -11572,7 +11614,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="102">
+      <c r="A32" s="97">
         <v>8</v>
       </c>
       <c r="B32" s="31" t="s">
@@ -11598,7 +11640,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="102">
+      <c r="A33" s="97">
         <v>9</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -11613,7 +11655,7 @@
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="102">
+      <c r="A34" s="97">
         <v>10</v>
       </c>
       <c r="B34" s="31" t="s">
@@ -11626,14 +11668,14 @@
         <v>638</v>
       </c>
       <c r="F34" s="5"/>
-      <c r="G34" s="94" t="s">
+      <c r="G34" s="100" t="s">
         <v>665</v>
       </c>
-      <c r="H34" s="94"/>
-      <c r="I34" s="94"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="100"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="102">
+      <c r="A35" s="97">
         <v>11</v>
       </c>
       <c r="B35" s="90" t="s">
@@ -11659,7 +11701,7 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="103">
+      <c r="A36" s="98">
         <v>12</v>
       </c>
       <c r="B36" s="31" t="s">
@@ -11676,17 +11718,17 @@
         <v>2</v>
       </c>
       <c r="G36" s="31" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H36" s="31" t="s">
         <v>76</v>
       </c>
       <c r="I36" s="26" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="103">
+      <c r="A37" s="98">
         <v>13</v>
       </c>
       <c r="B37" s="31" t="s">
@@ -11713,7 +11755,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="30">
-      <c r="A38" s="103">
+      <c r="A38" s="98">
         <v>14</v>
       </c>
       <c r="B38" s="30" t="s">
@@ -11722,7 +11764,7 @@
       <c r="C38" s="30" t="s">
         <v>589</v>
       </c>
-      <c r="D38" s="100" t="s">
+      <c r="D38" s="95" t="s">
         <v>647</v>
       </c>
       <c r="F38" s="10">
@@ -11757,7 +11799,7 @@
       <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="104">
+      <c r="A40" s="99">
         <v>16</v>
       </c>
       <c r="B40" s="31" t="s">
@@ -11769,12 +11811,15 @@
       <c r="D40" s="31" t="s">
         <v>664</v>
       </c>
-      <c r="G40" t="s">
-        <v>108</v>
-      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="100" t="s">
+        <v>672</v>
+      </c>
+      <c r="H40" s="100"/>
+      <c r="I40" s="100"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="104">
+      <c r="A41" s="99">
         <v>17</v>
       </c>
       <c r="B41" s="20" t="s">
@@ -11786,9 +11831,21 @@
       <c r="D41" s="20" t="s">
         <v>94</v>
       </c>
+      <c r="F41" s="10">
+        <v>1</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="25" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="104">
+      <c r="A42" s="99">
         <v>18</v>
       </c>
       <c r="B42" s="20" t="s">
@@ -11801,6 +11858,18 @@
         <v>98</v>
       </c>
       <c r="E42" s="92"/>
+      <c r="F42" s="10">
+        <v>2</v>
+      </c>
+      <c r="G42" s="58" t="s">
+        <v>675</v>
+      </c>
+      <c r="H42" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" t="s">
+        <v>677</v>
+      </c>
       <c r="J42" s="92"/>
       <c r="K42" s="92"/>
       <c r="L42" s="92"/>
@@ -11808,202 +11877,273 @@
     <row r="43" spans="1:12">
       <c r="A43" s="14"/>
       <c r="B43" s="27"/>
+      <c r="F43" s="10">
+        <v>3</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" s="89" t="s">
+        <v>654</v>
+      </c>
       <c r="J43" s="93"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="5"/>
+      <c r="A44" s="5">
+        <v>10</v>
+      </c>
       <c r="B44" s="94" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="C44" s="94"/>
       <c r="D44" s="94"/>
       <c r="E44" s="27"/>
+      <c r="F44" s="10">
+        <v>4</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="H44" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I44" s="41" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="10">
-        <v>1</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>673</v>
+      <c r="A45" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
+      <c r="F45" s="10">
+        <v>5</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="H45" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="I45" s="36" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="10">
-        <v>2</v>
-      </c>
-      <c r="B46" s="58" t="s">
-        <v>676</v>
-      </c>
-      <c r="C46" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" t="s">
-        <v>678</v>
+        <v>1</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="72" t="s">
+        <v>683</v>
       </c>
       <c r="E46" t="s">
         <v>108</v>
       </c>
-      <c r="G46" t="s">
-        <v>108</v>
-      </c>
-      <c r="H46" t="s">
-        <v>108</v>
-      </c>
-      <c r="I46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="10">
-        <v>3</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="89" t="s">
-        <v>654</v>
+      <c r="F46" s="10">
+        <v>6</v>
+      </c>
+      <c r="G46" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" s="41" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30">
+      <c r="A47" s="44">
+        <v>2</v>
+      </c>
+      <c r="B47" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="D47" s="46" t="s">
+        <v>684</v>
+      </c>
+      <c r="F47" s="10">
+        <v>7</v>
+      </c>
+      <c r="G47" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="H47" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="41" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="10">
+        <v>3</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="F48" s="10">
+        <v>8</v>
+      </c>
+      <c r="G48" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="H48" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="I48" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="10">
         <v>4</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="41" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="10">
+      <c r="B49" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="D49" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="F49" s="10">
+        <v>9</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="H49" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="I49" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="10">
         <v>5</v>
       </c>
-      <c r="B49" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="D49" s="36" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="10">
+      <c r="B50" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="D50" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="F50" s="10">
+        <v>10</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I50" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="10">
         <v>6</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>265</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" s="41" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="10">
+      <c r="B51" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="D51" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="F51" s="10">
+        <v>11</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I51" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="10">
         <v>7</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="41" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="10">
+      <c r="B52" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="10">
         <v>8</v>
       </c>
-      <c r="B52" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>262</v>
-      </c>
-      <c r="D52" s="41" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="10">
-        <v>9</v>
-      </c>
-      <c r="B53" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="C53" s="40" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="41" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="10">
-        <v>10</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="10">
-        <v>11</v>
-      </c>
-      <c r="B55" s="20" t="s">
+      <c r="B53" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="20" t="s">
+      <c r="C53" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:9">
       <c r="E57" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G24:I24"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update revisi jasa & tambah revisi manufaktur
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="722">
   <si>
     <t>Revisi2</t>
   </si>
@@ -2548,9 +2548,6 @@
     <t>status_akhir</t>
   </si>
   <si>
-    <t xml:space="preserve">  0 = lanjut service, 1=cancel service, 2= gagal service, 3= berhasil service</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">0 = blm selesai, 1 = selesai etape ini, </t>
     </r>
@@ -2599,9 +2596,6 @@
     <t>0 = blm di ambil, 1 = sdh di ambil</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0 = baru masuk, 1 = sdg di kerjakan, 2 = lanjut service, 3 = cancel service, 4 = gagal service, 5 = berhasil service</t>
-  </si>
-  <si>
     <t>tgl  bayar, today</t>
   </si>
   <si>
@@ -2611,9 +2605,6 @@
     <t>jumlah_tagihan</t>
   </si>
   <si>
-    <t>jumlah tagihan</t>
-  </si>
-  <si>
     <t>0 = transfer bank, 1 = cek, 2 = langsung/tunai, 3 = return barang jual</t>
   </si>
   <si>
@@ -2693,6 +2684,150 @@
   </si>
   <si>
     <t xml:space="preserve">0 = pembayaran jasa tunai, 1 = pembayaran jasa kredit. </t>
+  </si>
+  <si>
+    <t>status_konfirm</t>
+  </si>
+  <si>
+    <t>0 = blm konfirm ke klien, 1 = sdh konfirm ke klien</t>
+  </si>
+  <si>
+    <t>tgl_konfirm</t>
+  </si>
+  <si>
+    <t>jam_konfirm</t>
+  </si>
+  <si>
+    <t>tgl  konfirm</t>
+  </si>
+  <si>
+    <t>jam konfirm</t>
+  </si>
+  <si>
+    <t>p_qc</t>
+  </si>
+  <si>
+    <t>PK tabel quality control</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>p_item_qc</t>
+  </si>
+  <si>
+    <t>PK tabel item qc</t>
+  </si>
+  <si>
+    <t>nama_item</t>
+  </si>
+  <si>
+    <t>nama item</t>
+  </si>
+  <si>
+    <t>id_item_qc</t>
+  </si>
+  <si>
+    <t>FK p_item_qc</t>
+  </si>
+  <si>
+    <t>hasil_qc</t>
+  </si>
+  <si>
+    <t>0 = bug, 1 = no bug</t>
+  </si>
+  <si>
+    <t>hasilnya</t>
+  </si>
+  <si>
+    <t>jika ada bug tuliskan di sini bugnya apa</t>
+  </si>
+  <si>
+    <t>p_klaim_garansi</t>
+  </si>
+  <si>
+    <r>
+      <t>besarnya diskon jika ada,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> nullable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dp biaya service,  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  0 = lanjut service, 1=cancel service, 2= gagal service, 3= berhasil service,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 = baru masuk, 1 = sdg di kerjakan, 2 = lanjut service, 3 = cancel service, 4 = gagal service, 5 = berhasil service, 6 = selesai quality control, 7 = perbaikan ulang, 8 = perbaikan garansi</t>
+  </si>
+  <si>
+    <t>jumlah tagihan / total akhir</t>
+  </si>
+  <si>
+    <t>PK tabel claim garansi</t>
+  </si>
+  <si>
+    <t>FK tabel p_nota_Tagihan</t>
+  </si>
+  <si>
+    <t>Keluhan</t>
+  </si>
+  <si>
+    <t>apa yg di klaim</t>
+  </si>
+  <si>
+    <t>status_claim</t>
+  </si>
+  <si>
+    <t>0 = diterima, 1 = di tolak</t>
+  </si>
+  <si>
+    <t>alasan_terima_tolak</t>
+  </si>
+  <si>
+    <t>alasan nya apa di terima/ditolak</t>
+  </si>
+  <si>
+    <t>konfirm_client</t>
+  </si>
+  <si>
+    <t>0 = blm konfirm, 1 =  sdh konfigrm</t>
+  </si>
+  <si>
+    <t>noted: tambahkan shift penjualan.</t>
+  </si>
+  <si>
+    <t>setiap shift penjualan tercatatat:</t>
+  </si>
+  <si>
+    <t>berapa kas yg dipegang ketika memulai shift</t>
+  </si>
+  <si>
+    <t>berapa pengeluaran ketika menjalankan shift</t>
+  </si>
+  <si>
+    <t>berapa saldo kas akhir ketika selseai shift</t>
   </si>
 </sst>
 </file>
@@ -2951,7 +3086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3163,6 +3298,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3175,18 +3322,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3983,7 +4120,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -4000,30 +4137,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -4249,11 +4386,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="100" t="s">
+      <c r="G12" s="104" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
+      <c r="H12" s="104"/>
+      <c r="I12" s="104"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -4486,21 +4623,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="100" t="s">
+      <c r="G24" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="100"/>
-      <c r="I24" s="100"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="104" t="s">
         <v>587</v>
       </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="104"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -4648,11 +4785,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="100" t="s">
+      <c r="G33" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="H33" s="100"/>
-      <c r="I33" s="100"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -4904,11 +5041,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="100" t="s">
+      <c r="B45" s="104" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="100"/>
-      <c r="D45" s="100"/>
+      <c r="C45" s="104"/>
+      <c r="D45" s="104"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -7191,10 +7328,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="B90" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -8575,7 +8712,7 @@
         <v>287</v>
       </c>
       <c r="D62" s="36" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="F62" s="10">
         <v>7</v>
@@ -9094,10 +9231,10 @@
       <c r="A87" s="10">
         <v>1</v>
       </c>
-      <c r="B87" s="107" t="s">
+      <c r="B87" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="C87" s="107" t="s">
+      <c r="C87" s="102" t="s">
         <v>76</v>
       </c>
       <c r="D87" s="72" t="s">
@@ -9164,7 +9301,7 @@
       <c r="A92" s="10">
         <v>6</v>
       </c>
-      <c r="B92" s="108" t="s">
+      <c r="B92" s="103" t="s">
         <v>289</v>
       </c>
       <c r="C92" s="10" t="s">
@@ -9178,10 +9315,10 @@
       <c r="A93" s="10">
         <v>7</v>
       </c>
-      <c r="B93" s="107" t="s">
+      <c r="B93" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="C93" s="107" t="s">
+      <c r="C93" s="102" t="s">
         <v>76</v>
       </c>
       <c r="D93" s="26" t="s">
@@ -9192,14 +9329,39 @@
       <c r="A94" s="10">
         <v>8</v>
       </c>
-      <c r="B94" s="107" t="s">
+      <c r="B94" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="C94" s="107" t="s">
+      <c r="C94" s="102" t="s">
         <v>76</v>
       </c>
       <c r="D94" s="20" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="110" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" t="s">
+        <v>721</v>
       </c>
     </row>
   </sheetData>
@@ -9213,7 +9375,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9223,6 +9385,7 @@
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9532,19 +9695,19 @@
       <c r="A1" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="108" t="s">
         <v>490</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
       <c r="F1" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="108" t="s">
         <v>508</v>
       </c>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -9680,11 +9843,11 @@
       <c r="F7" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="108" t="s">
         <v>516</v>
       </c>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -9818,11 +9981,11 @@
       <c r="F13" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G13" s="104" t="s">
+      <c r="G13" s="108" t="s">
         <v>519</v>
       </c>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="108"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -9896,11 +10059,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="108" t="s">
         <v>522</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -10004,19 +10167,19 @@
       <c r="A27" s="79">
         <v>17</v>
       </c>
-      <c r="B27" s="102" t="s">
+      <c r="B27" s="106" t="s">
         <v>530</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
       <c r="F27" s="81">
         <v>17</v>
       </c>
-      <c r="G27" s="103" t="s">
+      <c r="G27" s="107" t="s">
         <v>557</v>
       </c>
-      <c r="H27" s="103"/>
-      <c r="I27" s="103"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -10282,19 +10445,19 @@
       <c r="A41" s="79">
         <v>17</v>
       </c>
-      <c r="B41" s="102" t="s">
+      <c r="B41" s="106" t="s">
         <v>546</v>
       </c>
-      <c r="C41" s="102"/>
-      <c r="D41" s="102"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="106"/>
       <c r="F41" s="81">
         <v>18</v>
       </c>
-      <c r="G41" s="103" t="s">
+      <c r="G41" s="107" t="s">
         <v>564</v>
       </c>
-      <c r="H41" s="103"/>
-      <c r="I41" s="103"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -10564,11 +10727,11 @@
       <c r="A54" s="73">
         <v>2</v>
       </c>
-      <c r="B54" s="104" t="s">
+      <c r="B54" s="108" t="s">
         <v>458</v>
       </c>
-      <c r="C54" s="104"/>
-      <c r="D54" s="104"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -10856,21 +11019,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="44.28515625" customWidth="1"/>
+    <col min="9" max="9" width="44.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" customWidth="1"/>
@@ -10880,19 +11043,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="104" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="108" t="s">
         <v>622</v>
       </c>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -10959,17 +11122,17 @@
       <c r="D4" s="89" t="s">
         <v>582</v>
       </c>
-      <c r="F4" s="106">
+      <c r="F4" s="101">
         <v>2</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -11080,11 +11243,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="100" t="s">
+      <c r="G9" s="104" t="s">
         <v>603</v>
       </c>
-      <c r="H9" s="100"/>
-      <c r="I9" s="100"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -11208,11 +11371,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="104" t="s">
         <v>599</v>
       </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -11304,7 +11467,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45">
+    <row r="19" spans="1:9" ht="60">
       <c r="A19" s="10">
         <v>3</v>
       </c>
@@ -11327,7 +11490,7 @@
         <v>286</v>
       </c>
       <c r="I19" s="41" t="s">
-        <v>653</v>
+        <v>705</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -11346,14 +11509,14 @@
       <c r="F20" s="10">
         <v>10</v>
       </c>
-      <c r="G20" s="30" t="s">
-        <v>651</v>
-      </c>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="31" t="s">
+        <v>682</v>
+      </c>
+      <c r="H20" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="I20" s="70" t="s">
-        <v>652</v>
+      <c r="I20" s="68" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -11372,41 +11535,51 @@
       <c r="F21" s="10">
         <v>11</v>
       </c>
-      <c r="G21" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>94</v>
+      <c r="G21" s="31" t="s">
+        <v>684</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="68" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="F22" s="10"/>
-      <c r="G22" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>98</v>
+      <c r="F22" s="65">
+        <v>12</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>685</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>639</v>
+      </c>
+      <c r="I22" s="68" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="104" t="s">
         <v>624</v>
       </c>
-      <c r="C23" s="100"/>
-      <c r="D23" s="100"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="F23" s="10">
+        <v>13</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>650</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="I23" s="68" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
@@ -11421,12 +11594,18 @@
       <c r="D24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="100" t="s">
-        <v>676</v>
-      </c>
-      <c r="H24" s="100"/>
-      <c r="I24" s="100"/>
+      <c r="F24" s="10">
+        <v>14</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="68" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="96">
@@ -11442,16 +11621,16 @@
         <v>625</v>
       </c>
       <c r="F25" s="10">
-        <v>1</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>674</v>
+        <v>15</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>690</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="68" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -11468,16 +11647,16 @@
         <v>637</v>
       </c>
       <c r="F26" s="10">
-        <v>2</v>
-      </c>
-      <c r="G26" s="40" t="s">
-        <v>636</v>
-      </c>
-      <c r="H26" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>637</v>
+        <v>16</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -11494,16 +11673,16 @@
         <v>627</v>
       </c>
       <c r="F27" s="10">
-        <v>3</v>
-      </c>
-      <c r="G27" s="34" t="s">
-        <v>678</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>367</v>
-      </c>
-      <c r="I27" s="34" t="s">
-        <v>679</v>
+        <v>17</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -11519,18 +11698,6 @@
       <c r="D28" s="26" t="s">
         <v>638</v>
       </c>
-      <c r="F28" s="10">
-        <v>4</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>656</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="I28" s="89" t="s">
-        <v>657</v>
-      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="96">
@@ -11545,18 +11712,12 @@
       <c r="D29" s="26" t="s">
         <v>638</v>
       </c>
-      <c r="F29" s="10">
-        <v>5</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>589</v>
-      </c>
-      <c r="I29" s="39" t="s">
-        <v>671</v>
-      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="104" t="s">
+        <v>673</v>
+      </c>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="96">
@@ -11569,19 +11730,19 @@
         <v>76</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>650</v>
-      </c>
-      <c r="F30" s="65">
-        <v>6</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>589</v>
-      </c>
-      <c r="I30" s="41" t="s">
-        <v>660</v>
+        <v>649</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -11601,16 +11762,16 @@
         <v>108</v>
       </c>
       <c r="F31" s="10">
-        <v>7</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>94</v>
+        <v>2</v>
+      </c>
+      <c r="G31" s="109" t="s">
+        <v>636</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="26" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -11627,16 +11788,16 @@
         <v>631</v>
       </c>
       <c r="F32" s="10">
-        <v>8</v>
-      </c>
-      <c r="G32" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>98</v>
+        <v>3</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>675</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -11652,7 +11813,18 @@
       <c r="D33" s="26" t="s">
         <v>638</v>
       </c>
-      <c r="F33" s="14"/>
+      <c r="F33" s="10">
+        <v>4</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>654</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="89" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="97">
@@ -11667,12 +11839,18 @@
       <c r="D34" s="26" t="s">
         <v>638</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="100" t="s">
-        <v>665</v>
-      </c>
-      <c r="H34" s="100"/>
-      <c r="I34" s="100"/>
+      <c r="F34" s="10">
+        <v>5</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>589</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="97">
@@ -11685,19 +11863,19 @@
         <v>76</v>
       </c>
       <c r="D35" s="90" t="s">
-        <v>648</v>
-      </c>
-      <c r="F35" s="10">
-        <v>1</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I35" s="25" t="s">
-        <v>666</v>
+        <v>647</v>
+      </c>
+      <c r="F35" s="65">
+        <v>6</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>589</v>
+      </c>
+      <c r="I35" s="41" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -11711,20 +11889,20 @@
         <v>286</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="10">
-        <v>2</v>
-      </c>
-      <c r="G36" s="31" t="s">
-        <v>675</v>
-      </c>
-      <c r="H36" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="26" t="s">
-        <v>677</v>
+        <v>7</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -11742,16 +11920,16 @@
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="10">
-        <v>3</v>
-      </c>
-      <c r="G37" s="31" t="s">
-        <v>668</v>
-      </c>
-      <c r="H37" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>669</v>
+        <v>8</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30">
@@ -11765,58 +11943,54 @@
         <v>589</v>
       </c>
       <c r="D38" s="95" t="s">
-        <v>647</v>
-      </c>
-      <c r="F38" s="10">
-        <v>4</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>667</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" s="26" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="30">
       <c r="A39" s="10">
         <v>15</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C39" s="31" t="s">
         <v>589</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="41" t="s">
+        <v>659</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="100" t="s">
         <v>662</v>
       </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="100"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="99">
         <v>16</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C40" s="31" t="s">
         <v>96</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>664</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="100" t="s">
-        <v>672</v>
-      </c>
-      <c r="H40" s="100"/>
-      <c r="I40" s="100"/>
+        <v>661</v>
+      </c>
+      <c r="F40" s="10">
+        <v>1</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="25" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="99">
@@ -11832,16 +12006,16 @@
         <v>94</v>
       </c>
       <c r="F41" s="10">
-        <v>1</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" s="25" t="s">
-        <v>673</v>
+        <v>2</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>672</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -11859,16 +12033,16 @@
       </c>
       <c r="E42" s="92"/>
       <c r="F42" s="10">
-        <v>2</v>
-      </c>
-      <c r="G42" s="58" t="s">
-        <v>675</v>
-      </c>
-      <c r="H42" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="I42" t="s">
-        <v>677</v>
+        <v>3</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>665</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>666</v>
       </c>
       <c r="J42" s="92"/>
       <c r="K42" s="92"/>
@@ -11878,16 +12052,16 @@
       <c r="A43" s="14"/>
       <c r="B43" s="27"/>
       <c r="F43" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>259</v>
+        <v>664</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="I43" s="89" t="s">
-        <v>654</v>
+        <v>122</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>667</v>
       </c>
       <c r="J43" s="93"/>
     </row>
@@ -11896,23 +12070,11 @@
         <v>10</v>
       </c>
       <c r="B44" s="94" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C44" s="94"/>
       <c r="D44" s="94"/>
       <c r="E44" s="27"/>
-      <c r="F44" s="10">
-        <v>4</v>
-      </c>
-      <c r="G44" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="H44" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="I44" s="41" t="s">
-        <v>655</v>
-      </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="9" t="s">
@@ -11928,18 +12090,12 @@
         <v>74</v>
       </c>
       <c r="E45" s="27"/>
-      <c r="F45" s="10">
-        <v>5</v>
-      </c>
-      <c r="G45" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="H45" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="I45" s="36" t="s">
-        <v>659</v>
-      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="100" t="s">
+        <v>669</v>
+      </c>
+      <c r="H45" s="100"/>
+      <c r="I45" s="100"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="10">
@@ -11952,22 +12108,22 @@
         <v>76</v>
       </c>
       <c r="D46" s="72" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="E46" t="s">
         <v>108</v>
       </c>
       <c r="F46" s="10">
-        <v>6</v>
-      </c>
-      <c r="G46" s="31" t="s">
-        <v>265</v>
-      </c>
-      <c r="H46" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I46" s="41" t="s">
-        <v>427</v>
+        <v>1</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="30">
@@ -11981,19 +12137,19 @@
         <v>241</v>
       </c>
       <c r="D47" s="46" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="F47" s="10">
-        <v>7</v>
-      </c>
-      <c r="G47" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="H47" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I47" s="41" t="s">
-        <v>426</v>
+        <v>2</v>
+      </c>
+      <c r="G47" s="58" t="s">
+        <v>672</v>
+      </c>
+      <c r="H47" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -12010,16 +12166,16 @@
         <v>284</v>
       </c>
       <c r="F48" s="10">
-        <v>8</v>
-      </c>
-      <c r="G48" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="H48" s="40" t="s">
-        <v>262</v>
-      </c>
-      <c r="I48" s="41" t="s">
-        <v>425</v>
+        <v>3</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I48" s="89" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -12036,16 +12192,16 @@
         <v>292</v>
       </c>
       <c r="F49" s="10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G49" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="H49" s="40" t="s">
-        <v>264</v>
+        <v>255</v>
+      </c>
+      <c r="H49" s="26" t="s">
+        <v>122</v>
       </c>
       <c r="I49" s="41" t="s">
-        <v>425</v>
+        <v>653</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -12062,16 +12218,16 @@
         <v>291</v>
       </c>
       <c r="F50" s="10">
-        <v>10</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H50" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I50" s="20" t="s">
-        <v>94</v>
+        <v>5</v>
+      </c>
+      <c r="G50" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="I50" s="36" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -12088,16 +12244,16 @@
         <v>293</v>
       </c>
       <c r="F51" s="10">
-        <v>11</v>
-      </c>
-      <c r="G51" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I51" s="20" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I51" s="41" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -12113,6 +12269,18 @@
       <c r="D52" s="26" t="s">
         <v>186</v>
       </c>
+      <c r="F52" s="10">
+        <v>7</v>
+      </c>
+      <c r="G52" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="H52" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I52" s="41" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="10">
@@ -12127,23 +12295,461 @@
       <c r="D53" s="20" t="s">
         <v>98</v>
       </c>
+      <c r="F53" s="10">
+        <v>8</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="I53" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="F54" s="10">
+        <v>9</v>
+      </c>
+      <c r="G54" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="H54" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="I54" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="F55" s="10">
+        <v>10</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I55" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="5">
+        <v>10</v>
+      </c>
+      <c r="B56" s="100" t="s">
+        <v>688</v>
+      </c>
+      <c r="C56" s="100"/>
+      <c r="D56" s="100"/>
+      <c r="F56" s="10">
+        <v>11</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H56" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I56" s="20" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="57" spans="1:9">
+      <c r="A57" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="E57" t="s">
         <v>108</v>
       </c>
     </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="10">
+        <v>1</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="72" t="s">
+        <v>689</v>
+      </c>
+      <c r="F58" s="5">
+        <v>12</v>
+      </c>
+      <c r="G58" s="100" t="s">
+        <v>691</v>
+      </c>
+      <c r="H58" s="100"/>
+      <c r="I58" s="100"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="44">
+        <v>2</v>
+      </c>
+      <c r="B59" s="109" t="s">
+        <v>636</v>
+      </c>
+      <c r="C59" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>637</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="10">
+        <v>3</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>695</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="89" t="s">
+        <v>696</v>
+      </c>
+      <c r="F60" s="10">
+        <v>1</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I60" s="25" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="10">
+        <v>4</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>632</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="F61" s="10">
+        <v>2</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>693</v>
+      </c>
+      <c r="H61" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="I61" s="89" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="10">
+        <v>5</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>633</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="F62" s="10">
+        <v>3</v>
+      </c>
+      <c r="G62" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="I62" s="26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="10">
+        <v>6</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>697</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="41" t="s">
+        <v>698</v>
+      </c>
+      <c r="F63" s="10">
+        <v>4</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H63" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I63" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="10">
+        <v>7</v>
+      </c>
+      <c r="B64" s="31" t="s">
+        <v>699</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>700</v>
+      </c>
+      <c r="F64" s="10">
+        <v>5</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I64" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="10">
+        <v>8</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="10">
+        <v>9</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="F67" s="5">
+        <v>12</v>
+      </c>
+      <c r="G67" s="100" t="s">
+        <v>701</v>
+      </c>
+      <c r="H67" s="100"/>
+      <c r="I67" s="100"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="F68" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="B69" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69" s="10">
+        <v>1</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I69" s="25" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="F70" s="10">
+        <v>2</v>
+      </c>
+      <c r="G70" s="26" t="s">
+        <v>672</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I70" s="89" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="F71" s="10">
+        <v>3</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>636</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I71" s="26" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="D72" t="s">
+        <v>108</v>
+      </c>
+      <c r="F72" s="10">
+        <v>4</v>
+      </c>
+      <c r="G72" s="26" t="s">
+        <v>709</v>
+      </c>
+      <c r="H72" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="I72" s="26" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="F73" s="10">
+        <v>5</v>
+      </c>
+      <c r="G73" s="31" t="s">
+        <v>711</v>
+      </c>
+      <c r="H73" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="I73" s="26" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="F74" s="10">
+        <v>6</v>
+      </c>
+      <c r="G74" s="31" t="s">
+        <v>713</v>
+      </c>
+      <c r="H74" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="I74" s="26" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="F75" s="10">
+        <v>7</v>
+      </c>
+      <c r="G75" s="31" t="s">
+        <v>715</v>
+      </c>
+      <c r="H75" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="I75" s="26" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="F76" s="10">
+        <v>8</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H76" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I76" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="F77" s="10">
+        <v>9</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H77" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I77" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="G80" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="6">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G29:I29"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update sub menu manufaktur
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="rev marketing" sheetId="8" r:id="rId6"/>
     <sheet name="superadmin_ukm" sheetId="10" r:id="rId7"/>
     <sheet name="jasa" sheetId="12" r:id="rId8"/>
+    <sheet name="manufaktur" sheetId="14" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="788">
   <si>
     <t>Revisi2</t>
   </si>
@@ -2365,18 +2367,6 @@
     <t>FK tabel satuan</t>
   </si>
   <si>
-    <t>p_alur_jasa</t>
-  </si>
-  <si>
-    <t>PK tabel alur layanan</t>
-  </si>
-  <si>
-    <t>nama_alur</t>
-  </si>
-  <si>
-    <t>nama alur layanan</t>
-  </si>
-  <si>
     <t>p_order_jasa</t>
   </si>
   <si>
@@ -2828,6 +2818,261 @@
   </si>
   <si>
     <t>berapa saldo kas akhir ketika selseai shift</t>
+  </si>
+  <si>
+    <t>jenis_barang</t>
+  </si>
+  <si>
+    <t>enum(0,1,2)</t>
+  </si>
+  <si>
+    <t>0 = brg mentah, 1 = brg dlm proses, 3 =brg jadi</t>
+  </si>
+  <si>
+    <t>p_proses_bisnis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK tabel proses bisnis dan jasa di gabung </t>
+  </si>
+  <si>
+    <t>proses_bisnis</t>
+  </si>
+  <si>
+    <t>proses produksi (manufaktur), alur layanan (jasa)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK p_barang, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jika manufaktur jenis_barang = 3, jika jasa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">keterangan, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>nullable</t>
+    </r>
+  </si>
+  <si>
+    <t>p_proses_produksi</t>
+  </si>
+  <si>
+    <t>p_bahan_produksi</t>
+  </si>
+  <si>
+    <t>p_tenaga_produksi</t>
+  </si>
+  <si>
+    <t>id_proses_bisnis</t>
+  </si>
+  <si>
+    <t>jemur</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>tgl mulai</t>
+  </si>
+  <si>
+    <t>tgl selesai</t>
+  </si>
+  <si>
+    <t>PK tabel bahan produksi</t>
+  </si>
+  <si>
+    <t>id_proses_produksi</t>
+  </si>
+  <si>
+    <t>FK tabel p_proses_produksi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FK p_barang.jenis_barang=1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FK p_barang.jenis_brg=2, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>brg jadi</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">proses produksi </t>
+  </si>
+  <si>
+    <t>barang_mentah</t>
+  </si>
+  <si>
+    <t>jumlah_bahan</t>
+  </si>
+  <si>
+    <t>banyaknya brg mentah</t>
+  </si>
+  <si>
+    <t>PK tabel tenaga kerja dlm membuat produk</t>
+  </si>
+  <si>
+    <t>tenaga_kerja</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FK h_karyawan</t>
+  </si>
+  <si>
+    <t>upah_perjam</t>
+  </si>
+  <si>
+    <t>upah karyawan per jam, FK h_gaji</t>
+  </si>
+  <si>
+    <t>tgl mulai produksi brg, today</t>
+  </si>
+  <si>
+    <t>nama proses</t>
+  </si>
+  <si>
+    <t>campur</t>
+  </si>
+  <si>
+    <t>goreng</t>
+  </si>
+  <si>
+    <t>bumbu</t>
+  </si>
+  <si>
+    <t>packing</t>
+  </si>
+  <si>
+    <t>proses</t>
+  </si>
+  <si>
+    <t>tgl_produksi_awal</t>
+  </si>
+  <si>
+    <t>tgl_produksi_akhir</t>
+  </si>
+  <si>
+    <t>31-02-2020</t>
+  </si>
+  <si>
+    <t>rincian_produksi</t>
+  </si>
+  <si>
+    <t>apa yg di kerjakan</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>ada brg setengah jadi</t>
+  </si>
+  <si>
+    <t>brg_jadi</t>
+  </si>
+  <si>
+    <t>nm_brg_1/2_jadi</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>sohun</t>
+  </si>
+  <si>
+    <t>id_pp</t>
+  </si>
+  <si>
+    <t>mulai_produksi</t>
+  </si>
+  <si>
+    <t>proses_produksi</t>
+  </si>
+  <si>
+    <t>jumlah brg setengah jadi</t>
+  </si>
+  <si>
+    <t>p_tambah_produksi</t>
+  </si>
+  <si>
+    <t>FK p_barang.jenis_brg = 2</t>
+  </si>
+  <si>
+    <t>supervisor_produksi</t>
+  </si>
+  <si>
+    <t>FK h_karyawan</t>
+  </si>
+  <si>
+    <t>PK tabel tambah produksi manufaktur</t>
+  </si>
+  <si>
+    <t>FK tabel p_proses_bisnis</t>
+  </si>
+  <si>
+    <t>apa yg di kerjakan, masalah, solusi, dll</t>
+  </si>
+  <si>
+    <t>brg_dlm_proses</t>
+  </si>
+  <si>
+    <t>FK p_barang.jenis_brg = 1, nullable</t>
+  </si>
+  <si>
+    <t>jum_bdp</t>
+  </si>
+  <si>
+    <t>jumlah brg dlm proses, nullable</t>
+  </si>
+  <si>
+    <t>jum_brg_jadi</t>
+  </si>
+  <si>
+    <t>jumlah brg jadi</t>
+  </si>
+  <si>
+    <t>status_bdp</t>
+  </si>
+  <si>
+    <t>0 = langsung di olah menjd brg jadi, 1 = masukkan ke stok akhir</t>
+  </si>
+  <si>
+    <t>jam_selsesai</t>
   </si>
 </sst>
 </file>
@@ -3086,7 +3331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3307,6 +3552,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3322,8 +3581,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3898,6 +4161,227 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="117" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="117" t="s">
+        <v>763</v>
+      </c>
+      <c r="C2" s="117" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2" s="117" t="s">
+        <v>762</v>
+      </c>
+      <c r="E2" s="117" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>751</v>
+      </c>
+      <c r="D3" t="s">
+        <v>765</v>
+      </c>
+      <c r="E3" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>753</v>
+      </c>
+      <c r="D4" t="s">
+        <v>765</v>
+      </c>
+      <c r="E4" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>752</v>
+      </c>
+      <c r="D5" t="s">
+        <v>766</v>
+      </c>
+      <c r="E5" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D6" t="s">
+        <v>765</v>
+      </c>
+      <c r="E6" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="116" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="116" t="s">
+        <v>768</v>
+      </c>
+      <c r="C10" s="116" t="s">
+        <v>756</v>
+      </c>
+      <c r="D10" s="116" t="s">
+        <v>757</v>
+      </c>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="93">
+        <v>43873</v>
+      </c>
+      <c r="D11" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="116" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>755</v>
+      </c>
+      <c r="C16" t="s">
+        <v>733</v>
+      </c>
+      <c r="D16" t="s">
+        <v>760</v>
+      </c>
+      <c r="E16" t="s">
+        <v>734</v>
+      </c>
+      <c r="F16" t="s">
+        <v>640</v>
+      </c>
+      <c r="G16" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>751</v>
+      </c>
+      <c r="C17" s="93">
+        <v>43873</v>
+      </c>
+      <c r="D17" t="s">
+        <v>761</v>
+      </c>
+      <c r="F17" t="s">
+        <v>766</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>731</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="E22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
@@ -4120,7 +4604,7 @@
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -4137,30 +4621,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="104" t="s">
+      <c r="G2" s="110" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -4292,17 +4776,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="10">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="11"/>
+      <c r="B8" s="34" t="s">
+        <v>718</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>719</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>720</v>
+      </c>
       <c r="F8" s="10">
         <v>5</v>
       </c>
@@ -4321,10 +4807,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D9" s="11"/>
       <c r="F9" s="10">
@@ -4345,14 +4831,12 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="D10" s="11"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:11">
@@ -4360,13 +4844,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>598</v>
+        <v>96</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="F11" s="14"/>
     </row>
@@ -4375,35 +4859,35 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>104</v>
+        <v>76</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>598</v>
       </c>
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="104" t="s">
+      <c r="G12" s="110" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
         <v>10</v>
       </c>
-      <c r="B13" s="34" t="s">
-        <v>577</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>578</v>
+      <c r="B13" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>71</v>
@@ -4425,14 +4909,14 @@
       <c r="A14" s="10">
         <v>11</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>107</v>
+      <c r="B14" s="34" t="s">
+        <v>577</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>578</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
@@ -4452,13 +4936,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F15" s="10">
         <v>2</v>
@@ -4478,13 +4962,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F16" s="10">
         <v>3</v>
@@ -4503,14 +4987,14 @@
       <c r="A17" s="10">
         <v>14</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>117</v>
+      <c r="B17" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="F17" s="10">
         <v>4</v>
@@ -4529,14 +5013,14 @@
       <c r="A18" s="10">
         <v>15</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>123</v>
+      <c r="B18" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="F18" s="10">
         <v>6</v>
@@ -4551,18 +5035,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30">
+    <row r="19" spans="1:9">
       <c r="A19" s="10">
         <v>16</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>128</v>
+      <c r="B19" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="F19" s="10">
         <v>7</v>
@@ -4577,32 +5061,32 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="30">
       <c r="A20" s="88">
         <v>17</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>131</v>
+      <c r="B20" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="10">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>94</v>
+      <c r="B21" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -4610,12 +5094,23 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="17" t="s">
+      <c r="C23" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4623,21 +5118,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="104" t="s">
+      <c r="G24" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
+      <c r="H24" s="110"/>
+      <c r="I24" s="110"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="104" t="s">
+      <c r="B25" s="110" t="s">
         <v>587</v>
       </c>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -4785,11 +5280,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="104" t="s">
+      <c r="G33" s="110" t="s">
         <v>144</v>
       </c>
-      <c r="H33" s="104"/>
-      <c r="I33" s="104"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="110"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -5041,11 +5536,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="104" t="s">
+      <c r="B45" s="110" t="s">
         <v>151</v>
       </c>
-      <c r="C45" s="104"/>
-      <c r="D45" s="104"/>
+      <c r="C45" s="110"/>
+      <c r="D45" s="110"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -7330,7 +7825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B90" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
@@ -8712,7 +9207,7 @@
         <v>287</v>
       </c>
       <c r="D62" s="36" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F62" s="10">
         <v>7</v>
@@ -9340,28 +9835,28 @@
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="110" t="s">
-        <v>717</v>
+      <c r="B98" s="105" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
   </sheetData>
@@ -9695,19 +10190,19 @@
       <c r="A1" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="114" t="s">
         <v>490</v>
       </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
       <c r="F1" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="114" t="s">
         <v>508</v>
       </c>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -9843,11 +10338,11 @@
       <c r="F7" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G7" s="108" t="s">
+      <c r="G7" s="114" t="s">
         <v>516</v>
       </c>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -9981,11 +10476,11 @@
       <c r="F13" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G13" s="108" t="s">
+      <c r="G13" s="114" t="s">
         <v>519</v>
       </c>
-      <c r="H13" s="108"/>
-      <c r="I13" s="108"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -10059,11 +10554,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="114" t="s">
         <v>522</v>
       </c>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -10167,19 +10662,19 @@
       <c r="A27" s="79">
         <v>17</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="112" t="s">
         <v>530</v>
       </c>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
       <c r="F27" s="81">
         <v>17</v>
       </c>
-      <c r="G27" s="107" t="s">
+      <c r="G27" s="113" t="s">
         <v>557</v>
       </c>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -10445,19 +10940,19 @@
       <c r="A41" s="79">
         <v>17</v>
       </c>
-      <c r="B41" s="106" t="s">
+      <c r="B41" s="112" t="s">
         <v>546</v>
       </c>
-      <c r="C41" s="106"/>
-      <c r="D41" s="106"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
       <c r="F41" s="81">
         <v>18</v>
       </c>
-      <c r="G41" s="107" t="s">
+      <c r="G41" s="113" t="s">
         <v>564</v>
       </c>
-      <c r="H41" s="107"/>
-      <c r="I41" s="107"/>
+      <c r="H41" s="113"/>
+      <c r="I41" s="113"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -10727,11 +11222,11 @@
       <c r="A54" s="73">
         <v>2</v>
       </c>
-      <c r="B54" s="108" t="s">
+      <c r="B54" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="C54" s="108"/>
-      <c r="D54" s="108"/>
+      <c r="C54" s="114"/>
+      <c r="D54" s="114"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -10930,7 +11425,7 @@
         <v>96</v>
       </c>
       <c r="D68" s="76" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -10952,13 +11447,13 @@
         <v>14</v>
       </c>
       <c r="B70" s="75" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C70" s="75" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D70" s="35" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -11021,8 +11516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D13"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11043,19 +11538,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="110" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="108" t="s">
-        <v>622</v>
-      </c>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
+      <c r="G1" s="114" t="s">
+        <v>618</v>
+      </c>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -11106,7 +11601,7 @@
         <v>76</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
@@ -11126,13 +11621,13 @@
         <v>2</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -11152,13 +11647,13 @@
         <v>2</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>103</v>
       </c>
       <c r="I5" s="89" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -11232,22 +11727,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>127</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="104" t="s">
-        <v>603</v>
-      </c>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
+      <c r="G9" s="110" t="s">
+        <v>599</v>
+      </c>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -11298,7 +11793,7 @@
         <v>76</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -11324,7 +11819,7 @@
         <v>119</v>
       </c>
       <c r="I12" s="89" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -11350,7 +11845,7 @@
         <v>76</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -11364,18 +11859,18 @@
         <v>76</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="104" t="s">
-        <v>599</v>
-      </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
+      <c r="B15" s="110" t="s">
+        <v>721</v>
+      </c>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -11386,7 +11881,7 @@
         <v>76</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -11406,13 +11901,13 @@
         <v>6</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>76</v>
       </c>
       <c r="I16" s="90" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -11426,33 +11921,33 @@
         <v>76</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>600</v>
+        <v>722</v>
       </c>
       <c r="F17" s="10">
         <v>7</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="H17" s="30" t="s">
         <v>103</v>
       </c>
       <c r="I17" s="70" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="10">
         <v>2</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>601</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="89" t="s">
-        <v>602</v>
+      <c r="B18" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>725</v>
       </c>
       <c r="F18" s="10">
         <v>8</v>
@@ -11464,136 +11959,136 @@
         <v>103</v>
       </c>
       <c r="I18" s="91" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="60">
-      <c r="A19" s="10">
+      <c r="A19" s="109">
         <v>3</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>238</v>
+      <c r="B19" s="108" t="s">
+        <v>723</v>
+      </c>
+      <c r="C19" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>724</v>
       </c>
       <c r="F19" s="65">
         <v>9</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="H19" s="31" t="s">
         <v>286</v>
       </c>
       <c r="I19" s="41" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="10">
         <v>4</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>94</v>
+      <c r="B20" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>726</v>
       </c>
       <c r="F20" s="10">
         <v>10</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="H20" s="31" t="s">
         <v>286</v>
       </c>
       <c r="I20" s="68" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="10">
+      <c r="A21" s="109">
         <v>5</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="10">
         <v>11</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>119</v>
       </c>
       <c r="I21" s="68" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="22" spans="1:9">
+      <c r="A22" s="10">
+        <v>6</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="F22" s="65">
         <v>12</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="I22" s="68" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="5">
-        <v>2</v>
-      </c>
-      <c r="B23" s="104" t="s">
-        <v>624</v>
-      </c>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
       <c r="F23" s="10">
         <v>13</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="H23" s="31" t="s">
         <v>286</v>
       </c>
       <c r="I23" s="68" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>74</v>
-      </c>
+      <c r="A24" s="5">
+        <v>2</v>
+      </c>
+      <c r="B24" s="110" t="s">
+        <v>620</v>
+      </c>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
       <c r="F24" s="10">
         <v>14</v>
       </c>
@@ -11604,47 +12099,47 @@
         <v>76</v>
       </c>
       <c r="I24" s="68" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="96">
-        <v>1</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>625</v>
+      <c r="A25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="F25" s="10">
         <v>15</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="H25" s="31" t="s">
         <v>122</v>
       </c>
       <c r="I25" s="68" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="96">
-        <v>2</v>
-      </c>
-      <c r="B26" s="57" t="s">
-        <v>636</v>
-      </c>
-      <c r="C26" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>637</v>
+        <v>1</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>621</v>
       </c>
       <c r="F26" s="10">
         <v>16</v>
@@ -11661,16 +12156,16 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="96">
-        <v>3</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>626</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="89" t="s">
-        <v>627</v>
+        <v>2</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>632</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" t="s">
+        <v>633</v>
       </c>
       <c r="F27" s="10">
         <v>17</v>
@@ -11687,50 +12182,50 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="96">
-        <v>4</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>632</v>
+        <v>3</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>622</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>638</v>
+        <v>76</v>
+      </c>
+      <c r="D28" s="89" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="96">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>639</v>
+        <v>119</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="104" t="s">
-        <v>673</v>
-      </c>
-      <c r="H29" s="104"/>
-      <c r="I29" s="104"/>
+      <c r="G29" s="110" t="s">
+        <v>669</v>
+      </c>
+      <c r="H29" s="110"/>
+      <c r="I29" s="110"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="96">
-        <v>6</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>645</v>
+        <v>5</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>629</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>649</v>
+        <v>635</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>634</v>
       </c>
       <c r="F30" s="10">
         <v>1</v>
@@ -11742,21 +12237,21 @@
         <v>76</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="97">
-        <v>7</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>628</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>629</v>
+        <v>667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30">
+      <c r="A31" s="96">
+        <v>6</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>641</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>645</v>
       </c>
       <c r="E31" t="s">
         <v>108</v>
@@ -11764,80 +12259,80 @@
       <c r="F31" s="10">
         <v>2</v>
       </c>
-      <c r="G31" s="109" t="s">
-        <v>636</v>
+      <c r="G31" s="104" t="s">
+        <v>632</v>
       </c>
       <c r="H31" s="40" t="s">
         <v>76</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="97">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>103</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="F32" s="10">
         <v>3</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="H32" s="34" t="s">
         <v>367</v>
       </c>
       <c r="I32" s="34" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="97">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>634</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>119</v>
+        <v>626</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
       <c r="F33" s="10">
         <v>4</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="H33" s="26" t="s">
         <v>122</v>
       </c>
       <c r="I33" s="89" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="97">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>639</v>
+        <v>119</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F34" s="10">
         <v>5</v>
@@ -11849,21 +12344,21 @@
         <v>589</v>
       </c>
       <c r="I34" s="39" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="97">
-        <v>11</v>
-      </c>
-      <c r="B35" s="90" t="s">
-        <v>644</v>
-      </c>
-      <c r="C35" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="90" t="s">
-        <v>647</v>
+        <v>10</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>631</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>635</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>634</v>
       </c>
       <c r="F35" s="65">
         <v>6</v>
@@ -11875,21 +12370,21 @@
         <v>589</v>
       </c>
       <c r="I35" s="41" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="98">
-        <v>12</v>
-      </c>
-      <c r="B36" s="31" t="s">
+      <c r="A36" s="97">
+        <v>11</v>
+      </c>
+      <c r="B36" s="90" t="s">
         <v>640</v>
       </c>
-      <c r="C36" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>648</v>
+      <c r="C36" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="90" t="s">
+        <v>643</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="10">
@@ -11907,16 +12402,16 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="98">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>103</v>
+        <v>286</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="10">
@@ -11932,52 +12427,52 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30">
+    <row r="38" spans="1:12">
       <c r="A38" s="98">
+        <v>13</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>637</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="30">
+      <c r="A39" s="98">
         <v>14</v>
       </c>
-      <c r="B38" s="30" t="s">
-        <v>646</v>
-      </c>
-      <c r="C38" s="30" t="s">
+      <c r="B39" s="30" t="s">
+        <v>642</v>
+      </c>
+      <c r="C39" s="30" t="s">
         <v>589</v>
       </c>
-      <c r="D38" s="95" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="30">
-      <c r="A39" s="10">
-        <v>15</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>658</v>
-      </c>
-      <c r="C39" s="31" t="s">
-        <v>589</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>659</v>
+      <c r="D39" s="95" t="s">
+        <v>700</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="100" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="H39" s="100"/>
       <c r="I39" s="100"/>
     </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="99">
-        <v>16</v>
+    <row r="40" spans="1:12" ht="30">
+      <c r="A40" s="10">
+        <v>15</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>661</v>
+        <v>589</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>655</v>
       </c>
       <c r="F40" s="10">
         <v>1</v>
@@ -11989,126 +12484,124 @@
         <v>76</v>
       </c>
       <c r="I40" s="25" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="99">
-        <v>17</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>94</v>
+        <v>16</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>656</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>657</v>
       </c>
       <c r="F41" s="10">
         <v>2</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="H41" s="31" t="s">
         <v>76</v>
       </c>
       <c r="I41" s="26" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="99">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E42" s="92"/>
       <c r="F42" s="10">
         <v>3</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="H42" s="40" t="s">
         <v>76</v>
       </c>
       <c r="I42" s="26" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="J42" s="92"/>
       <c r="K42" s="92"/>
       <c r="L42" s="92"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="14"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="99">
+        <v>18</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="F43" s="10">
         <v>4</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="H43" s="26" t="s">
         <v>122</v>
       </c>
       <c r="I43" s="26" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="J43" s="93"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="5">
+      <c r="E44" s="27"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="5">
         <v>10</v>
       </c>
-      <c r="B44" s="94" t="s">
-        <v>679</v>
-      </c>
-      <c r="C44" s="94"/>
-      <c r="D44" s="94"/>
-      <c r="E44" s="27"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>74</v>
-      </c>
+      <c r="B45" s="94" t="s">
+        <v>675</v>
+      </c>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
       <c r="E45" s="27"/>
       <c r="F45" s="5"/>
       <c r="G45" s="100" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="H45" s="100"/>
       <c r="I45" s="100"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="10">
-        <v>1</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="72" t="s">
-        <v>680</v>
+      <c r="A46" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E46" t="s">
         <v>108</v>
@@ -12123,47 +12616,47 @@
         <v>76</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="30">
-      <c r="A47" s="44">
-        <v>2</v>
-      </c>
-      <c r="B47" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="C47" s="45" t="s">
-        <v>241</v>
-      </c>
-      <c r="D47" s="46" t="s">
-        <v>681</v>
+        <v>666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="10">
+        <v>1</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="72" t="s">
+        <v>676</v>
       </c>
       <c r="F47" s="10">
         <v>2</v>
       </c>
       <c r="G47" s="58" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="H47" s="58" t="s">
         <v>76</v>
       </c>
       <c r="I47" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="10">
-        <v>3</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="36" t="s">
-        <v>284</v>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30">
+      <c r="A48" s="44">
+        <v>2</v>
+      </c>
+      <c r="B48" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="C48" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>677</v>
       </c>
       <c r="F48" s="10">
         <v>3</v>
@@ -12175,21 +12668,21 @@
         <v>119</v>
       </c>
       <c r="I48" s="89" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>286</v>
+        <v>76</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="F49" s="10">
         <v>4</v>
@@ -12201,21 +12694,21 @@
         <v>122</v>
       </c>
       <c r="I49" s="41" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="10">
-        <v>5</v>
-      </c>
-      <c r="B50" s="31" t="s">
-        <v>288</v>
+        <v>4</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>283</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>291</v>
+        <v>286</v>
+      </c>
+      <c r="D50" s="36" t="s">
+        <v>292</v>
       </c>
       <c r="F50" s="10">
         <v>5</v>
@@ -12227,21 +12720,21 @@
         <v>287</v>
       </c>
       <c r="I50" s="36" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="10">
-        <v>6</v>
-      </c>
-      <c r="B51" s="30" t="s">
-        <v>289</v>
+        <v>5</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>288</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="D51" s="39" t="s">
-        <v>293</v>
+        <v>290</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>291</v>
       </c>
       <c r="F51" s="10">
         <v>6</v>
@@ -12258,16 +12751,16 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="10">
-        <v>7</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>186</v>
+        <v>6</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>293</v>
       </c>
       <c r="F52" s="10">
         <v>7</v>
@@ -12284,16 +12777,16 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>98</v>
+      <c r="D53" s="26" t="s">
+        <v>186</v>
       </c>
       <c r="F53" s="10">
         <v>8</v>
@@ -12309,6 +12802,18 @@
       </c>
     </row>
     <row r="54" spans="1:9">
+      <c r="A54" s="10">
+        <v>8</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="F54" s="10">
         <v>9</v>
       </c>
@@ -12341,7 +12846,7 @@
         <v>10</v>
       </c>
       <c r="B56" s="100" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="C56" s="100"/>
       <c r="D56" s="100"/>
@@ -12386,13 +12891,13 @@
         <v>76</v>
       </c>
       <c r="D58" s="72" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="F58" s="5">
         <v>12</v>
       </c>
       <c r="G58" s="100" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="H58" s="100"/>
       <c r="I58" s="100"/>
@@ -12401,14 +12906,14 @@
       <c r="A59" s="44">
         <v>2</v>
       </c>
-      <c r="B59" s="109" t="s">
-        <v>636</v>
+      <c r="B59" s="104" t="s">
+        <v>632</v>
       </c>
       <c r="C59" s="40" t="s">
         <v>76</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>71</v>
@@ -12428,13 +12933,13 @@
         <v>3</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C60" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D60" s="89" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="F60" s="10">
         <v>1</v>
@@ -12446,7 +12951,7 @@
         <v>76</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -12454,25 +12959,25 @@
         <v>4</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>119</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F61" s="10">
         <v>2</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="H61" s="26" t="s">
         <v>96</v>
       </c>
       <c r="I61" s="89" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -12480,13 +12985,13 @@
         <v>5</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F62" s="10">
         <v>3</v>
@@ -12506,13 +13011,13 @@
         <v>6</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>127</v>
       </c>
       <c r="D63" s="41" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="F63" s="10">
         <v>4</v>
@@ -12532,13 +13037,13 @@
         <v>7</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C64" s="30" t="s">
         <v>103</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="F64" s="10">
         <v>5</v>
@@ -12586,7 +13091,7 @@
         <v>12</v>
       </c>
       <c r="G67" s="100" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="H67" s="100"/>
       <c r="I67" s="100"/>
@@ -12619,7 +13124,7 @@
         <v>76</v>
       </c>
       <c r="I69" s="25" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -12627,13 +13132,13 @@
         <v>2</v>
       </c>
       <c r="G70" s="26" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="H70" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I70" s="89" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -12641,13 +13146,13 @@
         <v>3</v>
       </c>
       <c r="G71" s="31" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="H71" s="20" t="s">
         <v>76</v>
       </c>
       <c r="I71" s="26" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -12658,13 +13163,13 @@
         <v>4</v>
       </c>
       <c r="G72" s="26" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="H72" s="26" t="s">
         <v>103</v>
       </c>
       <c r="I72" s="26" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -12672,13 +13177,13 @@
         <v>5</v>
       </c>
       <c r="G73" s="31" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="H73" s="31" t="s">
         <v>127</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -12686,13 +13191,13 @@
         <v>6</v>
       </c>
       <c r="G74" s="31" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="H74" s="31" t="s">
         <v>103</v>
       </c>
       <c r="I74" s="26" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -12700,13 +13205,13 @@
         <v>7</v>
       </c>
       <c r="G75" s="31" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="H75" s="31" t="s">
         <v>127</v>
       </c>
       <c r="I75" s="26" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -12744,7 +13249,7 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="G29:I29"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B15:D15"/>
@@ -12754,4 +13259,666 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="44.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="5">
+        <v>1</v>
+      </c>
+      <c r="B1" s="110" t="s">
+        <v>721</v>
+      </c>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="F1" s="5">
+        <v>2</v>
+      </c>
+      <c r="G1" s="110" t="s">
+        <v>772</v>
+      </c>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>722</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>739</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="109">
+        <v>3</v>
+      </c>
+      <c r="B5" s="108" t="s">
+        <v>723</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>740</v>
+      </c>
+      <c r="F5" s="109">
+        <v>3</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>733</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>726</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>774</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="109">
+        <v>5</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="109">
+        <v>5</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>779</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="F9" s="109">
+        <v>7</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>781</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="106" t="s">
+        <v>728</v>
+      </c>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>785</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="109">
+        <v>9</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>783</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="10">
+        <v>1</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>735</v>
+      </c>
+      <c r="F12" s="10">
+        <v>10</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>736</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>737</v>
+      </c>
+      <c r="F13" s="109">
+        <v>11</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="109">
+        <v>3</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>741</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>738</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="10">
+        <v>4</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>742</v>
+      </c>
+      <c r="C15" s="115" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>743</v>
+      </c>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="109">
+        <v>5</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4</v>
+      </c>
+      <c r="G16" s="110" t="s">
+        <v>729</v>
+      </c>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="10">
+        <v>6</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>744</v>
+      </c>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="F19" s="10">
+        <v>2</v>
+      </c>
+      <c r="G19" s="118" t="s">
+        <v>736</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>737</v>
+      </c>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="F20" s="109">
+        <v>3</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>745</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5">
+        <v>4</v>
+      </c>
+      <c r="B21" s="110" t="s">
+        <v>727</v>
+      </c>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="F21" s="10">
+        <v>4</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>747</v>
+      </c>
+      <c r="H21" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="109">
+        <v>5</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="10">
+        <v>1</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>744</v>
+      </c>
+      <c r="F23" s="10">
+        <v>6</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="10">
+        <v>2</v>
+      </c>
+      <c r="B24" s="118" t="s">
+        <v>736</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>737</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="109">
+        <v>3</v>
+      </c>
+      <c r="B25" s="118" t="s">
+        <v>730</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="10">
+        <v>4</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>628</v>
+      </c>
+      <c r="C26" s="115"/>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="109">
+        <v>5</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>629</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="10">
+        <v>6</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="109">
+        <v>7</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="10">
+        <v>8</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>787</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="109">
+        <v>9</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="10">
+        <v>10</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
revisi menu coaching-investor-superadmin ukm
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
@@ -16,7 +16,8 @@
     <sheet name="superadmin_ukm" sheetId="7" r:id="rId7"/>
     <sheet name="jasa" sheetId="8" r:id="rId8"/>
     <sheet name="manufaktur" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
+    <sheet name="coach" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="1031">
   <si>
     <t>Revisi2</t>
   </si>
@@ -3745,6 +3746,462 @@
   <si>
     <t>jumlah hrg</t>
   </si>
+  <si>
+    <t>PK tabel data coach</t>
+  </si>
+  <si>
+    <t>nama coach</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>no rek</t>
+  </si>
+  <si>
+    <t>atas nama</t>
+  </si>
+  <si>
+    <t>tmp_lahir</t>
+  </si>
+  <si>
+    <t>tempat lahir</t>
+  </si>
+  <si>
+    <t>tgl_lahir</t>
+  </si>
+  <si>
+    <t>tanggal lahr</t>
+  </si>
+  <si>
+    <t>jenis_kel</t>
+  </si>
+  <si>
+    <t>0 = laki2, 1 = perempuan</t>
+  </si>
+  <si>
+    <t>status_perkawinan</t>
+  </si>
+  <si>
+    <t>0 = belum kawin, 1 = sudah kawin, 2 = janda, 3 = duda</t>
+  </si>
+  <si>
+    <t>telegram</t>
+  </si>
+  <si>
+    <t>signal</t>
+  </si>
+  <si>
+    <t>bip</t>
+  </si>
+  <si>
+    <t>c_pendidikan_formal</t>
+  </si>
+  <si>
+    <t>PK tabel pendidikan formal</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> photo</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd, smp, sma, dll </t>
+  </si>
+  <si>
+    <t>nm_sekolah</t>
+  </si>
+  <si>
+    <t>nama sekolah/pt, dll</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>c_pendidikan_non_formal</t>
+  </si>
+  <si>
+    <t>PK tabel pendidikan no formal</t>
+  </si>
+  <si>
+    <t>kursus, pelatihan, dll</t>
+  </si>
+  <si>
+    <t>sertikat</t>
+  </si>
+  <si>
+    <t>c_riwayat_mentor</t>
+  </si>
+  <si>
+    <t>PK tabel mengisi pelatihan /mentoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tgl mengisi </t>
+  </si>
+  <si>
+    <t>tgl_akhir</t>
+  </si>
+  <si>
+    <t>tempat</t>
+  </si>
+  <si>
+    <t>nm_pelatihan</t>
+  </si>
+  <si>
+    <t>nama_klien</t>
+  </si>
+  <si>
+    <t>c_riwayat_usaha</t>
+  </si>
+  <si>
+    <t>PK tabel riwayat usaha</t>
+  </si>
+  <si>
+    <t>nama_usaha</t>
+  </si>
+  <si>
+    <t>bentuk_usaha</t>
+  </si>
+  <si>
+    <t>enum(0,1,2,3)</t>
+  </si>
+  <si>
+    <t>0= PT, 1 = CV, 2=UD, 3=tanpa badanusaha</t>
+  </si>
+  <si>
+    <t>jabatan_usaha</t>
+  </si>
+  <si>
+    <t>di perusahan sebagai apa</t>
+  </si>
+  <si>
+    <t>status_usaha</t>
+  </si>
+  <si>
+    <t>0 = masih berjalan, 1 = tutup usaha</t>
+  </si>
+  <si>
+    <t>c_riwayat_buku</t>
+  </si>
+  <si>
+    <t>fb</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>ig</t>
+  </si>
+  <si>
+    <t>youtube</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>PK tabel buku/artikel yg pernah di tulis</t>
+  </si>
+  <si>
+    <t>nama__buku</t>
+  </si>
+  <si>
+    <t>judul buku/artikel</t>
+  </si>
+  <si>
+    <t>penerbit</t>
+  </si>
+  <si>
+    <t>nama penerbit</t>
+  </si>
+  <si>
+    <t>thn terbit</t>
+  </si>
+  <si>
+    <t>gambar buku</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>link untuk melihat buku/tulisan</t>
+  </si>
+  <si>
+    <t>c_rek_coach</t>
+  </si>
+  <si>
+    <t>PK tabel rek coach</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
+  </si>
+  <si>
+    <t>atas nama pemilik</t>
+  </si>
+  <si>
+    <t>jenis_mentor</t>
+  </si>
+  <si>
+    <t>0 = pelatihan, 1 = mentoring/pendampingan</t>
+  </si>
+  <si>
+    <t>specialist</t>
+  </si>
+  <si>
+    <t>specialist bidang coach</t>
+  </si>
+  <si>
+    <t>varchar(250)</t>
+  </si>
+  <si>
+    <t>PK tabel bidang yg di tangani utuk umkm</t>
+  </si>
+  <si>
+    <t>aspek_usaha</t>
+  </si>
+  <si>
+    <t>c_aspek_usaha</t>
+  </si>
+  <si>
+    <t>PK tabel aspek coaching</t>
+  </si>
+  <si>
+    <t>c_aspek_coaching</t>
+  </si>
+  <si>
+    <t>id_coach</t>
+  </si>
+  <si>
+    <t>c_coach</t>
+  </si>
+  <si>
+    <t>FK tabel c_coach</t>
+  </si>
+  <si>
+    <t>id_aspek_usaha</t>
+  </si>
+  <si>
+    <t>FK tabel uc_aspek_usaha</t>
+  </si>
+  <si>
+    <t>keterangan tambahn gabug sj di sini</t>
+  </si>
+  <si>
+    <t>c_biaya_coaching</t>
+  </si>
+  <si>
+    <t>PK tabel biaya coaching</t>
+  </si>
+  <si>
+    <t>ket ttg biaya di sini</t>
+  </si>
+  <si>
+    <t>model_biaya</t>
+  </si>
+  <si>
+    <t>0 = bagi hasil selama coaching, 2 = fixed, 3 = kesepakatan dg umkm</t>
+  </si>
+  <si>
+    <t>besarnya</t>
+  </si>
+  <si>
+    <t>int(12)</t>
+  </si>
+  <si>
+    <t>besarnya biaya.</t>
+  </si>
+  <si>
+    <t>lama_coaching</t>
+  </si>
+  <si>
+    <t>administrasi, marketing, keuangan, HRD, penggajian, investasi, marketing, produksi, penjualan, jasa</t>
+  </si>
+  <si>
+    <t>status_coach</t>
+  </si>
+  <si>
+    <t>0= aktif, 1= non aktif</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>c_reg_coaching</t>
+  </si>
+  <si>
+    <t>PK tabel registrasi coaching</t>
+  </si>
+  <si>
+    <t>FK u_user_ukm</t>
+  </si>
+  <si>
+    <t>tgl registrasi</t>
+  </si>
+  <si>
+    <t>descripsi perusahaan:</t>
+  </si>
+  <si>
+    <t>thn berdiri</t>
+  </si>
+  <si>
+    <t>badan hukum</t>
+  </si>
+  <si>
+    <t>bidang usaha</t>
+  </si>
+  <si>
+    <t>spesifik usaha</t>
+  </si>
+  <si>
+    <t>jumlah karyawan</t>
+  </si>
+  <si>
+    <t>deskripsi masalah perusahaan</t>
+  </si>
+  <si>
+    <t>goal yg diinginkan ikut pendampingan</t>
+  </si>
+  <si>
+    <t>tgl_registrasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date </t>
+  </si>
+  <si>
+    <t>masalah_usaha</t>
+  </si>
+  <si>
+    <t>descripsi masalah yg ingin diselesaiakan</t>
+  </si>
+  <si>
+    <t>goal_coaching</t>
+  </si>
+  <si>
+    <t>goal yg ingin di capai dg ikut coaching</t>
+  </si>
+  <si>
+    <t>tgl_approve</t>
+  </si>
+  <si>
+    <t>status_app</t>
+  </si>
+  <si>
+    <t>0= approve, 1 = reject</t>
+  </si>
+  <si>
+    <t>alasan</t>
+  </si>
+  <si>
+    <t>alasan approve / reject</t>
+  </si>
+  <si>
+    <t>c_proses_coaching</t>
+  </si>
+  <si>
+    <t>c_identifikasi_problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK tabel </t>
+  </si>
+  <si>
+    <t>id_batch_coaching</t>
+  </si>
+  <si>
+    <t>FK c_batch_coaching</t>
+  </si>
+  <si>
+    <t>FK c_aspek_usaha</t>
+  </si>
+  <si>
+    <t>masalah</t>
+  </si>
+  <si>
+    <t>tgl identifikasi masalah</t>
+  </si>
+  <si>
+    <t>c_rencana_solusi</t>
+  </si>
+  <si>
+    <t>rencana solusi</t>
+  </si>
+  <si>
+    <t>PK tabel proses coaching</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>report yg di butuhkan</t>
+  </si>
+  <si>
+    <t>tgl_periksa</t>
+  </si>
+  <si>
+    <t>tgl periksa laporan oleh coaching</t>
+  </si>
+  <si>
+    <t>rekomendasi</t>
+  </si>
+  <si>
+    <t>id_rencana_solusi</t>
+  </si>
+  <si>
+    <t>FK c_rencana_solusi</t>
+  </si>
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>goal yg ingin di capai</t>
+  </si>
+  <si>
+    <t>feedback_ukm</t>
+  </si>
+  <si>
+    <t>feedback dari ukm</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>0= sdg berlangsung, 1 = selesai</t>
+  </si>
+  <si>
+    <t>id_reg_coach</t>
+  </si>
+  <si>
+    <t>FK c_reg_coaching</t>
+  </si>
+  <si>
+    <t>tgl_im</t>
+  </si>
+  <si>
+    <t>id_ip</t>
+  </si>
+  <si>
+    <t>FK c_identifikasi_problem</t>
+  </si>
+  <si>
+    <t>tgl_awal</t>
+  </si>
+  <si>
+    <t>jumlah_hari</t>
+  </si>
+  <si>
+    <t>tgl_awal - tgl_akhir</t>
+  </si>
 </sst>
 </file>
 
@@ -3756,7 +4213,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3803,8 +4260,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3839,6 +4302,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3966,7 +4435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4155,8 +4624,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4164,13 +4654,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4750,9 +5253,1813 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="33"/>
+    <col min="6" max="6" width="6.28515625" style="33" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="33" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="33" customWidth="1"/>
+    <col min="9" max="9" width="44.85546875" style="33" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="33" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="33" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" style="33"/>
+    <col min="13" max="13" width="15.5703125" style="33" customWidth="1"/>
+    <col min="14" max="16384" width="8.5703125" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5"/>
+      <c r="B1" s="103" t="s">
+        <v>957</v>
+      </c>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="93" t="s">
+        <v>895</v>
+      </c>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>879</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="80" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>578</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="97" t="s">
+        <v>899</v>
+      </c>
+      <c r="H4" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="81" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="68">
+        <v>3</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>974</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>975</v>
+      </c>
+      <c r="F5" s="68">
+        <v>3</v>
+      </c>
+      <c r="G5" s="81" t="s">
+        <v>901</v>
+      </c>
+      <c r="H5" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="82" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>972</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="81" t="s">
+        <v>973</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="81" t="s">
+        <v>546</v>
+      </c>
+      <c r="H6" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="81" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="68">
+        <v>5</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>832</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="95" t="s">
+        <v>880</v>
+      </c>
+      <c r="F7" s="68">
+        <v>5</v>
+      </c>
+      <c r="G7" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H7" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="81" t="s">
+        <v>884</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="68">
+        <v>7</v>
+      </c>
+      <c r="B9" s="97" t="s">
+        <v>886</v>
+      </c>
+      <c r="C9" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="97" t="s">
+        <v>887</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="94" t="s">
+        <v>904</v>
+      </c>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="81" t="s">
+        <v>888</v>
+      </c>
+      <c r="C10" s="81" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" s="81" t="s">
+        <v>889</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="68">
+        <v>9</v>
+      </c>
+      <c r="B11" s="81" t="s">
+        <v>890</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="82" t="s">
+        <v>891</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="80" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="81" t="s">
+        <v>897</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>898</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2</v>
+      </c>
+      <c r="G12" s="81" t="s">
+        <v>901</v>
+      </c>
+      <c r="H12" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="82" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="68">
+        <v>11</v>
+      </c>
+      <c r="B13" s="97" t="s">
+        <v>562</v>
+      </c>
+      <c r="C13" s="81" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="F13" s="68">
+        <v>3</v>
+      </c>
+      <c r="G13" s="81" t="s">
+        <v>546</v>
+      </c>
+      <c r="H13" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="81" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="97" t="s">
+        <v>569</v>
+      </c>
+      <c r="C14" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="F14" s="10">
+        <v>4</v>
+      </c>
+      <c r="G14" s="97" t="s">
+        <v>907</v>
+      </c>
+      <c r="H14" s="97" t="s">
+        <v>219</v>
+      </c>
+      <c r="I14" s="81"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="68">
+        <v>13</v>
+      </c>
+      <c r="B15" s="97" t="s">
+        <v>572</v>
+      </c>
+      <c r="C15" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
+      <c r="G15" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H15" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="97" t="s">
+        <v>578</v>
+      </c>
+      <c r="C16" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="68">
+        <v>15</v>
+      </c>
+      <c r="B17" s="97" t="s">
+        <v>574</v>
+      </c>
+      <c r="C17" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="94" t="s">
+        <v>908</v>
+      </c>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="10">
+        <v>16</v>
+      </c>
+      <c r="B18" s="97" t="s">
+        <v>892</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="F18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="68">
+        <v>17</v>
+      </c>
+      <c r="B19" s="81" t="s">
+        <v>893</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="80" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+      <c r="B20" s="81" t="s">
+        <v>894</v>
+      </c>
+      <c r="C20" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
+      <c r="G20" s="99" t="s">
+        <v>946</v>
+      </c>
+      <c r="H20" s="99" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="68">
+        <v>19</v>
+      </c>
+      <c r="B21" s="81" t="s">
+        <v>926</v>
+      </c>
+      <c r="C21" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="F21" s="68">
+        <v>3</v>
+      </c>
+      <c r="G21" s="81" t="s">
+        <v>654</v>
+      </c>
+      <c r="H21" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" s="82" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
+      <c r="B22" s="97" t="s">
+        <v>927</v>
+      </c>
+      <c r="C22" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="81"/>
+      <c r="F22" s="10">
+        <v>4</v>
+      </c>
+      <c r="G22" s="81" t="s">
+        <v>911</v>
+      </c>
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="68">
+        <v>21</v>
+      </c>
+      <c r="B23" s="97" t="s">
+        <v>928</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="81"/>
+      <c r="F23" s="68">
+        <v>5</v>
+      </c>
+      <c r="G23" s="97" t="s">
+        <v>912</v>
+      </c>
+      <c r="H23" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23" s="81"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="97" t="s">
+        <v>929</v>
+      </c>
+      <c r="C24" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="81"/>
+      <c r="F24" s="10">
+        <v>6</v>
+      </c>
+      <c r="G24" s="97" t="s">
+        <v>913</v>
+      </c>
+      <c r="H24" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="81"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="68">
+        <v>23</v>
+      </c>
+      <c r="B25" s="97" t="s">
+        <v>930</v>
+      </c>
+      <c r="C25" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="81"/>
+      <c r="F25" s="68">
+        <v>7</v>
+      </c>
+      <c r="G25" s="97" t="s">
+        <v>914</v>
+      </c>
+      <c r="H25" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="81"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
+      <c r="B26" s="97" t="s">
+        <v>931</v>
+      </c>
+      <c r="C26" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="81"/>
+      <c r="F26" s="10">
+        <v>8</v>
+      </c>
+      <c r="G26" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H26" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="68">
+        <v>25</v>
+      </c>
+      <c r="B27" s="97" t="s">
+        <v>948</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>975</v>
+      </c>
+      <c r="D27" s="81" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="F28" s="5"/>
+      <c r="G28" s="94" t="s">
+        <v>941</v>
+      </c>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="80" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="D31" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="10">
+        <v>2</v>
+      </c>
+      <c r="G31" s="81" t="s">
+        <v>339</v>
+      </c>
+      <c r="H31" s="81" t="s">
+        <v>943</v>
+      </c>
+      <c r="I31" s="82" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="5"/>
+      <c r="B32" s="94" t="s">
+        <v>915</v>
+      </c>
+      <c r="C32" s="94"/>
+      <c r="D32" s="94"/>
+      <c r="F32" s="68">
+        <v>3</v>
+      </c>
+      <c r="G32" s="81" t="s">
+        <v>881</v>
+      </c>
+      <c r="H32" s="81" t="s">
+        <v>944</v>
+      </c>
+      <c r="I32" s="81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="10">
+        <v>4</v>
+      </c>
+      <c r="G33" s="97" t="s">
+        <v>883</v>
+      </c>
+      <c r="H33" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="I33" s="81" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="10">
+        <v>1</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="80" t="s">
+        <v>916</v>
+      </c>
+      <c r="F34" s="68">
+        <v>5</v>
+      </c>
+      <c r="G34" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H34" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="10">
+        <v>2</v>
+      </c>
+      <c r="B35" s="81" t="s">
+        <v>917</v>
+      </c>
+      <c r="C35" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="82" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="68">
+        <v>3</v>
+      </c>
+      <c r="B36" s="81" t="s">
+        <v>918</v>
+      </c>
+      <c r="C36" s="81" t="s">
+        <v>919</v>
+      </c>
+      <c r="D36" s="81" t="s">
+        <v>920</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="94" t="s">
+        <v>953</v>
+      </c>
+      <c r="H36" s="94"/>
+      <c r="I36" s="94"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="10">
+        <v>4</v>
+      </c>
+      <c r="B37" s="97" t="s">
+        <v>921</v>
+      </c>
+      <c r="C37" s="97" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="81" t="s">
+        <v>922</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="68">
+        <v>5</v>
+      </c>
+      <c r="B38" s="97" t="s">
+        <v>923</v>
+      </c>
+      <c r="C38" s="81" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="81" t="s">
+        <v>924</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="80" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45">
+      <c r="A39" s="10">
+        <v>6</v>
+      </c>
+      <c r="B39" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="C39" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>958</v>
+      </c>
+      <c r="F39" s="10">
+        <v>2</v>
+      </c>
+      <c r="G39" s="81" t="s">
+        <v>952</v>
+      </c>
+      <c r="H39" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="I39" s="82" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="5"/>
+      <c r="B40" s="94" t="s">
+        <v>925</v>
+      </c>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="F40" s="10">
+        <v>3</v>
+      </c>
+      <c r="G40" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H40" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="10">
+        <v>1</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="80" t="s">
+        <v>932</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="94" t="s">
+        <v>955</v>
+      </c>
+      <c r="H42" s="94"/>
+      <c r="I42" s="94"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="10">
+        <v>2</v>
+      </c>
+      <c r="B43" s="81" t="s">
+        <v>933</v>
+      </c>
+      <c r="C43" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="82" t="s">
+        <v>934</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="68">
+        <v>3</v>
+      </c>
+      <c r="B44" s="81" t="s">
+        <v>935</v>
+      </c>
+      <c r="C44" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="81" t="s">
+        <v>936</v>
+      </c>
+      <c r="F44" s="10">
+        <v>1</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I44" s="80" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="10">
+        <v>4</v>
+      </c>
+      <c r="B45" s="97" t="s">
+        <v>546</v>
+      </c>
+      <c r="C45" s="97" t="s">
+        <v>903</v>
+      </c>
+      <c r="D45" s="81" t="s">
+        <v>937</v>
+      </c>
+      <c r="F45" s="10">
+        <v>2</v>
+      </c>
+      <c r="G45" s="81" t="s">
+        <v>956</v>
+      </c>
+      <c r="H45" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45" s="82" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="68">
+        <v>5</v>
+      </c>
+      <c r="B46" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="81" t="s">
+        <v>938</v>
+      </c>
+      <c r="F46" s="10">
+        <v>3</v>
+      </c>
+      <c r="G46" s="100" t="s">
+        <v>959</v>
+      </c>
+      <c r="H46" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" s="100" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="10">
+        <v>6</v>
+      </c>
+      <c r="B47" s="97" t="s">
+        <v>939</v>
+      </c>
+      <c r="C47" s="97" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="97" t="s">
+        <v>940</v>
+      </c>
+      <c r="F47" s="10">
+        <v>4</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>970</v>
+      </c>
+      <c r="H47" s="96" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="68">
+        <v>7</v>
+      </c>
+      <c r="B48" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="C48" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="81" t="s">
+        <v>958</v>
+      </c>
+      <c r="F48" s="10">
+        <v>5</v>
+      </c>
+      <c r="G48" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="H48" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="I48" s="97" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="F49" s="10">
+        <v>6</v>
+      </c>
+      <c r="G49" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H49" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I49" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="5"/>
+      <c r="B51" s="98" t="s">
+        <v>976</v>
+      </c>
+      <c r="C51" s="94"/>
+      <c r="D51" s="94"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="94" t="s">
+        <v>962</v>
+      </c>
+      <c r="H51" s="94"/>
+      <c r="I51" s="94"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="10">
+        <v>1</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="80" t="s">
+        <v>977</v>
+      </c>
+      <c r="F53" s="10">
+        <v>1</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H53" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I53" s="80" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="10">
+        <v>2</v>
+      </c>
+      <c r="B54" s="81" t="s">
+        <v>593</v>
+      </c>
+      <c r="C54" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="82" t="s">
+        <v>978</v>
+      </c>
+      <c r="F54" s="10">
+        <v>2</v>
+      </c>
+      <c r="G54" s="81" t="s">
+        <v>956</v>
+      </c>
+      <c r="H54" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="I54" s="82" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="30">
+      <c r="A55" s="10">
+        <v>3</v>
+      </c>
+      <c r="B55" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="82" t="s">
+        <v>347</v>
+      </c>
+      <c r="F55" s="10">
+        <v>3</v>
+      </c>
+      <c r="G55" s="97" t="s">
+        <v>965</v>
+      </c>
+      <c r="H55" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="I55" s="82" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="10">
+        <v>4</v>
+      </c>
+      <c r="B56" s="97" t="s">
+        <v>988</v>
+      </c>
+      <c r="C56" s="97" t="s">
+        <v>989</v>
+      </c>
+      <c r="D56" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="F56" s="10">
+        <v>4</v>
+      </c>
+      <c r="G56" s="97" t="s">
+        <v>967</v>
+      </c>
+      <c r="H56" s="97" t="s">
+        <v>968</v>
+      </c>
+      <c r="I56" s="97" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="10">
+        <v>5</v>
+      </c>
+      <c r="B57" s="100" t="s">
+        <v>990</v>
+      </c>
+      <c r="C57" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" s="100" t="s">
+        <v>991</v>
+      </c>
+      <c r="F57" s="10">
+        <v>5</v>
+      </c>
+      <c r="G57" s="100" t="s">
+        <v>176</v>
+      </c>
+      <c r="H57" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="I57" s="100" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="10">
+        <v>6</v>
+      </c>
+      <c r="B58" s="97" t="s">
+        <v>992</v>
+      </c>
+      <c r="C58" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" s="81" t="s">
+        <v>993</v>
+      </c>
+      <c r="F58" s="10">
+        <v>6</v>
+      </c>
+      <c r="G58" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H58" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I58" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="10">
+        <v>7</v>
+      </c>
+      <c r="B59" s="97" t="s">
+        <v>994</v>
+      </c>
+      <c r="C59" s="97" t="s">
+        <v>989</v>
+      </c>
+      <c r="D59" s="97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="10">
+        <v>8</v>
+      </c>
+      <c r="B60" s="100" t="s">
+        <v>995</v>
+      </c>
+      <c r="C60" s="100" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="100" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="10">
+        <v>9</v>
+      </c>
+      <c r="B61" s="97" t="s">
+        <v>997</v>
+      </c>
+      <c r="C61" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" s="81" t="s">
+        <v>998</v>
+      </c>
+      <c r="F61" s="111"/>
+      <c r="G61" s="112"/>
+      <c r="H61" s="112"/>
+      <c r="I61" s="112"/>
+      <c r="J61" s="96"/>
+      <c r="K61" s="96"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="10">
+        <v>10</v>
+      </c>
+      <c r="B62" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="C62" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="81" t="s">
+        <v>958</v>
+      </c>
+      <c r="F62" s="111"/>
+      <c r="G62" s="111"/>
+      <c r="H62" s="111"/>
+      <c r="I62" s="111"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="E63" s="26"/>
+      <c r="F63" s="113"/>
+      <c r="G63" s="99"/>
+      <c r="H63" s="99"/>
+      <c r="I63" s="114"/>
+      <c r="J63" s="96"/>
+      <c r="K63" s="96"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="5"/>
+      <c r="B65" s="98" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C65" s="94"/>
+      <c r="D65" s="94"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="26"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="115" t="s">
+        <v>74</v>
+      </c>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="10">
+        <v>1</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="80" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E67" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="10">
+        <v>2</v>
+      </c>
+      <c r="B68" s="81" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C68" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="82" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F68" s="5"/>
+      <c r="G68" s="94" t="s">
+        <v>999</v>
+      </c>
+      <c r="H68" s="94"/>
+      <c r="I68" s="94"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="10">
+        <v>3</v>
+      </c>
+      <c r="B69" s="97" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C69" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D69" s="81" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="10">
+        <v>4</v>
+      </c>
+      <c r="B70" s="97" t="s">
+        <v>959</v>
+      </c>
+      <c r="C70" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" s="82" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F70" s="10">
+        <v>1</v>
+      </c>
+      <c r="G70" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H70" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I70" s="80" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="10">
+        <v>5</v>
+      </c>
+      <c r="B71" s="97" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C71" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" s="97"/>
+      <c r="F71" s="10">
+        <v>2</v>
+      </c>
+      <c r="G71" s="81" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H71" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="I71" s="82" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="10">
+        <v>6</v>
+      </c>
+      <c r="B72" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="C72" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" s="81" t="s">
+        <v>958</v>
+      </c>
+      <c r="F72" s="10">
+        <v>3</v>
+      </c>
+      <c r="G72" s="99" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H72" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="I72" s="99" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="F73" s="10">
+        <v>4</v>
+      </c>
+      <c r="G73" s="81" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H73" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="I73" s="82" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="F74" s="10">
+        <v>5</v>
+      </c>
+      <c r="G74" s="97" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H74" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="I74" s="82"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="5"/>
+      <c r="B75" s="94" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C75" s="94"/>
+      <c r="D75" s="94"/>
+      <c r="F75" s="10">
+        <v>6</v>
+      </c>
+      <c r="G75" s="100" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H75" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="I75" s="100" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F76" s="10">
+        <v>7</v>
+      </c>
+      <c r="G76" s="110" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H76" s="110" t="s">
+        <v>134</v>
+      </c>
+      <c r="I76" s="33" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="10">
+        <v>1</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D77" s="80" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G77" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="H77" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="I77" s="81" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="10">
+        <v>2</v>
+      </c>
+      <c r="B78" s="81" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C78" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="82" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="10">
+        <v>3</v>
+      </c>
+      <c r="B79" s="97" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C79" s="97" t="s">
+        <v>950</v>
+      </c>
+      <c r="D79" s="81" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G79" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="10">
+        <v>4</v>
+      </c>
+      <c r="B80" s="97" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C80" s="97" t="s">
+        <v>950</v>
+      </c>
+      <c r="D80" s="81" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G80" s="33" t="s">
+        <v>561</v>
+      </c>
+      <c r="H80" s="102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="10">
+        <v>5</v>
+      </c>
+      <c r="B81" s="97" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C81" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="D81" s="81" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G81" s="33" t="s">
+        <v>562</v>
+      </c>
+      <c r="I81" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="10">
+        <v>6</v>
+      </c>
+      <c r="B82" s="97" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C82" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" s="81"/>
+      <c r="I82" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="10">
+        <v>7</v>
+      </c>
+      <c r="B83" s="97" t="s">
+        <v>911</v>
+      </c>
+      <c r="C83" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D83" s="81"/>
+      <c r="G83" s="33" t="s">
+        <v>979</v>
+      </c>
+      <c r="H83" s="102"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="10">
+        <v>8</v>
+      </c>
+      <c r="B84" s="97" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C84" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D84" s="97" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="10">
+        <v>9</v>
+      </c>
+      <c r="B85" s="97" t="s">
+        <v>956</v>
+      </c>
+      <c r="C85" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D85" s="81" t="s">
+        <v>958</v>
+      </c>
+      <c r="G85" s="101" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="G86" s="33" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="G87" s="33" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="G88" s="33" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="G89" s="33" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="G90" s="33" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="G93" s="33" t="s">
+        <v>986</v>
+      </c>
+      <c r="I93" s="102"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="G94" s="33" t="s">
+        <v>987</v>
+      </c>
+      <c r="I94" s="102"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -5125,26 +7432,26 @@
       <c r="A37" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="98" t="s">
+      <c r="B37" s="108" t="s">
         <v>872</v>
       </c>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="99" t="s">
+      <c r="C37" s="108"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="109" t="s">
         <v>873</v>
       </c>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99" t="s">
+      <c r="F37" s="109"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="109" t="s">
         <v>874</v>
       </c>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="99" t="s">
+      <c r="I37" s="109"/>
+      <c r="J37" s="109"/>
+      <c r="K37" s="109" t="s">
         <v>875</v>
       </c>
-      <c r="L37" s="99"/>
-      <c r="M37" s="99"/>
+      <c r="L37" s="109"/>
+      <c r="M37" s="109"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="81"/>
@@ -5237,15 +7544,15 @@
         <v>42044</v>
       </c>
       <c r="B40" s="81">
-        <f>K39</f>
+        <f t="shared" ref="B40:D42" si="0">K39</f>
         <v>200</v>
       </c>
       <c r="C40" s="81">
-        <f>L39</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D40" s="91">
-        <f>M39</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="E40" s="81">
@@ -5279,15 +7586,15 @@
         <v>42045</v>
       </c>
       <c r="B41" s="81">
-        <f>K40</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="C41" s="92">
-        <f>L40</f>
+        <f t="shared" si="0"/>
         <v>106</v>
       </c>
       <c r="D41" s="91">
-        <f>M40</f>
+        <f t="shared" si="0"/>
         <v>53000</v>
       </c>
       <c r="E41" s="81"/>
@@ -5322,15 +7629,15 @@
         <v>43879</v>
       </c>
       <c r="B42" s="81">
-        <f>K41</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C42" s="92">
-        <f>L41</f>
+        <f t="shared" si="0"/>
         <v>106</v>
       </c>
       <c r="D42" s="89">
-        <f>M41</f>
+        <f t="shared" si="0"/>
         <v>10600</v>
       </c>
       <c r="E42" s="91">
@@ -5705,30 +8012,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -5954,11 +8261,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="93" t="s">
+      <c r="G12" s="103" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -6202,21 +8509,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="93" t="s">
+      <c r="G24" s="103" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="103"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -6364,11 +8671,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="93" t="s">
+      <c r="G33" s="103" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -6620,11 +8927,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="93" t="s">
+      <c r="B45" s="103" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="93"/>
-      <c r="D45" s="93"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="103"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -11710,8 +14017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -11728,19 +14035,19 @@
       <c r="A1" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="105" t="s">
         <v>474</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
       <c r="F1" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="105" t="s">
         <v>476</v>
       </c>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -11876,11 +14183,11 @@
       <c r="F7" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="105" t="s">
         <v>492</v>
       </c>
-      <c r="H7" s="97"/>
-      <c r="I7" s="97"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -12014,11 +14321,11 @@
       <c r="F13" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="G13" s="97" t="s">
+      <c r="G13" s="105" t="s">
         <v>503</v>
       </c>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -12092,11 +14399,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="105" t="s">
         <v>506</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="97"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -12200,19 +14507,19 @@
       <c r="A27" s="53">
         <v>17</v>
       </c>
-      <c r="B27" s="95" t="s">
+      <c r="B27" s="106" t="s">
         <v>514</v>
       </c>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
       <c r="F27" s="54">
         <v>17</v>
       </c>
-      <c r="G27" s="96" t="s">
+      <c r="G27" s="107" t="s">
         <v>515</v>
       </c>
-      <c r="H27" s="96"/>
-      <c r="I27" s="96"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="107"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -12478,19 +14785,19 @@
       <c r="A41" s="53">
         <v>17</v>
       </c>
-      <c r="B41" s="95" t="s">
+      <c r="B41" s="106" t="s">
         <v>538</v>
       </c>
-      <c r="C41" s="95"/>
-      <c r="D41" s="95"/>
+      <c r="C41" s="106"/>
+      <c r="D41" s="106"/>
       <c r="F41" s="54">
         <v>18</v>
       </c>
-      <c r="G41" s="96" t="s">
+      <c r="G41" s="107" t="s">
         <v>539</v>
       </c>
-      <c r="H41" s="96"/>
-      <c r="I41" s="96"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -12760,11 +15067,11 @@
       <c r="A54" s="61">
         <v>2</v>
       </c>
-      <c r="B54" s="97" t="s">
+      <c r="B54" s="105" t="s">
         <v>558</v>
       </c>
-      <c r="C54" s="97"/>
-      <c r="D54" s="97"/>
+      <c r="C54" s="105"/>
+      <c r="D54" s="105"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -13023,6 +15330,9 @@
       </c>
     </row>
     <row r="73" spans="1:4">
+      <c r="A73" s="10">
+        <v>17</v>
+      </c>
       <c r="B73" s="63" t="s">
         <v>593</v>
       </c>
@@ -13035,16 +15345,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="B54:D54"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="B54:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -13056,7 +15366,7 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A45" sqref="A45:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -13077,19 +15387,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="103" t="s">
         <v>595</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="105" t="s">
         <v>596</v>
       </c>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -13277,11 +15587,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="103" t="s">
         <v>614</v>
       </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -13405,11 +15715,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>622</v>
       </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -13623,11 +15933,11 @@
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="93" t="s">
+      <c r="B24" s="103" t="s">
         <v>645</v>
       </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
       <c r="F24" s="10">
         <v>14</v>
       </c>
@@ -13747,11 +16057,11 @@
         <v>655</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="93" t="s">
+      <c r="G29" s="103" t="s">
         <v>656</v>
       </c>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="69">
@@ -14827,19 +17137,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="103" t="s">
         <v>724</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="103" t="s">
         <v>725</v>
       </c>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
@@ -15161,11 +17471,11 @@
       <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>752</v>
       </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
       <c r="F15" s="68">
         <v>13</v>
       </c>
@@ -15486,19 +17796,19 @@
       <c r="A30" s="5">
         <v>4</v>
       </c>
-      <c r="B30" s="93" t="s">
+      <c r="B30" s="103" t="s">
         <v>782</v>
       </c>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="103"/>
       <c r="F30" s="5">
         <v>4</v>
       </c>
-      <c r="G30" s="93" t="s">
+      <c r="G30" s="103" t="s">
         <v>783</v>
       </c>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
@@ -15739,11 +18049,11 @@
       <c r="F41" s="5">
         <v>4</v>
       </c>
-      <c r="G41" s="93" t="s">
+      <c r="G41" s="103" t="s">
         <v>795</v>
       </c>
-      <c r="H41" s="93"/>
-      <c r="I41" s="93"/>
+      <c r="H41" s="103"/>
+      <c r="I41" s="103"/>
     </row>
     <row r="42" spans="1:9">
       <c r="F42" s="9" t="s">
@@ -15763,11 +18073,11 @@
       <c r="A43" s="5">
         <v>4</v>
       </c>
-      <c r="B43" s="93" t="s">
+      <c r="B43" s="103" t="s">
         <v>796</v>
       </c>
-      <c r="C43" s="93"/>
-      <c r="D43" s="93"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="103"/>
       <c r="F43" s="10">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
final update revisi investor
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -21,7 +21,6 @@
     <sheet name="Sheet1" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3171" uniqueCount="1128">
   <si>
     <t>Revisi2</t>
   </si>
@@ -4461,6 +4460,39 @@
   </si>
   <si>
     <t>pengajuan_investasi</t>
+  </si>
+  <si>
+    <t>i_segmen_umkm</t>
+  </si>
+  <si>
+    <t>PK tabel segment umkm yg mau di biayai</t>
+  </si>
+  <si>
+    <t>c_data_lanjutan</t>
+  </si>
+  <si>
+    <t>id_reg_investor</t>
+  </si>
+  <si>
+    <t>nama_data</t>
+  </si>
+  <si>
+    <t>file_data</t>
+  </si>
+  <si>
+    <t>FK c_reg_investor.status_app = 0</t>
+  </si>
+  <si>
+    <t>FK tabel user investor</t>
+  </si>
+  <si>
+    <t>hasil_akhir</t>
+  </si>
+  <si>
+    <t>0 = deal, 1 = no deal</t>
+  </si>
+  <si>
+    <t>tgl_deal</t>
   </si>
 </sst>
 </file>
@@ -4714,7 +4746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4941,12 +4973,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5553,8 +5594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:D64"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -5577,11 +5618,11 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="5"/>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="117" t="s">
         <v>957</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
       <c r="F1" s="5"/>
       <c r="G1" s="91" t="s">
         <v>895</v>
@@ -7763,10 +7804,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -7791,19 +7832,19 @@
       <c r="A1" s="108">
         <v>1</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="122" t="s">
         <v>1081</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
       <c r="F1" s="59">
         <v>2</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="119" t="s">
         <v>1108</v>
       </c>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="109" t="s">
@@ -7968,10 +8009,10 @@
       <c r="F8" s="10">
         <v>6</v>
       </c>
-      <c r="G8" s="111" t="s">
+      <c r="G8" s="110" t="s">
         <v>1083</v>
       </c>
-      <c r="H8" s="111" t="s">
+      <c r="H8" s="110" t="s">
         <v>101</v>
       </c>
     </row>
@@ -8187,14 +8228,14 @@
       <c r="F17" s="10">
         <v>14</v>
       </c>
-      <c r="G17" s="79" t="s">
-        <v>1086</v>
-      </c>
-      <c r="H17" s="79" t="s">
-        <v>1087</v>
-      </c>
-      <c r="I17" s="80" t="s">
-        <v>1088</v>
+      <c r="G17" s="27" t="s">
+        <v>589</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -8211,14 +8252,11 @@
       <c r="F18" s="10">
         <v>15</v>
       </c>
-      <c r="G18" s="27" t="s">
-        <v>589</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>590</v>
+      <c r="G18" s="110" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H18" s="95" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -8235,11 +8273,14 @@
       <c r="F19" s="10">
         <v>16</v>
       </c>
-      <c r="G19" s="111" t="s">
-        <v>1090</v>
-      </c>
-      <c r="H19" s="95" t="s">
+      <c r="G19" s="27" t="s">
+        <v>591</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>101</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -8256,14 +8297,14 @@
       <c r="F20" s="10">
         <v>17</v>
       </c>
-      <c r="G20" s="27" t="s">
-        <v>591</v>
+      <c r="G20" s="111" t="s">
+        <v>1089</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -8279,18 +8320,7 @@
       <c r="D21" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="F21" s="10">
-        <v>18</v>
-      </c>
-      <c r="G21" s="112" t="s">
-        <v>1089</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="27" t="s">
-        <v>594</v>
-      </c>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="10">
@@ -8316,11 +8346,11 @@
       </c>
       <c r="D23" s="95"/>
       <c r="F23" s="109"/>
-      <c r="G23" s="120" t="s">
-        <v>1109</v>
-      </c>
-      <c r="H23" s="120"/>
-      <c r="I23" s="120"/>
+      <c r="G23" s="123" t="s">
+        <v>1117</v>
+      </c>
+      <c r="H23" s="123"/>
+      <c r="I23" s="123"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10">
@@ -8369,7 +8399,7 @@
         <v>284</v>
       </c>
       <c r="I25" s="79" t="s">
-        <v>1092</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -8388,14 +8418,14 @@
       <c r="F26" s="10">
         <v>2</v>
       </c>
-      <c r="G26" s="79" t="s">
-        <v>1093</v>
-      </c>
-      <c r="H26" s="79" t="s">
-        <v>307</v>
-      </c>
-      <c r="I26" s="79" t="s">
-        <v>1094</v>
+      <c r="G26" s="95" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H26" s="95" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I26" s="115" t="s">
+        <v>1088</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -8414,28 +8444,28 @@
       <c r="F27" s="10">
         <v>3</v>
       </c>
-      <c r="G27" s="79" t="s">
-        <v>1095</v>
-      </c>
-      <c r="H27" s="79" t="s">
-        <v>943</v>
-      </c>
-      <c r="I27" s="79" t="s">
-        <v>1096</v>
+      <c r="G27" s="95" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H27" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="95" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="F28" s="10">
         <v>4</v>
       </c>
-      <c r="G28" s="79" t="s">
-        <v>1097</v>
-      </c>
-      <c r="H28" s="79" t="s">
-        <v>122</v>
-      </c>
-      <c r="I28" s="79" t="s">
-        <v>1098</v>
+      <c r="G28" s="111" t="s">
+        <v>1089</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -8445,18 +8475,10 @@
       </c>
       <c r="C29" s="106"/>
       <c r="D29" s="106"/>
-      <c r="F29" s="10">
-        <v>5</v>
-      </c>
-      <c r="G29" s="79" t="s">
-        <v>1099</v>
-      </c>
-      <c r="H29" s="79" t="s">
-        <v>112</v>
-      </c>
-      <c r="I29" s="79" t="s">
-        <v>1100</v>
-      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="9" t="s">
@@ -8471,18 +8493,12 @@
       <c r="D30" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="10">
-        <v>6</v>
-      </c>
-      <c r="G30" s="95" t="s">
-        <v>1101</v>
-      </c>
-      <c r="H30" s="95" t="s">
-        <v>1102</v>
-      </c>
-      <c r="I30" s="95" t="s">
-        <v>1103</v>
-      </c>
+      <c r="F30" s="109"/>
+      <c r="G30" s="114" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H30" s="114"/>
+      <c r="I30" s="114"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="10">
@@ -8497,17 +8513,17 @@
       <c r="D31" s="78" t="s">
         <v>1112</v>
       </c>
-      <c r="F31" s="10">
-        <v>7</v>
-      </c>
-      <c r="G31" s="95" t="s">
-        <v>1104</v>
-      </c>
-      <c r="H31" s="95" t="s">
-        <v>108</v>
-      </c>
-      <c r="I31" s="95" t="s">
-        <v>1105</v>
+      <c r="F31" s="109" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="109" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="109" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="109" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -8524,16 +8540,16 @@
         <v>975</v>
       </c>
       <c r="F32" s="10">
-        <v>8</v>
-      </c>
-      <c r="G32" s="95" t="s">
-        <v>1106</v>
-      </c>
-      <c r="H32" s="95" t="s">
-        <v>219</v>
-      </c>
-      <c r="I32" s="113" t="s">
-        <v>1107</v>
+        <v>1</v>
+      </c>
+      <c r="G32" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" s="79" t="s">
+        <v>284</v>
+      </c>
+      <c r="I32" s="79" t="s">
+        <v>1092</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -8550,16 +8566,16 @@
         <v>347</v>
       </c>
       <c r="F33" s="10">
-        <v>9</v>
-      </c>
-      <c r="G33" s="95" t="s">
-        <v>1035</v>
-      </c>
-      <c r="H33" s="95" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="95" t="s">
-        <v>1110</v>
+        <v>2</v>
+      </c>
+      <c r="G33" s="79" t="s">
+        <v>1093</v>
+      </c>
+      <c r="H33" s="79" t="s">
+        <v>307</v>
+      </c>
+      <c r="I33" s="79" t="s">
+        <v>1094</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -8576,16 +8592,16 @@
         <v>123</v>
       </c>
       <c r="F34" s="10">
-        <v>10</v>
-      </c>
-      <c r="G34" s="112" t="s">
-        <v>1089</v>
-      </c>
-      <c r="H34" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I34" s="27" t="s">
-        <v>594</v>
+        <v>3</v>
+      </c>
+      <c r="G34" s="79" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H34" s="79" t="s">
+        <v>943</v>
+      </c>
+      <c r="I34" s="79" t="s">
+        <v>1096</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -8601,7 +8617,18 @@
       <c r="D35" s="98" t="s">
         <v>1114</v>
       </c>
-      <c r="F35" s="110"/>
+      <c r="F35" s="10">
+        <v>4</v>
+      </c>
+      <c r="G35" s="79" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H35" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="I35" s="79" t="s">
+        <v>1098</v>
+      </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="10">
@@ -8616,6 +8643,18 @@
       <c r="D36" s="79" t="s">
         <v>1115</v>
       </c>
+      <c r="F36" s="10">
+        <v>5</v>
+      </c>
+      <c r="G36" s="79" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H36" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="I36" s="79" t="s">
+        <v>1100</v>
+      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="10">
@@ -8630,6 +8669,18 @@
       <c r="D37" s="95" t="s">
         <v>123</v>
       </c>
+      <c r="F37" s="10">
+        <v>6</v>
+      </c>
+      <c r="G37" s="95" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H37" s="95" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I37" s="95" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="10">
@@ -8644,6 +8695,18 @@
       <c r="D38" s="98" t="s">
         <v>993</v>
       </c>
+      <c r="F38" s="10">
+        <v>7</v>
+      </c>
+      <c r="G38" s="95" t="s">
+        <v>1104</v>
+      </c>
+      <c r="H38" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="95" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="10">
@@ -8658,32 +8721,259 @@
       <c r="D39" s="79" t="s">
         <v>995</v>
       </c>
+      <c r="F39" s="10">
+        <v>8</v>
+      </c>
+      <c r="G39" s="95" t="s">
+        <v>1106</v>
+      </c>
+      <c r="H39" s="95" t="s">
+        <v>219</v>
+      </c>
+      <c r="I39" s="112" t="s">
+        <v>1107</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="10">
         <v>10</v>
       </c>
-      <c r="B40" s="95" t="s">
-        <v>956</v>
-      </c>
-      <c r="C40" s="95" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="79" t="s">
-        <v>958</v>
+      <c r="B40" s="101" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C40" s="101" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="101" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F40" s="10">
+        <v>9</v>
+      </c>
+      <c r="G40" s="95" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H40" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="95" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="15"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
+      <c r="A41" s="10">
+        <v>11</v>
+      </c>
+      <c r="B41" s="101" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C41" s="95" t="s">
+        <v>986</v>
+      </c>
+      <c r="D41" s="95" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" s="10">
+        <v>10</v>
+      </c>
+      <c r="G41" s="111" t="s">
+        <v>1089</v>
+      </c>
+      <c r="H41" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="79" t="s">
+        <v>1124</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="15"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
+      <c r="A42" s="10">
+        <v>12</v>
+      </c>
+      <c r="B42" s="95" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C42" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="95" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="10">
+        <v>13</v>
+      </c>
+      <c r="B43" s="111" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="79" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="G45" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="5"/>
+      <c r="B46" s="113" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C46" s="113"/>
+      <c r="D46" s="113"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="10">
+        <v>1</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="78" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="10">
+        <v>2</v>
+      </c>
+      <c r="B49" s="79" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C49" s="79" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="80" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="10">
+        <v>3</v>
+      </c>
+      <c r="B50" s="95" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C50" s="95" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="80"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="10">
+        <v>4</v>
+      </c>
+      <c r="B51" s="95" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C51" s="95" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" s="95" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="10">
+        <v>5</v>
+      </c>
+      <c r="B52" s="95" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C52" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="95" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="10">
+        <v>6</v>
+      </c>
+      <c r="B53" s="111" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="79" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="15">
+        <v>7</v>
+      </c>
+      <c r="B54" s="94"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="26"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="15">
+        <v>8</v>
+      </c>
+      <c r="B55" s="116"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="116"/>
+      <c r="E55" s="26"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="15">
+        <v>9</v>
+      </c>
+      <c r="B56" s="94"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="15">
+        <v>10</v>
+      </c>
+      <c r="B57" s="94"/>
+      <c r="C57" s="94"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9073,26 +9363,26 @@
       <c r="A37" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="121" t="s">
+      <c r="B37" s="124" t="s">
         <v>872</v>
       </c>
-      <c r="C37" s="121"/>
-      <c r="D37" s="121"/>
-      <c r="E37" s="122" t="s">
+      <c r="C37" s="124"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125" t="s">
         <v>873</v>
       </c>
-      <c r="F37" s="122"/>
-      <c r="G37" s="122"/>
-      <c r="H37" s="122" t="s">
+      <c r="F37" s="125"/>
+      <c r="G37" s="125"/>
+      <c r="H37" s="125" t="s">
         <v>874</v>
       </c>
-      <c r="I37" s="122"/>
-      <c r="J37" s="122"/>
-      <c r="K37" s="122" t="s">
+      <c r="I37" s="125"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="125" t="s">
         <v>875</v>
       </c>
-      <c r="L37" s="122"/>
-      <c r="M37" s="122"/>
+      <c r="L37" s="125"/>
+      <c r="M37" s="125"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="79"/>
@@ -9653,30 +9943,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -9902,11 +10192,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="114" t="s">
+      <c r="G12" s="117" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="117"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -10150,21 +10440,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="114" t="s">
+      <c r="G24" s="117" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="114" t="s">
+      <c r="B25" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="114"/>
-      <c r="D25" s="114"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="117"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -10312,11 +10602,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="114" t="s">
+      <c r="G33" s="117" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="114"/>
-      <c r="I33" s="114"/>
+      <c r="H33" s="117"/>
+      <c r="I33" s="117"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -10568,11 +10858,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="114" t="s">
+      <c r="B45" s="117" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
+      <c r="C45" s="117"/>
+      <c r="D45" s="117"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -15677,19 +15967,19 @@
       <c r="A1" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="119" t="s">
         <v>474</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
       <c r="F1" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="119" t="s">
         <v>476</v>
       </c>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -15825,11 +16115,11 @@
       <c r="F7" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="G7" s="116" t="s">
+      <c r="G7" s="119" t="s">
         <v>492</v>
       </c>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -15963,11 +16253,11 @@
       <c r="F13" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="G13" s="116" t="s">
+      <c r="G13" s="119" t="s">
         <v>503</v>
       </c>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="119"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -16041,11 +16331,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="119" t="s">
         <v>506</v>
       </c>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -16149,19 +16439,19 @@
       <c r="A27" s="53">
         <v>17</v>
       </c>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="120" t="s">
         <v>514</v>
       </c>
-      <c r="C27" s="117"/>
-      <c r="D27" s="117"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
       <c r="F27" s="54">
         <v>17</v>
       </c>
-      <c r="G27" s="118" t="s">
+      <c r="G27" s="121" t="s">
         <v>515</v>
       </c>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
+      <c r="H27" s="121"/>
+      <c r="I27" s="121"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -16429,19 +16719,19 @@
       <c r="A41" s="53">
         <v>17</v>
       </c>
-      <c r="B41" s="117" t="s">
+      <c r="B41" s="120" t="s">
         <v>538</v>
       </c>
-      <c r="C41" s="117"/>
-      <c r="D41" s="117"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
       <c r="F41" s="54">
         <v>18</v>
       </c>
-      <c r="G41" s="118" t="s">
+      <c r="G41" s="121" t="s">
         <v>539</v>
       </c>
-      <c r="H41" s="118"/>
-      <c r="I41" s="118"/>
+      <c r="H41" s="121"/>
+      <c r="I41" s="121"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -16711,11 +17001,11 @@
       <c r="A54" s="59">
         <v>2</v>
       </c>
-      <c r="B54" s="116" t="s">
+      <c r="B54" s="119" t="s">
         <v>558</v>
       </c>
-      <c r="C54" s="116"/>
-      <c r="D54" s="116"/>
+      <c r="C54" s="119"/>
+      <c r="D54" s="119"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -17031,19 +17321,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="117" t="s">
         <v>595</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="119" t="s">
         <v>596</v>
       </c>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -17231,11 +17521,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="114" t="s">
+      <c r="G9" s="117" t="s">
         <v>614</v>
       </c>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="117"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -17359,11 +17649,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="117" t="s">
         <v>622</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -17577,11 +17867,11 @@
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="114" t="s">
+      <c r="B24" s="117" t="s">
         <v>645</v>
       </c>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="117"/>
       <c r="F24" s="10">
         <v>14</v>
       </c>
@@ -17701,11 +17991,11 @@
         <v>655</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="114" t="s">
+      <c r="G29" s="117" t="s">
         <v>656</v>
       </c>
-      <c r="H29" s="114"/>
-      <c r="I29" s="114"/>
+      <c r="H29" s="117"/>
+      <c r="I29" s="117"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="67">
@@ -18781,19 +19071,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="117" t="s">
         <v>724</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="117" t="s">
         <v>725</v>
       </c>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
@@ -19115,11 +19405,11 @@
       <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="117" t="s">
         <v>752</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
       <c r="F15" s="66">
         <v>13</v>
       </c>
@@ -19440,19 +19730,19 @@
       <c r="A30" s="5">
         <v>4</v>
       </c>
-      <c r="B30" s="114" t="s">
+      <c r="B30" s="117" t="s">
         <v>782</v>
       </c>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
       <c r="F30" s="5">
         <v>4</v>
       </c>
-      <c r="G30" s="114" t="s">
+      <c r="G30" s="117" t="s">
         <v>783</v>
       </c>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
+      <c r="H30" s="117"/>
+      <c r="I30" s="117"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
@@ -19693,11 +19983,11 @@
       <c r="F41" s="5">
         <v>4</v>
       </c>
-      <c r="G41" s="114" t="s">
+      <c r="G41" s="117" t="s">
         <v>795</v>
       </c>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
+      <c r="H41" s="117"/>
+      <c r="I41" s="117"/>
     </row>
     <row r="42" spans="1:9">
       <c r="F42" s="9" t="s">
@@ -19717,11 +20007,11 @@
       <c r="A43" s="5">
         <v>4</v>
       </c>
-      <c r="B43" s="114" t="s">
+      <c r="B43" s="117" t="s">
         <v>796</v>
       </c>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="117"/>
       <c r="F43" s="10">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
reivi tambah stok per gudang
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Sheet13" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="1252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3639" uniqueCount="1284">
   <si>
     <t>Revisi2</t>
   </si>
@@ -4935,6 +4936,102 @@
   </si>
   <si>
     <t>FK p_komisi_sales.id_ky, nullable</t>
+  </si>
+  <si>
+    <t>p_gudang</t>
+  </si>
+  <si>
+    <t>PK tabel gudang</t>
+  </si>
+  <si>
+    <t>nama_gudang</t>
+  </si>
+  <si>
+    <t>p_masuk_gudang</t>
+  </si>
+  <si>
+    <t>PK tabel barang masuk gudang</t>
+  </si>
+  <si>
+    <t>tgl brg masuk gudang</t>
+  </si>
+  <si>
+    <t>int(11)</t>
+  </si>
+  <si>
+    <t>nama_pengirim</t>
+  </si>
+  <si>
+    <t>pengirim brg</t>
+  </si>
+  <si>
+    <t>nama_penerima</t>
+  </si>
+  <si>
+    <t>FK p_karyawan</t>
+  </si>
+  <si>
+    <t>p_keluar_gudang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes: data p_gudang tidak bisa di edit status gudangnya dan tdk bisa di hapus datanya </t>
+  </si>
+  <si>
+    <t>tgl brg keluar gudang</t>
+  </si>
+  <si>
+    <t>jumlah barang keluar</t>
+  </si>
+  <si>
+    <t>jumlah barang masuk</t>
+  </si>
+  <si>
+    <t>FK karyawan</t>
+  </si>
+  <si>
+    <t>p_detail_keluar_gudang</t>
+  </si>
+  <si>
+    <t>p_detail_masuk_gudang</t>
+  </si>
+  <si>
+    <t>id_masuk_gudang</t>
+  </si>
+  <si>
+    <t>FK p_masuk_gudang</t>
+  </si>
+  <si>
+    <t>id_gudang</t>
+  </si>
+  <si>
+    <t>FK p_gudang</t>
+  </si>
+  <si>
+    <t>gudang_asal</t>
+  </si>
+  <si>
+    <t>gudang_tujuan</t>
+  </si>
+  <si>
+    <t>FK gudang</t>
+  </si>
+  <si>
+    <t>p_stok_gudang</t>
+  </si>
+  <si>
+    <t>id_keluar_gudang</t>
+  </si>
+  <si>
+    <t>nama gudang, Gudang A, Gudang B, dst</t>
+  </si>
+  <si>
+    <t>jenis_gudang</t>
+  </si>
+  <si>
+    <t>0 = gudang penyimpanan, 1 = showroom penjualan, default 0. jenis_gudang = 1, unik / hnya satu data</t>
+  </si>
+  <si>
+    <t>tambahan baru</t>
   </si>
 </sst>
 </file>
@@ -5010,7 +5107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5062,6 +5159,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5227,7 +5330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5485,6 +5588,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5497,14 +5609,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5533,8 +5642,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6137,19 +6247,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="138" t="s">
         <v>756</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="135" t="s">
+      <c r="G1" s="138" t="s">
         <v>757</v>
       </c>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
@@ -6471,11 +6581,11 @@
       <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="138" t="s">
         <v>784</v>
       </c>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
       <c r="F15" s="59">
         <v>13</v>
       </c>
@@ -6796,19 +6906,19 @@
       <c r="A30" s="5">
         <v>4</v>
       </c>
-      <c r="B30" s="135" t="s">
+      <c r="B30" s="138" t="s">
         <v>814</v>
       </c>
-      <c r="C30" s="135"/>
-      <c r="D30" s="135"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
       <c r="F30" s="5">
         <v>4</v>
       </c>
-      <c r="G30" s="135" t="s">
+      <c r="G30" s="138" t="s">
         <v>815</v>
       </c>
-      <c r="H30" s="135"/>
-      <c r="I30" s="135"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="138"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
@@ -7049,11 +7159,11 @@
       <c r="F41" s="5">
         <v>4</v>
       </c>
-      <c r="G41" s="135" t="s">
+      <c r="G41" s="138" t="s">
         <v>827</v>
       </c>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
+      <c r="H41" s="138"/>
+      <c r="I41" s="138"/>
     </row>
     <row r="42" spans="1:9">
       <c r="F42" s="9" t="s">
@@ -7073,11 +7183,11 @@
       <c r="A43" s="5">
         <v>4</v>
       </c>
-      <c r="B43" s="135" t="s">
+      <c r="B43" s="138" t="s">
         <v>828</v>
       </c>
-      <c r="C43" s="135"/>
-      <c r="D43" s="135"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="138"/>
       <c r="F43" s="10">
         <v>1</v>
       </c>
@@ -7396,11 +7506,11 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="5"/>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="138" t="s">
         <v>838</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="F1" s="5"/>
       <c r="G1" s="8" t="s">
         <v>839</v>
@@ -9837,19 +9947,19 @@
       <c r="A1" s="69">
         <v>1</v>
       </c>
-      <c r="B1" s="139" t="s">
+      <c r="B1" s="143" t="s">
         <v>1038</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="F1" s="53">
         <v>2</v>
       </c>
-      <c r="G1" s="132" t="s">
+      <c r="G1" s="137" t="s">
         <v>1039</v>
       </c>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -10351,11 +10461,11 @@
       </c>
       <c r="D23" s="11"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="135" t="s">
+      <c r="G23" s="138" t="s">
         <v>1056</v>
       </c>
-      <c r="H23" s="135"/>
-      <c r="I23" s="135"/>
+      <c r="H23" s="138"/>
+      <c r="I23" s="138"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10">
@@ -11376,26 +11486,26 @@
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="140" t="s">
+      <c r="B37" s="144" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="140"/>
-      <c r="D37" s="140"/>
-      <c r="E37" s="141" t="s">
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="145" t="s">
         <v>1144</v>
       </c>
-      <c r="F37" s="141"/>
-      <c r="G37" s="141"/>
-      <c r="H37" s="142" t="s">
+      <c r="F37" s="145"/>
+      <c r="G37" s="145"/>
+      <c r="H37" s="146" t="s">
         <v>1145</v>
       </c>
-      <c r="I37" s="142"/>
-      <c r="J37" s="142"/>
-      <c r="K37" s="142" t="s">
+      <c r="I37" s="146"/>
+      <c r="J37" s="146"/>
+      <c r="K37" s="146" t="s">
         <v>1146</v>
       </c>
-      <c r="L37" s="142"/>
-      <c r="M37" s="142"/>
+      <c r="L37" s="146"/>
+      <c r="M37" s="146"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="11"/>
@@ -11781,13 +11891,13 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="143" t="s">
+      <c r="A62" s="147" t="s">
         <v>1156</v>
       </c>
-      <c r="B62" s="143"/>
-      <c r="C62" s="143"/>
-      <c r="D62" s="143"/>
-      <c r="E62" s="143"/>
+      <c r="B62" s="147"/>
+      <c r="C62" s="147"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="147"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="89"/>
@@ -11991,13 +12101,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="148" t="s">
         <v>1156</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="98"/>
@@ -12179,13 +12289,13 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="148" t="s">
         <v>1156</v>
       </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="144"/>
+      <c r="B17" s="148"/>
+      <c r="C17" s="148"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="148"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="98"/>
@@ -12620,34 +12730,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="134" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="114">
         <v>1</v>
       </c>
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="136" t="s">
         <v>1206</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
       <c r="F2" s="101">
         <v>2</v>
       </c>
-      <c r="G2" s="132" t="s">
+      <c r="G2" s="137" t="s">
         <v>1234</v>
       </c>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="115" t="s">
@@ -13124,30 +13234,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="138" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="135" t="s">
+      <c r="G2" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -13373,11 +13483,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="135" t="s">
+      <c r="G12" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="135"/>
-      <c r="I12" s="135"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -13621,21 +13731,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="135" t="s">
+      <c r="G24" s="138" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="135"/>
-      <c r="I24" s="135"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="135" t="s">
+      <c r="B25" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="135"/>
-      <c r="D25" s="135"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -13783,11 +13893,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="135" t="s">
+      <c r="G33" s="138" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="135"/>
-      <c r="I33" s="135"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="138"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -14039,11 +14149,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="135" t="s">
+      <c r="B45" s="138" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="135"/>
-      <c r="D45" s="135"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="138"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -14327,19 +14437,19 @@
       <c r="A60" s="5">
         <v>13</v>
       </c>
-      <c r="B60" s="135" t="s">
+      <c r="B60" s="138" t="s">
         <v>1185</v>
       </c>
-      <c r="C60" s="135"/>
-      <c r="D60" s="135"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="138"/>
       <c r="F60" s="5">
         <v>14</v>
       </c>
-      <c r="G60" s="135" t="s">
+      <c r="G60" s="138" t="s">
         <v>1186</v>
       </c>
-      <c r="H60" s="135"/>
-      <c r="I60" s="135"/>
+      <c r="H60" s="138"/>
+      <c r="I60" s="138"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="9" t="s">
@@ -14626,16 +14736,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G24:I24"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="G60:I60"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="G33:I33"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14644,10 +14754,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="B97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -14655,8 +14765,8 @@
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
@@ -16000,7 +16110,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="60">
+    <row r="58" spans="1:9" ht="45">
       <c r="A58" s="10">
         <v>6</v>
       </c>
@@ -16152,7 +16262,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="60">
+    <row r="64" spans="1:9" ht="45">
       <c r="A64" s="10">
         <v>12</v>
       </c>
@@ -16355,7 +16465,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="135">
+    <row r="73" spans="1:11" ht="120">
       <c r="A73" s="30">
         <v>2</v>
       </c>
@@ -16745,9 +16855,529 @@
         <v>99</v>
       </c>
     </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="15"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="B91" s="149" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C91" s="149"/>
+      <c r="D91" s="149"/>
+      <c r="E91" s="149"/>
+      <c r="F91" s="149"/>
+      <c r="G91" s="149"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="5">
+        <v>13</v>
+      </c>
+      <c r="B92" s="35" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C92" s="34"/>
+      <c r="D92" s="34"/>
+      <c r="F92" s="5">
+        <v>15</v>
+      </c>
+      <c r="G92" s="35" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H92" s="34"/>
+      <c r="I92" s="34"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="B93" s="129" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" s="129" t="s">
+        <v>73</v>
+      </c>
+      <c r="D93" s="129" t="s">
+        <v>74</v>
+      </c>
+      <c r="F93" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="G93" s="129" t="s">
+        <v>72</v>
+      </c>
+      <c r="H93" s="129" t="s">
+        <v>73</v>
+      </c>
+      <c r="I93" s="129" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="10">
+        <v>1</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D94" s="103" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F94" s="10">
+        <v>1</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I94" s="103" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="10">
+        <v>2</v>
+      </c>
+      <c r="B95" s="98" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C95" s="98" t="s">
+        <v>101</v>
+      </c>
+      <c r="D95" s="98" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F95" s="10">
+        <v>2</v>
+      </c>
+      <c r="G95" s="98" t="s">
+        <v>1178</v>
+      </c>
+      <c r="H95" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="I95" s="98" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="30">
+      <c r="A96" s="10">
+        <v>3</v>
+      </c>
+      <c r="B96" s="106" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C96" s="106" t="s">
+        <v>134</v>
+      </c>
+      <c r="D96" s="107" t="s">
+        <v>1282</v>
+      </c>
+      <c r="F96" s="10">
+        <v>3</v>
+      </c>
+      <c r="G96" s="116" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H96" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="I96" s="98" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="10">
+        <v>4</v>
+      </c>
+      <c r="B97" s="116" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="108"/>
+      <c r="D97" s="98"/>
+      <c r="F97" s="10">
+        <v>4</v>
+      </c>
+      <c r="G97" s="116" t="s">
+        <v>1261</v>
+      </c>
+      <c r="H97" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="I97" s="98" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="10">
+        <v>5</v>
+      </c>
+      <c r="B98" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="C98" s="116"/>
+      <c r="D98" s="98"/>
+      <c r="F98" s="10">
+        <v>5</v>
+      </c>
+      <c r="G98" s="112" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H98" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="I98" s="112" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="10"/>
+      <c r="C99" s="116"/>
+      <c r="D99" s="98"/>
+      <c r="F99" s="10">
+        <v>6</v>
+      </c>
+      <c r="G99" s="112" t="s">
+        <v>1276</v>
+      </c>
+      <c r="H99" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="I99" s="112" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="10"/>
+      <c r="C100" s="98"/>
+      <c r="D100" s="98"/>
+      <c r="E100" t="s">
+        <v>110</v>
+      </c>
+      <c r="F100" s="10">
+        <v>7</v>
+      </c>
+      <c r="G100" s="116" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="B101" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E101" s="25"/>
+      <c r="F101" s="10">
+        <v>8</v>
+      </c>
+      <c r="G101" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="H101" s="116"/>
+      <c r="I101" s="98"/>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="F103" s="98"/>
+      <c r="G103" s="132" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H103" s="98"/>
+      <c r="I103" s="98"/>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="5">
+        <v>14</v>
+      </c>
+      <c r="B104" s="35" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C104" s="34"/>
+      <c r="D104" s="34"/>
+      <c r="F104" s="10">
+        <v>1</v>
+      </c>
+      <c r="G104" t="s">
+        <v>75</v>
+      </c>
+      <c r="H104" s="98" t="s">
+        <v>337</v>
+      </c>
+      <c r="I104" s="98" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="B105" s="129" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" s="129" t="s">
+        <v>73</v>
+      </c>
+      <c r="D105" s="129" t="s">
+        <v>74</v>
+      </c>
+      <c r="F105" s="10">
+        <v>2</v>
+      </c>
+      <c r="G105" s="98" t="s">
+        <v>1279</v>
+      </c>
+      <c r="H105" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="I105" s="98" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="10">
+        <v>1</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D106" s="103" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F106" s="10">
+        <v>3</v>
+      </c>
+      <c r="G106" s="116" t="s">
+        <v>143</v>
+      </c>
+      <c r="H106" s="98" t="s">
+        <v>337</v>
+      </c>
+      <c r="I106" s="98" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="10">
+        <v>2</v>
+      </c>
+      <c r="B107" s="98" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C107" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="D107" s="98" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F107" s="10">
+        <v>4</v>
+      </c>
+      <c r="G107" s="98" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H107" s="116" t="s">
+        <v>1258</v>
+      </c>
+      <c r="I107" s="98" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="10">
+        <v>3</v>
+      </c>
+      <c r="B108" s="116" t="s">
+        <v>206</v>
+      </c>
+      <c r="C108" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="D108" s="98" t="s">
+        <v>344</v>
+      </c>
+      <c r="G108" s="116"/>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="10">
+        <v>4</v>
+      </c>
+      <c r="B109" s="106" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C109" s="106" t="s">
+        <v>76</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" s="10">
+        <v>5</v>
+      </c>
+      <c r="B110" s="116" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C110" s="116" t="s">
+        <v>112</v>
+      </c>
+      <c r="D110" s="98" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F110" s="98"/>
+      <c r="G110" s="132" t="s">
+        <v>1278</v>
+      </c>
+      <c r="H110" s="98"/>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" s="10">
+        <v>6</v>
+      </c>
+      <c r="B111" s="116" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C111" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="D111" s="98" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F111" s="10">
+        <v>1</v>
+      </c>
+      <c r="G111" s="98" t="s">
+        <v>75</v>
+      </c>
+      <c r="H111" s="98" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" s="10">
+        <v>7</v>
+      </c>
+      <c r="B112" s="116" t="s">
+        <v>94</v>
+      </c>
+      <c r="C112" s="98"/>
+      <c r="D112" s="98"/>
+      <c r="F112" s="10">
+        <v>2</v>
+      </c>
+      <c r="G112" s="116" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H112" s="116" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="B113" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="C113" s="98"/>
+      <c r="D113" s="98"/>
+      <c r="F113" s="10">
+        <v>3</v>
+      </c>
+      <c r="G113" s="98" t="s">
+        <v>143</v>
+      </c>
+      <c r="H113" s="98" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="F114" s="10">
+        <v>4</v>
+      </c>
+      <c r="G114" s="116" t="s">
+        <v>128</v>
+      </c>
+      <c r="H114" s="116" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="98"/>
+      <c r="B115" s="132" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C115" s="98"/>
+      <c r="D115" s="98"/>
+      <c r="G115" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="10">
+        <v>1</v>
+      </c>
+      <c r="B116" s="98" t="s">
+        <v>75</v>
+      </c>
+      <c r="C116" s="98" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D116" s="98"/>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="10">
+        <v>2</v>
+      </c>
+      <c r="B117" s="98" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C117" s="98" t="s">
+        <v>337</v>
+      </c>
+      <c r="D117" s="98" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="10">
+        <v>3</v>
+      </c>
+      <c r="B118" s="98" t="s">
+        <v>143</v>
+      </c>
+      <c r="C118" s="98" t="s">
+        <v>337</v>
+      </c>
+      <c r="D118" s="98" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="10">
+        <v>4</v>
+      </c>
+      <c r="B119" s="116" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C119" s="116" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D119" s="98" t="s">
+        <v>1267</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B91:G91"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16755,7 +17385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
@@ -17862,13 +18492,13 @@
       <c r="A50" s="10">
         <v>17</v>
       </c>
-      <c r="B50" s="145" t="s">
+      <c r="B50" s="130" t="s">
         <v>398</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="146" t="s">
+      <c r="D50" s="131" t="s">
         <v>1251</v>
       </c>
       <c r="F50" s="10">
@@ -19218,12 +19848,12 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="136" t="s">
+      <c r="A115" s="140" t="s">
         <v>1205</v>
       </c>
-      <c r="B115" s="136"/>
-      <c r="C115" s="136"/>
-      <c r="D115" s="136"/>
+      <c r="B115" s="140"/>
+      <c r="C115" s="140"/>
+      <c r="D115" s="140"/>
       <c r="E115" s="3" t="s">
         <v>110</v>
       </c>
@@ -19244,11 +19874,11 @@
       <c r="A116" s="101">
         <v>1</v>
       </c>
-      <c r="B116" s="132" t="s">
+      <c r="B116" s="137" t="s">
         <v>1202</v>
       </c>
-      <c r="C116" s="132"/>
-      <c r="D116" s="132"/>
+      <c r="C116" s="137"/>
+      <c r="D116" s="137"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="101" t="s">
@@ -19805,19 +20435,19 @@
       <c r="A1" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="137" t="s">
         <v>510</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
       <c r="F1" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="G1" s="132" t="s">
+      <c r="G1" s="137" t="s">
         <v>512</v>
       </c>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -19953,11 +20583,11 @@
       <c r="F7" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G7" s="132" t="s">
+      <c r="G7" s="137" t="s">
         <v>528</v>
       </c>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
+      <c r="H7" s="137"/>
+      <c r="I7" s="137"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -20091,11 +20721,11 @@
       <c r="F13" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G13" s="132" t="s">
+      <c r="G13" s="137" t="s">
         <v>539</v>
       </c>
-      <c r="H13" s="132"/>
-      <c r="I13" s="132"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -20169,11 +20799,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="132" t="s">
+      <c r="B18" s="137" t="s">
         <v>542</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="D18" s="132"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -20277,19 +20907,19 @@
       <c r="A27" s="48">
         <v>17</v>
       </c>
-      <c r="B27" s="137" t="s">
+      <c r="B27" s="141" t="s">
         <v>550</v>
       </c>
-      <c r="C27" s="137"/>
-      <c r="D27" s="137"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
       <c r="F27" s="49">
         <v>17</v>
       </c>
-      <c r="G27" s="138" t="s">
+      <c r="G27" s="142" t="s">
         <v>551</v>
       </c>
-      <c r="H27" s="138"/>
-      <c r="I27" s="138"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -20557,19 +21187,19 @@
       <c r="A41" s="48">
         <v>17</v>
       </c>
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="141" t="s">
         <v>574</v>
       </c>
-      <c r="C41" s="137"/>
-      <c r="D41" s="137"/>
+      <c r="C41" s="141"/>
+      <c r="D41" s="141"/>
       <c r="F41" s="49">
         <v>18</v>
       </c>
-      <c r="G41" s="138" t="s">
+      <c r="G41" s="142" t="s">
         <v>575</v>
       </c>
-      <c r="H41" s="138"/>
-      <c r="I41" s="138"/>
+      <c r="H41" s="142"/>
+      <c r="I41" s="142"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -20839,11 +21469,11 @@
       <c r="A54" s="53">
         <v>2</v>
       </c>
-      <c r="B54" s="132" t="s">
+      <c r="B54" s="137" t="s">
         <v>594</v>
       </c>
-      <c r="C54" s="132"/>
-      <c r="D54" s="132"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="137"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -21117,16 +21747,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="B54:D54"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="B54:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21159,19 +21789,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="138" t="s">
         <v>631</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="132" t="s">
+      <c r="G1" s="137" t="s">
         <v>632</v>
       </c>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -21359,11 +21989,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="135" t="s">
+      <c r="G9" s="138" t="s">
         <v>650</v>
       </c>
-      <c r="H9" s="135"/>
-      <c r="I9" s="135"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -21487,11 +22117,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="138" t="s">
         <v>658</v>
       </c>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -21705,11 +22335,11 @@
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="135" t="s">
+      <c r="B24" s="138" t="s">
         <v>680</v>
       </c>
-      <c r="C24" s="135"/>
-      <c r="D24" s="135"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
       <c r="F24" s="10">
         <v>14</v>
       </c>
@@ -21829,11 +22459,11 @@
         <v>689</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="135" t="s">
+      <c r="G29" s="138" t="s">
         <v>690</v>
       </c>
-      <c r="H29" s="135"/>
-      <c r="I29" s="135"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="60">

</xml_diff>

<commit_message>
Revisi masuk gudang dan rancangan stok gudang
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kantor\Cloning Repo Aturusaha.com\New31SIM11\Documen Aturusaha\Revisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299C49E4-89BD-4F88-82DB-2B7494CD0AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BA0C80-C807-4004-8812-B7E694EAD3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5124,7 +5124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5189,6 +5189,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -5353,7 +5359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5617,6 +5623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5632,11 +5639,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5665,10 +5675,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -10015,19 +10028,19 @@
       <c r="A1" s="69">
         <v>1</v>
       </c>
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="145" t="s">
         <v>1038</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
       <c r="F1" s="53">
         <v>2</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="138" t="s">
         <v>1039</v>
       </c>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -11554,26 +11567,26 @@
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="144" t="s">
+      <c r="B37" s="146" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145" t="s">
+      <c r="C37" s="146"/>
+      <c r="D37" s="146"/>
+      <c r="E37" s="147" t="s">
         <v>1144</v>
       </c>
-      <c r="F37" s="145"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="146" t="s">
+      <c r="F37" s="147"/>
+      <c r="G37" s="147"/>
+      <c r="H37" s="148" t="s">
         <v>1145</v>
       </c>
-      <c r="I37" s="146"/>
-      <c r="J37" s="146"/>
-      <c r="K37" s="146" t="s">
+      <c r="I37" s="148"/>
+      <c r="J37" s="148"/>
+      <c r="K37" s="148" t="s">
         <v>1146</v>
       </c>
-      <c r="L37" s="146"/>
-      <c r="M37" s="146"/>
+      <c r="L37" s="148"/>
+      <c r="M37" s="148"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
@@ -11959,13 +11972,13 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="147" t="s">
+      <c r="A62" s="149" t="s">
         <v>1156</v>
       </c>
-      <c r="B62" s="147"/>
-      <c r="C62" s="147"/>
-      <c r="D62" s="147"/>
-      <c r="E62" s="147"/>
+      <c r="B62" s="149"/>
+      <c r="C62" s="149"/>
+      <c r="D62" s="149"/>
+      <c r="E62" s="149"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="89"/>
@@ -12169,13 +12182,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="150" t="s">
         <v>1156</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="98"/>
@@ -12357,13 +12370,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="148" t="s">
+      <c r="A17" s="150" t="s">
         <v>1156</v>
       </c>
-      <c r="B17" s="148"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="148"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="150"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="98"/>
@@ -12798,34 +12811,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="114">
         <v>1</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="137" t="s">
         <v>1206</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
       <c r="F2" s="101">
         <v>2</v>
       </c>
-      <c r="G2" s="137" t="s">
+      <c r="G2" s="138" t="s">
         <v>1234</v>
       </c>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="115" t="s">
@@ -12969,9 +12982,9 @@
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="133"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -13091,11 +13104,11 @@
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="133" t="s">
+      <c r="G14" s="134" t="s">
         <v>1244</v>
       </c>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="117">
@@ -13302,12 +13315,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
@@ -14804,16 +14817,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G24:I24"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="G60:I60"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="G33:I33"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14824,8 +14837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16929,25 +16942,25 @@
       <c r="C90" s="17"/>
       <c r="D90" s="17"/>
     </row>
-    <row r="91" spans="1:9" s="149" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="150" t="s">
+    <row r="91" spans="1:9" s="133" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="141" t="s">
         <v>1282</v>
       </c>
-      <c r="C91" s="150"/>
-      <c r="D91" s="150"/>
-      <c r="E91" s="150"/>
-      <c r="F91" s="150"/>
-      <c r="G91" s="150"/>
+      <c r="C91" s="141"/>
+      <c r="D91" s="141"/>
+      <c r="E91" s="141"/>
+      <c r="F91" s="141"/>
+      <c r="G91" s="141"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>13</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="151" t="s">
         <v>1252</v>
       </c>
-      <c r="C92" s="34"/>
-      <c r="D92" s="34"/>
+      <c r="C92" s="152"/>
+      <c r="D92" s="152"/>
       <c r="F92" s="5">
         <v>15</v>
       </c>
@@ -17162,11 +17175,11 @@
       <c r="A104" s="5">
         <v>14</v>
       </c>
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="151" t="s">
         <v>1255</v>
       </c>
-      <c r="C104" s="34"/>
-      <c r="D104" s="34"/>
+      <c r="C104" s="152"/>
+      <c r="D104" s="152"/>
       <c r="F104" s="10">
         <v>1</v>
       </c>
@@ -17383,11 +17396,11 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="98"/>
-      <c r="B115" s="132" t="s">
+      <c r="B115" s="153" t="s">
         <v>1270</v>
       </c>
-      <c r="C115" s="98"/>
-      <c r="D115" s="98"/>
+      <c r="C115" s="153"/>
+      <c r="D115" s="153"/>
       <c r="G115" t="s">
         <v>110</v>
       </c>
@@ -19922,12 +19935,12 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="140" t="s">
+      <c r="A115" s="142" t="s">
         <v>1205</v>
       </c>
-      <c r="B115" s="140"/>
-      <c r="C115" s="140"/>
-      <c r="D115" s="140"/>
+      <c r="B115" s="142"/>
+      <c r="C115" s="142"/>
+      <c r="D115" s="142"/>
       <c r="E115" s="3" t="s">
         <v>110</v>
       </c>
@@ -19948,11 +19961,11 @@
       <c r="A116" s="101">
         <v>1</v>
       </c>
-      <c r="B116" s="137" t="s">
+      <c r="B116" s="138" t="s">
         <v>1202</v>
       </c>
-      <c r="C116" s="137"/>
-      <c r="D116" s="137"/>
+      <c r="C116" s="138"/>
+      <c r="D116" s="138"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="101" t="s">
@@ -20509,19 +20522,19 @@
       <c r="A1" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="138" t="s">
         <v>510</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
       <c r="F1" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="138" t="s">
         <v>512</v>
       </c>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -20657,11 +20670,11 @@
       <c r="F7" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G7" s="137" t="s">
+      <c r="G7" s="138" t="s">
         <v>528</v>
       </c>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -20795,11 +20808,11 @@
       <c r="F13" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G13" s="137" t="s">
+      <c r="G13" s="138" t="s">
         <v>539</v>
       </c>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -20873,11 +20886,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="138" t="s">
         <v>542</v>
       </c>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
@@ -20981,19 +20994,19 @@
       <c r="A27" s="48">
         <v>17</v>
       </c>
-      <c r="B27" s="141" t="s">
+      <c r="B27" s="143" t="s">
         <v>550</v>
       </c>
-      <c r="C27" s="141"/>
-      <c r="D27" s="141"/>
+      <c r="C27" s="143"/>
+      <c r="D27" s="143"/>
       <c r="F27" s="49">
         <v>17</v>
       </c>
-      <c r="G27" s="142" t="s">
+      <c r="G27" s="144" t="s">
         <v>551</v>
       </c>
-      <c r="H27" s="142"/>
-      <c r="I27" s="142"/>
+      <c r="H27" s="144"/>
+      <c r="I27" s="144"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -21261,19 +21274,19 @@
       <c r="A41" s="48">
         <v>17</v>
       </c>
-      <c r="B41" s="141" t="s">
+      <c r="B41" s="143" t="s">
         <v>574</v>
       </c>
-      <c r="C41" s="141"/>
-      <c r="D41" s="141"/>
+      <c r="C41" s="143"/>
+      <c r="D41" s="143"/>
       <c r="F41" s="49">
         <v>18</v>
       </c>
-      <c r="G41" s="142" t="s">
+      <c r="G41" s="144" t="s">
         <v>575</v>
       </c>
-      <c r="H41" s="142"/>
-      <c r="I41" s="142"/>
+      <c r="H41" s="144"/>
+      <c r="I41" s="144"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
@@ -21543,11 +21556,11 @@
       <c r="A54" s="53">
         <v>2</v>
       </c>
-      <c r="B54" s="137" t="s">
+      <c r="B54" s="138" t="s">
         <v>594</v>
       </c>
-      <c r="C54" s="137"/>
-      <c r="D54" s="137"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="138"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
@@ -21821,16 +21834,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="B54:D54"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="B54:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21871,11 +21884,11 @@
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="138" t="s">
         <v>632</v>
       </c>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
revisi menu klien dan leads-tambahan dokumen dashboard
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="500" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="investor" sheetId="11" r:id="rId12"/>
     <sheet name="Sheet1" sheetId="12" r:id="rId13"/>
     <sheet name="Sheet13" sheetId="13" r:id="rId14"/>
+    <sheet name="administrasi" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3639" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3665" uniqueCount="1292">
   <si>
     <t>Revisi2</t>
   </si>
@@ -5032,6 +5032,30 @@
   </si>
   <si>
     <t>tambahan baru</t>
+  </si>
+  <si>
+    <t>a_agenda_harian</t>
+  </si>
+  <si>
+    <t>tabel ageda harian</t>
+  </si>
+  <si>
+    <t>tgl_agenda</t>
+  </si>
+  <si>
+    <t>target_bulanan</t>
+  </si>
+  <si>
+    <t>agenda</t>
+  </si>
+  <si>
+    <t>texy</t>
+  </si>
+  <si>
+    <t>prioritas</t>
+  </si>
+  <si>
+    <t>0= penting &amp; mendesak, 1= penting &amp; tdk mendesak, 2 = tidak penting &amp; mendesak</t>
   </si>
 </sst>
 </file>
@@ -5330,7 +5354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5594,6 +5618,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5609,11 +5639,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5642,9 +5675,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6247,19 +6279,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="141" t="s">
         <v>756</v>
       </c>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="138" t="s">
+      <c r="G1" s="141" t="s">
         <v>757</v>
       </c>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
@@ -6581,11 +6613,11 @@
       <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="141" t="s">
         <v>784</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
       <c r="F15" s="59">
         <v>13</v>
       </c>
@@ -6906,19 +6938,19 @@
       <c r="A30" s="5">
         <v>4</v>
       </c>
-      <c r="B30" s="138" t="s">
+      <c r="B30" s="141" t="s">
         <v>814</v>
       </c>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="141"/>
       <c r="F30" s="5">
         <v>4</v>
       </c>
-      <c r="G30" s="138" t="s">
+      <c r="G30" s="141" t="s">
         <v>815</v>
       </c>
-      <c r="H30" s="138"/>
-      <c r="I30" s="138"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="141"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
@@ -7159,11 +7191,11 @@
       <c r="F41" s="5">
         <v>4</v>
       </c>
-      <c r="G41" s="138" t="s">
+      <c r="G41" s="141" t="s">
         <v>827</v>
       </c>
-      <c r="H41" s="138"/>
-      <c r="I41" s="138"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141"/>
     </row>
     <row r="42" spans="1:9">
       <c r="F42" s="9" t="s">
@@ -7183,11 +7215,11 @@
       <c r="A43" s="5">
         <v>4</v>
       </c>
-      <c r="B43" s="138" t="s">
+      <c r="B43" s="141" t="s">
         <v>828</v>
       </c>
-      <c r="C43" s="138"/>
-      <c r="D43" s="138"/>
+      <c r="C43" s="141"/>
+      <c r="D43" s="141"/>
       <c r="F43" s="10">
         <v>1</v>
       </c>
@@ -7506,11 +7538,11 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="5"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="141" t="s">
         <v>838</v>
       </c>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
       <c r="F1" s="5"/>
       <c r="G1" s="8" t="s">
         <v>839</v>
@@ -9947,19 +9979,19 @@
       <c r="A1" s="69">
         <v>1</v>
       </c>
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="146" t="s">
         <v>1038</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
       <c r="F1" s="53">
         <v>2</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="139" t="s">
         <v>1039</v>
       </c>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -10461,11 +10493,11 @@
       </c>
       <c r="D23" s="11"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="138" t="s">
+      <c r="G23" s="141" t="s">
         <v>1056</v>
       </c>
-      <c r="H23" s="138"/>
-      <c r="I23" s="138"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="141"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10">
@@ -11486,26 +11518,26 @@
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="144" t="s">
+      <c r="B37" s="147" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145" t="s">
+      <c r="C37" s="147"/>
+      <c r="D37" s="147"/>
+      <c r="E37" s="148" t="s">
         <v>1144</v>
       </c>
-      <c r="F37" s="145"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="146" t="s">
+      <c r="F37" s="148"/>
+      <c r="G37" s="148"/>
+      <c r="H37" s="149" t="s">
         <v>1145</v>
       </c>
-      <c r="I37" s="146"/>
-      <c r="J37" s="146"/>
-      <c r="K37" s="146" t="s">
+      <c r="I37" s="149"/>
+      <c r="J37" s="149"/>
+      <c r="K37" s="149" t="s">
         <v>1146</v>
       </c>
-      <c r="L37" s="146"/>
-      <c r="M37" s="146"/>
+      <c r="L37" s="149"/>
+      <c r="M37" s="149"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="11"/>
@@ -11891,13 +11923,13 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="147" t="s">
+      <c r="A62" s="150" t="s">
         <v>1156</v>
       </c>
-      <c r="B62" s="147"/>
-      <c r="C62" s="147"/>
-      <c r="D62" s="147"/>
-      <c r="E62" s="147"/>
+      <c r="B62" s="150"/>
+      <c r="C62" s="150"/>
+      <c r="D62" s="150"/>
+      <c r="E62" s="150"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="89"/>
@@ -12101,13 +12133,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="151" t="s">
         <v>1156</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="98"/>
@@ -12289,13 +12321,13 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="148" t="s">
+      <c r="A17" s="151" t="s">
         <v>1156</v>
       </c>
-      <c r="B17" s="148"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="148"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="151"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="98"/>
@@ -12490,6 +12522,156 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5">
+        <v>8</v>
+      </c>
+      <c r="B1" s="133" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="134" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="134" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="134" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="134" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="103" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="98" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="98" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="118" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="152" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="118" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C6" s="153" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="98" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C7" s="98" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" ht="60">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="98" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C8" s="98" t="s">
+        <v>901</v>
+      </c>
+      <c r="D8" s="107" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -12714,7 +12896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -12730,34 +12912,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="136" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="114">
         <v>1</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="138" t="s">
         <v>1206</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
       <c r="F2" s="101">
         <v>2</v>
       </c>
-      <c r="G2" s="137" t="s">
+      <c r="G2" s="139" t="s">
         <v>1234</v>
       </c>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="115" t="s">
@@ -12901,9 +13083,9 @@
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="133"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
+      <c r="I8" s="135"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="10">
@@ -13023,11 +13205,11 @@
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="133" t="s">
+      <c r="G14" s="135" t="s">
         <v>1244</v>
       </c>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="135"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="117">
@@ -13217,7 +13399,7 @@
   <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="A34" sqref="A34:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -13234,30 +13416,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="141" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="138" t="s">
+      <c r="G2" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -13483,11 +13665,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="138" t="s">
+      <c r="G12" s="141" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="138"/>
-      <c r="I12" s="138"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -13731,21 +13913,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="138" t="s">
+      <c r="G24" s="141" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="138"/>
-      <c r="I24" s="138"/>
+      <c r="H24" s="141"/>
+      <c r="I24" s="141"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="138" t="s">
+      <c r="B25" s="141" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="141"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -13893,11 +14075,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="138" t="s">
+      <c r="G33" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="138"/>
-      <c r="I33" s="138"/>
+      <c r="H33" s="141"/>
+      <c r="I33" s="141"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -14149,11 +14331,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="138" t="s">
+      <c r="B45" s="141" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="138"/>
-      <c r="D45" s="138"/>
+      <c r="C45" s="141"/>
+      <c r="D45" s="141"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -14437,19 +14619,19 @@
       <c r="A60" s="5">
         <v>13</v>
       </c>
-      <c r="B60" s="138" t="s">
+      <c r="B60" s="141" t="s">
         <v>1185</v>
       </c>
-      <c r="C60" s="138"/>
-      <c r="D60" s="138"/>
+      <c r="C60" s="141"/>
+      <c r="D60" s="141"/>
       <c r="F60" s="5">
         <v>14</v>
       </c>
-      <c r="G60" s="138" t="s">
+      <c r="G60" s="141" t="s">
         <v>1186</v>
       </c>
-      <c r="H60" s="138"/>
-      <c r="I60" s="138"/>
+      <c r="H60" s="141"/>
+      <c r="I60" s="141"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="9" t="s">
@@ -14736,16 +14918,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="B45:D45"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14756,7 +14938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
@@ -16862,14 +17044,14 @@
       <c r="D90" s="17"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="B91" s="149" t="s">
+      <c r="B91" s="142" t="s">
         <v>1283</v>
       </c>
-      <c r="C91" s="149"/>
-      <c r="D91" s="149"/>
-      <c r="E91" s="149"/>
-      <c r="F91" s="149"/>
-      <c r="G91" s="149"/>
+      <c r="C91" s="142"/>
+      <c r="D91" s="142"/>
+      <c r="E91" s="142"/>
+      <c r="F91" s="142"/>
+      <c r="G91" s="142"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="5">
@@ -19848,12 +20030,12 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="140" t="s">
+      <c r="A115" s="143" t="s">
         <v>1205</v>
       </c>
-      <c r="B115" s="140"/>
-      <c r="C115" s="140"/>
-      <c r="D115" s="140"/>
+      <c r="B115" s="143"/>
+      <c r="C115" s="143"/>
+      <c r="D115" s="143"/>
       <c r="E115" s="3" t="s">
         <v>110</v>
       </c>
@@ -19874,11 +20056,11 @@
       <c r="A116" s="101">
         <v>1</v>
       </c>
-      <c r="B116" s="137" t="s">
+      <c r="B116" s="139" t="s">
         <v>1202</v>
       </c>
-      <c r="C116" s="137"/>
-      <c r="D116" s="137"/>
+      <c r="C116" s="139"/>
+      <c r="D116" s="139"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="101" t="s">
@@ -20435,19 +20617,19 @@
       <c r="A1" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="139" t="s">
         <v>510</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
       <c r="F1" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="139" t="s">
         <v>512</v>
       </c>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -20583,11 +20765,11 @@
       <c r="F7" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G7" s="137" t="s">
+      <c r="G7" s="139" t="s">
         <v>528</v>
       </c>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -20721,11 +20903,11 @@
       <c r="F13" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G13" s="137" t="s">
+      <c r="G13" s="139" t="s">
         <v>539</v>
       </c>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="139"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -20799,11 +20981,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="139" t="s">
         <v>542</v>
       </c>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="139"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -20907,19 +21089,19 @@
       <c r="A27" s="48">
         <v>17</v>
       </c>
-      <c r="B27" s="141" t="s">
+      <c r="B27" s="144" t="s">
         <v>550</v>
       </c>
-      <c r="C27" s="141"/>
-      <c r="D27" s="141"/>
+      <c r="C27" s="144"/>
+      <c r="D27" s="144"/>
       <c r="F27" s="49">
         <v>17</v>
       </c>
-      <c r="G27" s="142" t="s">
+      <c r="G27" s="145" t="s">
         <v>551</v>
       </c>
-      <c r="H27" s="142"/>
-      <c r="I27" s="142"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -21187,19 +21369,19 @@
       <c r="A41" s="48">
         <v>17</v>
       </c>
-      <c r="B41" s="141" t="s">
+      <c r="B41" s="144" t="s">
         <v>574</v>
       </c>
-      <c r="C41" s="141"/>
-      <c r="D41" s="141"/>
+      <c r="C41" s="144"/>
+      <c r="D41" s="144"/>
       <c r="F41" s="49">
         <v>18</v>
       </c>
-      <c r="G41" s="142" t="s">
+      <c r="G41" s="145" t="s">
         <v>575</v>
       </c>
-      <c r="H41" s="142"/>
-      <c r="I41" s="142"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -21469,11 +21651,11 @@
       <c r="A54" s="53">
         <v>2</v>
       </c>
-      <c r="B54" s="137" t="s">
+      <c r="B54" s="139" t="s">
         <v>594</v>
       </c>
-      <c r="C54" s="137"/>
-      <c r="D54" s="137"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="139"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -21747,16 +21929,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21789,19 +21971,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="141" t="s">
         <v>631</v>
       </c>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="139" t="s">
         <v>632</v>
       </c>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -21989,11 +22171,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="138" t="s">
+      <c r="G9" s="141" t="s">
         <v>650</v>
       </c>
-      <c r="H9" s="138"/>
-      <c r="I9" s="138"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -22117,11 +22299,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="141" t="s">
         <v>658</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -22335,11 +22517,11 @@
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="141" t="s">
         <v>680</v>
       </c>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="141"/>
       <c r="F24" s="10">
         <v>14</v>
       </c>
@@ -22459,11 +22641,11 @@
         <v>689</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="138" t="s">
+      <c r="G29" s="141" t="s">
         <v>690</v>
       </c>
-      <c r="H29" s="138"/>
-      <c r="I29" s="138"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="141"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="60">

</xml_diff>

<commit_message>
revisi hal index, revisi format laporan
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
+++ b/Documen Aturusaha/Revisi/daftar tabel revisi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="973" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="hasil meet up investor" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sheet1" sheetId="12" r:id="rId13"/>
     <sheet name="Sheet13" sheetId="13" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -5642,6 +5642,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5657,11 +5659,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5693,8 +5695,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6305,19 +6305,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>756</v>
       </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
       <c r="F1" s="5">
         <v>2</v>
       </c>
-      <c r="G1" s="141" t="s">
+      <c r="G1" s="144" t="s">
         <v>757</v>
       </c>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9" t="s">
@@ -6639,11 +6639,11 @@
       <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="144" t="s">
         <v>784</v>
       </c>
-      <c r="C15" s="141"/>
-      <c r="D15" s="141"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
       <c r="F15" s="59">
         <v>13</v>
       </c>
@@ -6964,19 +6964,19 @@
       <c r="A30" s="5">
         <v>4</v>
       </c>
-      <c r="B30" s="141" t="s">
+      <c r="B30" s="144" t="s">
         <v>814</v>
       </c>
-      <c r="C30" s="141"/>
-      <c r="D30" s="141"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
       <c r="F30" s="5">
         <v>4</v>
       </c>
-      <c r="G30" s="141" t="s">
+      <c r="G30" s="144" t="s">
         <v>815</v>
       </c>
-      <c r="H30" s="141"/>
-      <c r="I30" s="141"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="144"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="9" t="s">
@@ -7217,11 +7217,11 @@
       <c r="F41" s="5">
         <v>4</v>
       </c>
-      <c r="G41" s="141" t="s">
+      <c r="G41" s="144" t="s">
         <v>827</v>
       </c>
-      <c r="H41" s="141"/>
-      <c r="I41" s="141"/>
+      <c r="H41" s="144"/>
+      <c r="I41" s="144"/>
     </row>
     <row r="42" spans="1:9">
       <c r="F42" s="9" t="s">
@@ -7241,11 +7241,11 @@
       <c r="A43" s="5">
         <v>4</v>
       </c>
-      <c r="B43" s="141" t="s">
+      <c r="B43" s="144" t="s">
         <v>828</v>
       </c>
-      <c r="C43" s="141"/>
-      <c r="D43" s="141"/>
+      <c r="C43" s="144"/>
+      <c r="D43" s="144"/>
       <c r="F43" s="10">
         <v>1</v>
       </c>
@@ -7564,11 +7564,11 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="5"/>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>838</v>
       </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
       <c r="F1" s="5"/>
       <c r="G1" s="8" t="s">
         <v>839</v>
@@ -10005,19 +10005,19 @@
       <c r="A1" s="69">
         <v>1</v>
       </c>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="149" t="s">
         <v>1038</v>
       </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
       <c r="F1" s="53">
         <v>2</v>
       </c>
-      <c r="G1" s="140" t="s">
+      <c r="G1" s="142" t="s">
         <v>1039</v>
       </c>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -10519,11 +10519,11 @@
       </c>
       <c r="D23" s="11"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="141" t="s">
+      <c r="G23" s="144" t="s">
         <v>1056</v>
       </c>
-      <c r="H23" s="141"/>
-      <c r="I23" s="141"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10">
@@ -11544,26 +11544,26 @@
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="148" t="s">
+      <c r="B37" s="150" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="148"/>
-      <c r="D37" s="148"/>
-      <c r="E37" s="149" t="s">
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="151" t="s">
         <v>1144</v>
       </c>
-      <c r="F37" s="149"/>
-      <c r="G37" s="149"/>
-      <c r="H37" s="150" t="s">
+      <c r="F37" s="151"/>
+      <c r="G37" s="151"/>
+      <c r="H37" s="152" t="s">
         <v>1145</v>
       </c>
-      <c r="I37" s="150"/>
-      <c r="J37" s="150"/>
-      <c r="K37" s="150" t="s">
+      <c r="I37" s="152"/>
+      <c r="J37" s="152"/>
+      <c r="K37" s="152" t="s">
         <v>1146</v>
       </c>
-      <c r="L37" s="150"/>
-      <c r="M37" s="150"/>
+      <c r="L37" s="152"/>
+      <c r="M37" s="152"/>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="11"/>
@@ -11949,13 +11949,13 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="151" t="s">
+      <c r="A62" s="153" t="s">
         <v>1156</v>
       </c>
-      <c r="B62" s="151"/>
-      <c r="C62" s="151"/>
-      <c r="D62" s="151"/>
-      <c r="E62" s="151"/>
+      <c r="B62" s="153"/>
+      <c r="C62" s="153"/>
+      <c r="D62" s="153"/>
+      <c r="E62" s="153"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="89"/>
@@ -12159,13 +12159,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="154" t="s">
         <v>1156</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="98"/>
@@ -12347,13 +12347,13 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="152" t="s">
+      <c r="A17" s="154" t="s">
         <v>1156</v>
       </c>
-      <c r="B17" s="152"/>
-      <c r="C17" s="152"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="152"/>
+      <c r="B17" s="154"/>
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="154"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="98"/>
@@ -12788,34 +12788,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="139" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="114">
         <v>1</v>
       </c>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="141" t="s">
         <v>1206</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
       <c r="F2" s="101">
         <v>2</v>
       </c>
-      <c r="G2" s="140" t="s">
+      <c r="G2" s="142" t="s">
         <v>1234</v>
       </c>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="115" t="s">
@@ -12959,9 +12959,9 @@
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="10">
@@ -13081,11 +13081,11 @@
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="100"/>
-      <c r="G14" s="136" t="s">
+      <c r="G14" s="138" t="s">
         <v>1244</v>
       </c>
-      <c r="H14" s="136"/>
-      <c r="I14" s="136"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="117">
@@ -13292,30 +13292,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="144" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
       <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="141" t="s">
+      <c r="G2" s="144" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="9" t="s">
@@ -13541,11 +13541,11 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="141" t="s">
+      <c r="G12" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="141"/>
-      <c r="I12" s="141"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="144"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10">
@@ -13789,21 +13789,21 @@
       <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G24" s="141" t="s">
+      <c r="G24" s="144" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="141" t="s">
+      <c r="B25" s="144" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="141"/>
-      <c r="D25" s="141"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
       <c r="F25" s="9" t="s">
         <v>71</v>
       </c>
@@ -13951,11 +13951,11 @@
       <c r="F33" s="5">
         <v>7</v>
       </c>
-      <c r="G33" s="141" t="s">
+      <c r="G33" s="144" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="5">
@@ -14207,11 +14207,11 @@
       <c r="A45" s="5">
         <v>9</v>
       </c>
-      <c r="B45" s="141" t="s">
+      <c r="B45" s="144" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="141"/>
-      <c r="D45" s="141"/>
+      <c r="C45" s="144"/>
+      <c r="D45" s="144"/>
       <c r="F45" s="9" t="s">
         <v>71</v>
       </c>
@@ -14495,19 +14495,19 @@
       <c r="A60" s="5">
         <v>13</v>
       </c>
-      <c r="B60" s="141" t="s">
+      <c r="B60" s="144" t="s">
         <v>1185</v>
       </c>
-      <c r="C60" s="141"/>
-      <c r="D60" s="141"/>
+      <c r="C60" s="144"/>
+      <c r="D60" s="144"/>
       <c r="F60" s="5">
         <v>14</v>
       </c>
-      <c r="G60" s="141" t="s">
+      <c r="G60" s="144" t="s">
         <v>1186</v>
       </c>
-      <c r="H60" s="141"/>
-      <c r="I60" s="141"/>
+      <c r="H60" s="144"/>
+      <c r="I60" s="144"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="9" t="s">
@@ -14794,16 +14794,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="B45:D45"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14814,8 +14814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="C90" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -14823,7 +14823,7 @@
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
@@ -16920,14 +16920,14 @@
       <c r="D90" s="17"/>
     </row>
     <row r="91" spans="1:9" s="135" customFormat="1">
-      <c r="B91" s="143" t="s">
+      <c r="B91" s="145" t="s">
         <v>1282</v>
       </c>
-      <c r="C91" s="143"/>
-      <c r="D91" s="143"/>
-      <c r="E91" s="143"/>
-      <c r="F91" s="143"/>
-      <c r="G91" s="143"/>
+      <c r="C91" s="145"/>
+      <c r="D91" s="145"/>
+      <c r="E91" s="145"/>
+      <c r="F91" s="145"/>
+      <c r="G91" s="145"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="5">
@@ -17085,7 +17085,7 @@
       <c r="F98" s="10">
         <v>5</v>
       </c>
-      <c r="G98" s="112" t="s">
+      <c r="G98" s="116" t="s">
         <v>1275</v>
       </c>
       <c r="H98" s="116" t="s">
@@ -17102,7 +17102,7 @@
       <c r="F99" s="10">
         <v>6</v>
       </c>
-      <c r="G99" s="112" t="s">
+      <c r="G99" s="116" t="s">
         <v>1276</v>
       </c>
       <c r="H99" s="116" t="s">
@@ -17267,13 +17267,13 @@
       <c r="A109" s="10">
         <v>4</v>
       </c>
-      <c r="B109" s="106" t="s">
+      <c r="B109" s="116" t="s">
         <v>1273</v>
       </c>
-      <c r="C109" s="106" t="s">
-        <v>76</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C109" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="D109" s="98" t="s">
         <v>1274</v>
       </c>
     </row>
@@ -17495,7 +17495,7 @@
       <c r="B126" s="118" t="s">
         <v>517</v>
       </c>
-      <c r="C126" s="153" t="s">
+      <c r="C126" s="136" t="s">
         <v>76</v>
       </c>
       <c r="D126" s="20"/>
@@ -17507,7 +17507,7 @@
       <c r="B127" s="118" t="s">
         <v>1291</v>
       </c>
-      <c r="C127" s="154" t="s">
+      <c r="C127" s="137" t="s">
         <v>76</v>
       </c>
       <c r="D127" s="11"/>
@@ -20042,12 +20042,12 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="144" t="s">
+      <c r="A115" s="146" t="s">
         <v>1205</v>
       </c>
-      <c r="B115" s="144"/>
-      <c r="C115" s="144"/>
-      <c r="D115" s="144"/>
+      <c r="B115" s="146"/>
+      <c r="C115" s="146"/>
+      <c r="D115" s="146"/>
       <c r="E115" s="3" t="s">
         <v>110</v>
       </c>
@@ -20068,11 +20068,11 @@
       <c r="A116" s="101">
         <v>1</v>
       </c>
-      <c r="B116" s="140" t="s">
+      <c r="B116" s="142" t="s">
         <v>1202</v>
       </c>
-      <c r="C116" s="140"/>
-      <c r="D116" s="140"/>
+      <c r="C116" s="142"/>
+      <c r="D116" s="142"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="101" t="s">
@@ -20629,19 +20629,19 @@
       <c r="A1" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B1" s="140" t="s">
+      <c r="B1" s="142" t="s">
         <v>510</v>
       </c>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
       <c r="F1" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="G1" s="140" t="s">
+      <c r="G1" s="142" t="s">
         <v>512</v>
       </c>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -20777,11 +20777,11 @@
       <c r="F7" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G7" s="140" t="s">
+      <c r="G7" s="142" t="s">
         <v>528</v>
       </c>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
+      <c r="H7" s="142"/>
+      <c r="I7" s="142"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="10">
@@ -20915,11 +20915,11 @@
       <c r="F13" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="G13" s="140" t="s">
+      <c r="G13" s="142" t="s">
         <v>539</v>
       </c>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
+      <c r="H13" s="142"/>
+      <c r="I13" s="142"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="10">
@@ -20993,11 +20993,11 @@
       <c r="A18" s="9">
         <v>18</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="142" t="s">
         <v>542</v>
       </c>
-      <c r="C18" s="140"/>
-      <c r="D18" s="140"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
@@ -21101,19 +21101,19 @@
       <c r="A27" s="48">
         <v>17</v>
       </c>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="147" t="s">
         <v>550</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
       <c r="F27" s="49">
         <v>17</v>
       </c>
-      <c r="G27" s="146" t="s">
+      <c r="G27" s="148" t="s">
         <v>551</v>
       </c>
-      <c r="H27" s="146"/>
-      <c r="I27" s="146"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="148"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
@@ -21381,19 +21381,19 @@
       <c r="A41" s="48">
         <v>17</v>
       </c>
-      <c r="B41" s="145" t="s">
+      <c r="B41" s="147" t="s">
         <v>574</v>
       </c>
-      <c r="C41" s="145"/>
-      <c r="D41" s="145"/>
+      <c r="C41" s="147"/>
+      <c r="D41" s="147"/>
       <c r="F41" s="49">
         <v>18</v>
       </c>
-      <c r="G41" s="146" t="s">
+      <c r="G41" s="148" t="s">
         <v>575</v>
       </c>
-      <c r="H41" s="146"/>
-      <c r="I41" s="146"/>
+      <c r="H41" s="148"/>
+      <c r="I41" s="148"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
@@ -21663,11 +21663,11 @@
       <c r="A54" s="53">
         <v>2</v>
       </c>
-      <c r="B54" s="140" t="s">
+      <c r="B54" s="142" t="s">
         <v>594</v>
       </c>
-      <c r="C54" s="140"/>
-      <c r="D54" s="140"/>
+      <c r="C54" s="142"/>
+      <c r="D54" s="142"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
@@ -21941,16 +21941,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21983,19 +21983,19 @@
       <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>631</v>
       </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
       <c r="F1" s="9">
         <v>4</v>
       </c>
-      <c r="G1" s="140" t="s">
+      <c r="G1" s="142" t="s">
         <v>632</v>
       </c>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
@@ -22183,11 +22183,11 @@
       <c r="F9" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="141" t="s">
+      <c r="G9" s="144" t="s">
         <v>650</v>
       </c>
-      <c r="H9" s="141"/>
-      <c r="I9" s="141"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="144"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="10">
@@ -22311,11 +22311,11 @@
       <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="144" t="s">
         <v>658</v>
       </c>
-      <c r="C15" s="141"/>
-      <c r="D15" s="141"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
       <c r="F15" s="10">
         <v>5</v>
       </c>
@@ -22529,11 +22529,11 @@
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="141" t="s">
+      <c r="B24" s="144" t="s">
         <v>680</v>
       </c>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
       <c r="F24" s="10">
         <v>14</v>
       </c>
@@ -22653,11 +22653,11 @@
         <v>689</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="141" t="s">
+      <c r="G29" s="144" t="s">
         <v>690</v>
       </c>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141"/>
+      <c r="H29" s="144"/>
+      <c r="I29" s="144"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="60">

</xml_diff>